<commit_message>
Summary Updated InDesign model, Jazz Age resources, and computer player logic Actions:
Problems
</commit_message>
<xml_diff>
--- a/docs/edition_points.xlsx
+++ b/docs/edition_points.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Compile\careers\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275DE66B-2B7D-42DE-BCB4-C7A16A3CED44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369773E6-AFDB-466B-89DE-7578F7870C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="1545" windowWidth="24075" windowHeight="13500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4350" yWindow="960" windowWidth="24075" windowHeight="13500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hi-Tech v1" sheetId="1" r:id="rId1"/>
     <sheet name="Hi-Tech v2" sheetId="2" r:id="rId2"/>
+    <sheet name="Jazz Age" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="75">
   <si>
     <t>Occupation</t>
   </si>
@@ -196,6 +197,72 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>AI Research, Aerospace Engineering</t>
+  </si>
+  <si>
+    <t>PPI</t>
+  </si>
+  <si>
+    <t>Radio Station KWDB</t>
+  </si>
+  <si>
+    <t>Bootlegger</t>
+  </si>
+  <si>
+    <t>Roosevelt College</t>
+  </si>
+  <si>
+    <t>Sapphire Records</t>
+  </si>
+  <si>
+    <t>Major League Baseball</t>
+  </si>
+  <si>
+    <t>Paul Whiteman's Orch.</t>
+  </si>
+  <si>
+    <t>Prohibition Agent</t>
+  </si>
+  <si>
+    <t>Cotton Club</t>
+  </si>
+  <si>
+    <t>Chicago Outfit</t>
+  </si>
+  <si>
+    <t>Stork Club</t>
+  </si>
+  <si>
+    <t>TOTALS</t>
+  </si>
+  <si>
+    <t>sort order is Points, Salary</t>
+  </si>
+  <si>
+    <t>Overall Ranking sort order: Points, Salary</t>
+  </si>
+  <si>
+    <t>Average Ranking</t>
+  </si>
+  <si>
+    <t>Stork Club, Paul Whiteman's</t>
+  </si>
+  <si>
+    <t>KWDB, Prohibition Agent</t>
+  </si>
+  <si>
+    <t>Chicago Outfit, KWDB</t>
+  </si>
+  <si>
+    <t>Sapphire Records, Prohibition Agent</t>
+  </si>
+  <si>
+    <t>KWDB,  Stork Club</t>
+  </si>
+  <si>
+    <t>Roosevelt College, Prohibition Agent</t>
   </si>
 </sst>
 </file>
@@ -390,7 +457,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -586,6 +653,9 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="37" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -593,6 +663,72 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -902,27 +1038,27 @@
   <sheetData>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="77"/>
+      <c r="C3" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="78"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="75" t="s">
+      <c r="K3" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="76"/>
-      <c r="S3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="78"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -1848,16 +1984,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2731D533-3189-49BB-AE83-771387574D8F}">
   <dimension ref="A3:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
     <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.140625" style="1"/>
@@ -1865,27 +2006,27 @@
   <sheetData>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="77"/>
+      <c r="C3" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="78"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="75" t="s">
+      <c r="K3" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="76"/>
-      <c r="S3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="78"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -2003,14 +2144,14 @@
         <v>10</v>
       </c>
       <c r="R5" s="34">
-        <f t="shared" ref="R5:R14" si="1">SUM(K5:Q5)/6</f>
+        <f>SUM(K5:Q5)/6</f>
         <v>5.5</v>
       </c>
       <c r="S5" s="4">
         <v>3</v>
       </c>
       <c r="T5" s="1">
-        <f t="shared" ref="T5:T14" si="2">SUM(K5:Q5)</f>
+        <f>SUM(K5:Q5)</f>
         <v>33</v>
       </c>
     </row>
@@ -2068,14 +2209,14 @@
         <v>9</v>
       </c>
       <c r="R6" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="R5:R14" si="1">SUM(K6:Q6)/6</f>
         <v>7.833333333333333</v>
       </c>
       <c r="S6" s="50">
         <v>9</v>
       </c>
       <c r="T6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="T5:T14" si="2">SUM(K6:Q6)</f>
         <v>47</v>
       </c>
     </row>
@@ -2635,7 +2776,10 @@
       <c r="B19" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2643,7 +2787,10 @@
       <c r="B20" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2651,7 +2798,10 @@
       <c r="B21" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2659,7 +2809,10 @@
       <c r="B22" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2667,7 +2820,10 @@
       <c r="B23" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2675,7 +2831,10 @@
       <c r="B24" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D24" t="s">
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2739,29 +2898,29 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="32">
+      <c r="A31" s="91">
         <v>1</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="92">
         <v>34</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="92">
         <v>24</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="29">
         <v>15</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="29">
         <f>SUM(C31:E31)</f>
         <v>73</v>
       </c>
-      <c r="G31" s="13">
-        <v>2</v>
-      </c>
-      <c r="H31" s="1">
+      <c r="G31" s="26">
+        <v>2</v>
+      </c>
+      <c r="H31" s="92">
         <v>2</v>
       </c>
       <c r="I31" s="7">
@@ -2770,15 +2929,34 @@
       <c r="J31" s="20">
         <v>3</v>
       </c>
-      <c r="K31" s="36"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="34"/>
-      <c r="S31" s="4"/>
+      <c r="K31" s="36">
+        <v>3</v>
+      </c>
+      <c r="L31" s="92">
+        <v>2</v>
+      </c>
+      <c r="M31" s="92">
+        <v>2</v>
+      </c>
+      <c r="N31" s="92">
+        <v>1</v>
+      </c>
+      <c r="O31" s="92">
+        <v>7</v>
+      </c>
+      <c r="P31" s="92">
+        <v>8</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>10</v>
+      </c>
+      <c r="R31" s="34">
+        <f>(O31+SUM(K31:M31))/4</f>
+        <v>3.5</v>
+      </c>
+      <c r="S31" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="41">
@@ -2797,7 +2975,7 @@
         <v>8</v>
       </c>
       <c r="F32" s="52">
-        <f t="shared" ref="F32:F36" si="4">SUM(C32:E32)</f>
+        <f>SUM(C32:E32)</f>
         <v>44</v>
       </c>
       <c r="G32" s="53">
@@ -2812,15 +2990,34 @@
       <c r="J32" s="47">
         <v>2</v>
       </c>
-      <c r="K32" s="48"/>
-      <c r="L32" s="49"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="49"/>
-      <c r="O32" s="49"/>
-      <c r="P32" s="49"/>
-      <c r="Q32" s="50"/>
-      <c r="R32" s="51"/>
-      <c r="S32" s="50"/>
+      <c r="K32" s="48">
+        <v>6</v>
+      </c>
+      <c r="L32" s="49">
+        <v>4</v>
+      </c>
+      <c r="M32" s="49">
+        <v>4</v>
+      </c>
+      <c r="N32" s="49">
+        <v>6</v>
+      </c>
+      <c r="O32" s="49">
+        <v>8</v>
+      </c>
+      <c r="P32" s="49">
+        <v>10</v>
+      </c>
+      <c r="Q32" s="50">
+        <v>9</v>
+      </c>
+      <c r="R32" s="51">
+        <f>(O32+SUM(K32:M32))/4</f>
+        <v>5.5</v>
+      </c>
+      <c r="S32" s="50">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="32">
@@ -2839,7 +3036,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(C33:E33)</f>
         <v>24</v>
       </c>
       <c r="G33" s="13">
@@ -2854,15 +3051,34 @@
       <c r="J33" s="22">
         <v>2</v>
       </c>
-      <c r="K33" s="35"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="34"/>
-      <c r="S33" s="4"/>
+      <c r="K33" s="35">
+        <v>7</v>
+      </c>
+      <c r="L33" s="1">
+        <v>6</v>
+      </c>
+      <c r="M33" s="1">
+        <v>10</v>
+      </c>
+      <c r="N33" s="1">
+        <v>9</v>
+      </c>
+      <c r="O33" s="1">
+        <v>10</v>
+      </c>
+      <c r="P33" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>1</v>
+      </c>
+      <c r="R33" s="34">
+        <f>(O33+SUM(K33:M33))/4</f>
+        <v>8.25</v>
+      </c>
+      <c r="S33" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="41">
@@ -2881,7 +3097,7 @@
         <v>6</v>
       </c>
       <c r="F34" s="52">
-        <f t="shared" si="4"/>
+        <f>SUM(C34:E34)</f>
         <v>22</v>
       </c>
       <c r="G34" s="53">
@@ -2896,15 +3112,34 @@
       <c r="J34" s="47">
         <v>2</v>
       </c>
-      <c r="K34" s="48"/>
-      <c r="L34" s="49"/>
-      <c r="M34" s="49"/>
-      <c r="N34" s="49"/>
-      <c r="O34" s="49"/>
-      <c r="P34" s="49"/>
-      <c r="Q34" s="50"/>
-      <c r="R34" s="51"/>
-      <c r="S34" s="50"/>
+      <c r="K34" s="48">
+        <v>9</v>
+      </c>
+      <c r="L34" s="49">
+        <v>7</v>
+      </c>
+      <c r="M34" s="49">
+        <v>6</v>
+      </c>
+      <c r="N34" s="49">
+        <v>10</v>
+      </c>
+      <c r="O34" s="49">
+        <v>1</v>
+      </c>
+      <c r="P34" s="49">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="50">
+        <v>2</v>
+      </c>
+      <c r="R34" s="51">
+        <f>(O34+SUM(K34:M34))/4</f>
+        <v>5.75</v>
+      </c>
+      <c r="S34" s="50">
+        <v>3</v>
+      </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="32">
@@ -2923,7 +3158,7 @@
         <v>8</v>
       </c>
       <c r="F35" s="14">
-        <f t="shared" si="4"/>
+        <f>SUM(C35:E35)</f>
         <v>28</v>
       </c>
       <c r="G35" s="6">
@@ -2938,15 +3173,34 @@
       <c r="J35" s="21">
         <v>2</v>
       </c>
-      <c r="K35" s="35"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="34"/>
-      <c r="S35" s="4"/>
+      <c r="K35" s="35">
+        <v>8</v>
+      </c>
+      <c r="L35" s="1">
+        <v>8</v>
+      </c>
+      <c r="M35" s="1">
+        <v>3</v>
+      </c>
+      <c r="N35" s="1">
+        <v>8</v>
+      </c>
+      <c r="O35" s="1">
+        <v>3</v>
+      </c>
+      <c r="P35" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q35" s="4">
+        <v>7</v>
+      </c>
+      <c r="R35" s="34">
+        <f>(O35+SUM(K35:M35))/4</f>
+        <v>5.5</v>
+      </c>
+      <c r="S35" s="4">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="41">
@@ -2965,7 +3219,7 @@
         <v>3</v>
       </c>
       <c r="F36" s="52">
-        <f t="shared" si="4"/>
+        <f>SUM(C36:E36)</f>
         <v>28</v>
       </c>
       <c r="G36" s="56">
@@ -2980,15 +3234,34 @@
       <c r="J36" s="57">
         <v>2</v>
       </c>
-      <c r="K36" s="48"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="49"/>
-      <c r="N36" s="49"/>
-      <c r="O36" s="49"/>
-      <c r="P36" s="49"/>
-      <c r="Q36" s="50"/>
-      <c r="R36" s="51"/>
-      <c r="S36" s="50"/>
+      <c r="K36" s="48">
+        <v>10</v>
+      </c>
+      <c r="L36" s="49">
+        <v>5</v>
+      </c>
+      <c r="M36" s="49">
+        <v>9</v>
+      </c>
+      <c r="N36" s="49">
+        <v>7</v>
+      </c>
+      <c r="O36" s="49">
+        <v>9</v>
+      </c>
+      <c r="P36" s="49">
+        <v>5</v>
+      </c>
+      <c r="Q36" s="50">
+        <v>5</v>
+      </c>
+      <c r="R36" s="51">
+        <f>(O36+SUM(K36:M36))/4</f>
+        <v>8.25</v>
+      </c>
+      <c r="S36" s="50">
+        <v>2</v>
+      </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="32">
@@ -3022,15 +3295,34 @@
       <c r="J37" s="22">
         <v>2</v>
       </c>
-      <c r="K37" s="35"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="34"/>
-      <c r="S37" s="4"/>
+      <c r="K37" s="35">
+        <v>1</v>
+      </c>
+      <c r="L37" s="1">
+        <v>9</v>
+      </c>
+      <c r="M37" s="1">
+        <v>7</v>
+      </c>
+      <c r="N37" s="1">
+        <v>4</v>
+      </c>
+      <c r="O37" s="1">
+        <v>2</v>
+      </c>
+      <c r="P37" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>4</v>
+      </c>
+      <c r="R37" s="34">
+        <f>(O37+SUM(K37:M37))/4</f>
+        <v>4.75</v>
+      </c>
+      <c r="S37" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="41">
@@ -3049,7 +3341,7 @@
         <v>7</v>
       </c>
       <c r="F38" s="52">
-        <f t="shared" ref="F38:F40" si="5">SUM(C38:E38)</f>
+        <f>SUM(C38:E38)</f>
         <v>45</v>
       </c>
       <c r="G38" s="73">
@@ -3064,15 +3356,34 @@
       <c r="J38" s="60">
         <v>2</v>
       </c>
-      <c r="K38" s="48"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="49"/>
-      <c r="O38" s="49"/>
-      <c r="P38" s="49"/>
-      <c r="Q38" s="50"/>
-      <c r="R38" s="51"/>
-      <c r="S38" s="50"/>
+      <c r="K38" s="48">
+        <v>4</v>
+      </c>
+      <c r="L38" s="49">
+        <v>10</v>
+      </c>
+      <c r="M38" s="49">
+        <v>5</v>
+      </c>
+      <c r="N38" s="49">
+        <v>5</v>
+      </c>
+      <c r="O38" s="49">
+        <v>4</v>
+      </c>
+      <c r="P38" s="49">
+        <v>9</v>
+      </c>
+      <c r="Q38" s="50">
+        <v>6</v>
+      </c>
+      <c r="R38" s="51">
+        <f>(O38+SUM(K38:M38))/4</f>
+        <v>5.75</v>
+      </c>
+      <c r="S38" s="50">
+        <v>4</v>
+      </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="32">
@@ -3091,7 +3402,7 @@
         <v>30</v>
       </c>
       <c r="F39" s="14">
-        <f t="shared" si="5"/>
+        <f>SUM(C39:E39)</f>
         <v>67</v>
       </c>
       <c r="G39" s="13">
@@ -3106,15 +3417,34 @@
       <c r="J39" s="22">
         <v>2</v>
       </c>
-      <c r="K39" s="35"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="34"/>
-      <c r="S39" s="4"/>
+      <c r="K39" s="35">
+        <v>5</v>
+      </c>
+      <c r="L39" s="1">
+        <v>3</v>
+      </c>
+      <c r="M39" s="1">
+        <v>1</v>
+      </c>
+      <c r="N39" s="1">
+        <v>2</v>
+      </c>
+      <c r="O39" s="1">
+        <v>6</v>
+      </c>
+      <c r="P39" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q39" s="4">
+        <v>3</v>
+      </c>
+      <c r="R39" s="34">
+        <f>(O39+SUM(K39:M39))/4</f>
+        <v>3.75</v>
+      </c>
+      <c r="S39" s="4">
+        <v>9</v>
+      </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="61">
@@ -3133,7 +3463,7 @@
         <v>4</v>
       </c>
       <c r="F40" s="65">
-        <f t="shared" si="5"/>
+        <f>SUM(C40:E40)</f>
         <v>66</v>
       </c>
       <c r="G40" s="66">
@@ -3148,19 +3478,1585 @@
       <c r="J40" s="68">
         <v>3</v>
       </c>
-      <c r="K40" s="69"/>
-      <c r="L40" s="63"/>
-      <c r="M40" s="63"/>
-      <c r="N40" s="63"/>
-      <c r="O40" s="63"/>
-      <c r="P40" s="63"/>
-      <c r="Q40" s="67"/>
-      <c r="R40" s="70"/>
-      <c r="S40" s="71"/>
+      <c r="K40" s="69">
+        <v>2</v>
+      </c>
+      <c r="L40" s="63">
+        <v>1</v>
+      </c>
+      <c r="M40" s="63">
+        <v>8</v>
+      </c>
+      <c r="N40" s="63">
+        <v>3</v>
+      </c>
+      <c r="O40" s="63">
+        <v>5</v>
+      </c>
+      <c r="P40" s="63">
+        <v>7</v>
+      </c>
+      <c r="Q40" s="67">
+        <v>8</v>
+      </c>
+      <c r="R40" s="74">
+        <f>(O40+SUM(K40:M40))/4</f>
+        <v>4</v>
+      </c>
+      <c r="S40" s="71">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:T14">
-    <sortCondition ref="A5:A14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A31:S40">
+    <sortCondition ref="A31:A40"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="K3:S3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66559D5-1C3E-471D-81A3-258D37D68792}">
+  <dimension ref="A3:T39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" customWidth="1"/>
+    <col min="17" max="17" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="12"/>
+      <c r="C3" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="78"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="S4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="T4" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="1">
+        <v>34</v>
+      </c>
+      <c r="D5" s="32">
+        <v>18</v>
+      </c>
+      <c r="E5" s="29">
+        <v>15</v>
+      </c>
+      <c r="F5" s="29">
+        <f>SUM(C5:E5)</f>
+        <v>67</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="20">
+        <v>3</v>
+      </c>
+      <c r="K5" s="36">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
+        <v>5</v>
+      </c>
+      <c r="M5" s="1">
+        <v>2</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>8</v>
+      </c>
+      <c r="P5" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>10</v>
+      </c>
+      <c r="R5" s="34">
+        <f t="shared" ref="R5:R14" si="0">SUM(K5:Q5)/6</f>
+        <v>5.5</v>
+      </c>
+      <c r="S5" s="4">
+        <v>1</v>
+      </c>
+      <c r="T5" s="1">
+        <f>SUM(K5:Q5)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="41">
+        <v>2</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="43">
+        <v>8</v>
+      </c>
+      <c r="D6" s="85">
+        <v>21</v>
+      </c>
+      <c r="E6" s="44">
+        <v>8</v>
+      </c>
+      <c r="F6" s="44">
+        <f>SUM(C6:E6)</f>
+        <v>37</v>
+      </c>
+      <c r="G6" s="43">
+        <v>1</v>
+      </c>
+      <c r="H6" s="43">
+        <v>1</v>
+      </c>
+      <c r="I6" s="46">
+        <v>1</v>
+      </c>
+      <c r="J6" s="47">
+        <v>2</v>
+      </c>
+      <c r="K6" s="48">
+        <v>7</v>
+      </c>
+      <c r="L6" s="49">
+        <v>3</v>
+      </c>
+      <c r="M6" s="49">
+        <v>5</v>
+      </c>
+      <c r="N6" s="49">
+        <v>6</v>
+      </c>
+      <c r="O6" s="49">
+        <v>10</v>
+      </c>
+      <c r="P6" s="49">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="50">
+        <v>8</v>
+      </c>
+      <c r="R6" s="51">
+        <f t="shared" si="0"/>
+        <v>8.1666666666666661</v>
+      </c>
+      <c r="S6" s="50">
+        <v>6</v>
+      </c>
+      <c r="T6" s="1">
+        <f t="shared" ref="T5:T14" si="1">SUM(K6:Q6)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="32">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="1">
+        <v>12</v>
+      </c>
+      <c r="D7" s="32">
+        <v>12</v>
+      </c>
+      <c r="E7" s="29">
+        <v>0</v>
+      </c>
+      <c r="F7" s="29">
+        <f>SUM(C7:E7)</f>
+        <v>24</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="4">
+        <v>4</v>
+      </c>
+      <c r="J7" s="22">
+        <v>2</v>
+      </c>
+      <c r="K7" s="35">
+        <v>5</v>
+      </c>
+      <c r="L7" s="1">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1">
+        <v>10</v>
+      </c>
+      <c r="N7" s="1">
+        <v>9</v>
+      </c>
+      <c r="O7" s="1">
+        <v>7</v>
+      </c>
+      <c r="P7" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>1</v>
+      </c>
+      <c r="R7" s="34">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="S7" s="4">
+        <v>9</v>
+      </c>
+      <c r="T7" s="1">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="41">
+        <v>4</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="43">
+        <v>4</v>
+      </c>
+      <c r="D8" s="85">
+        <v>12</v>
+      </c>
+      <c r="E8" s="44">
+        <v>3</v>
+      </c>
+      <c r="F8" s="44">
+        <f>SUM(C8:E8)</f>
+        <v>19</v>
+      </c>
+      <c r="G8" s="75">
+        <v>8</v>
+      </c>
+      <c r="H8" s="43">
+        <v>1</v>
+      </c>
+      <c r="I8" s="46">
+        <v>2</v>
+      </c>
+      <c r="J8" s="47">
+        <v>2</v>
+      </c>
+      <c r="K8" s="48">
+        <v>9</v>
+      </c>
+      <c r="L8" s="49">
+        <v>8</v>
+      </c>
+      <c r="M8" s="49">
+        <v>8</v>
+      </c>
+      <c r="N8" s="49">
+        <v>10</v>
+      </c>
+      <c r="O8" s="49">
+        <v>1</v>
+      </c>
+      <c r="P8" s="49">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="50">
+        <v>5</v>
+      </c>
+      <c r="R8" s="51">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="S8" s="50">
+        <v>10</v>
+      </c>
+      <c r="T8" s="1">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="32">
+        <v>5</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="5">
+        <v>6</v>
+      </c>
+      <c r="D9" s="16">
+        <v>14</v>
+      </c>
+      <c r="E9" s="14">
+        <v>8</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" ref="F9:F14" si="2">SUM(C9:E9)</f>
+        <v>28</v>
+      </c>
+      <c r="G9" s="79">
+        <v>5</v>
+      </c>
+      <c r="H9" s="5">
+        <v>2</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1</v>
+      </c>
+      <c r="J9" s="21">
+        <v>2</v>
+      </c>
+      <c r="K9" s="35">
+        <v>8</v>
+      </c>
+      <c r="L9" s="1">
+        <v>6</v>
+      </c>
+      <c r="M9" s="1">
+        <v>4</v>
+      </c>
+      <c r="N9" s="1">
+        <v>7</v>
+      </c>
+      <c r="O9" s="1">
+        <v>3</v>
+      </c>
+      <c r="P9" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>7</v>
+      </c>
+      <c r="R9" s="34">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="S9" s="4">
+        <v>7</v>
+      </c>
+      <c r="T9" s="1">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="41">
+        <v>6</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="49">
+        <v>2</v>
+      </c>
+      <c r="D10" s="41">
+        <v>23</v>
+      </c>
+      <c r="E10" s="58">
+        <v>3</v>
+      </c>
+      <c r="F10" s="44">
+        <f>SUM(C10:E10)</f>
+        <v>28</v>
+      </c>
+      <c r="G10" s="80">
+        <v>1</v>
+      </c>
+      <c r="H10" s="49">
+        <v>1</v>
+      </c>
+      <c r="I10" s="50">
+        <v>2</v>
+      </c>
+      <c r="J10" s="57">
+        <v>2</v>
+      </c>
+      <c r="K10" s="48">
+        <v>10</v>
+      </c>
+      <c r="L10" s="49">
+        <v>2</v>
+      </c>
+      <c r="M10" s="49">
+        <v>9</v>
+      </c>
+      <c r="N10" s="49">
+        <v>8</v>
+      </c>
+      <c r="O10" s="49">
+        <v>9</v>
+      </c>
+      <c r="P10" s="49">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="50">
+        <v>4</v>
+      </c>
+      <c r="R10" s="51">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="S10" s="50">
+        <v>8</v>
+      </c>
+      <c r="T10" s="1">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="32">
+        <v>7</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="1">
+        <v>30</v>
+      </c>
+      <c r="D11" s="32">
+        <v>9</v>
+      </c>
+      <c r="E11" s="15">
+        <v>5</v>
+      </c>
+      <c r="F11" s="14">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="G11" s="81">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2</v>
+      </c>
+      <c r="I11" s="4">
+        <v>2</v>
+      </c>
+      <c r="J11" s="22">
+        <v>2</v>
+      </c>
+      <c r="K11" s="35">
+        <v>2</v>
+      </c>
+      <c r="L11" s="1">
+        <v>9</v>
+      </c>
+      <c r="M11" s="1">
+        <v>6</v>
+      </c>
+      <c r="N11" s="1">
+        <v>4</v>
+      </c>
+      <c r="O11" s="1">
+        <v>2</v>
+      </c>
+      <c r="P11" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>2</v>
+      </c>
+      <c r="R11" s="34">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="S11" s="4">
+        <v>4</v>
+      </c>
+      <c r="T11" s="1">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="41">
+        <v>8</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="43">
+        <v>28</v>
+      </c>
+      <c r="D12" s="85">
+        <v>6</v>
+      </c>
+      <c r="E12" s="58">
+        <v>4</v>
+      </c>
+      <c r="F12" s="44">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="G12" s="82">
+        <v>4</v>
+      </c>
+      <c r="H12" s="43">
+        <v>1</v>
+      </c>
+      <c r="I12" s="46">
+        <v>2</v>
+      </c>
+      <c r="J12" s="60">
+        <v>2</v>
+      </c>
+      <c r="K12" s="48">
+        <v>3</v>
+      </c>
+      <c r="L12" s="49">
+        <v>10</v>
+      </c>
+      <c r="M12" s="49">
+        <v>7</v>
+      </c>
+      <c r="N12" s="49">
+        <v>5</v>
+      </c>
+      <c r="O12" s="49">
+        <v>4</v>
+      </c>
+      <c r="P12" s="49">
+        <v>7</v>
+      </c>
+      <c r="Q12" s="50">
+        <v>3</v>
+      </c>
+      <c r="R12" s="51">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="S12" s="50">
+        <v>5</v>
+      </c>
+      <c r="T12" s="1">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="32">
+        <v>9</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="32">
+        <v>20</v>
+      </c>
+      <c r="E13" s="25">
+        <v>30</v>
+      </c>
+      <c r="F13" s="29">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="G13" s="83">
+        <v>3</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0</v>
+      </c>
+      <c r="J13" s="22">
+        <v>2</v>
+      </c>
+      <c r="K13" s="35">
+        <v>6</v>
+      </c>
+      <c r="L13" s="1">
+        <v>4</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>3</v>
+      </c>
+      <c r="O13" s="1">
+        <v>6</v>
+      </c>
+      <c r="P13" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>9</v>
+      </c>
+      <c r="R13" s="34">
+        <f t="shared" si="0"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="S13" s="4">
+        <v>3</v>
+      </c>
+      <c r="T13" s="1">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="61">
+        <v>10</v>
+      </c>
+      <c r="B14" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="63">
+        <v>16</v>
+      </c>
+      <c r="D14" s="86">
+        <v>39</v>
+      </c>
+      <c r="E14" s="64">
+        <v>9</v>
+      </c>
+      <c r="F14" s="65">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="G14" s="84">
+        <v>4</v>
+      </c>
+      <c r="H14" s="63">
+        <v>2</v>
+      </c>
+      <c r="I14" s="67">
+        <v>1</v>
+      </c>
+      <c r="J14" s="68">
+        <v>3</v>
+      </c>
+      <c r="K14" s="69">
+        <v>4</v>
+      </c>
+      <c r="L14" s="63">
+        <v>1</v>
+      </c>
+      <c r="M14" s="63">
+        <v>3</v>
+      </c>
+      <c r="N14" s="63">
+        <v>2</v>
+      </c>
+      <c r="O14" s="63">
+        <v>5</v>
+      </c>
+      <c r="P14" s="63">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="67">
+        <v>6</v>
+      </c>
+      <c r="R14" s="74">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="S14" s="71">
+        <v>2</v>
+      </c>
+      <c r="T14" s="1">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="1">
+        <f>SUM(C5:C14)</f>
+        <v>150</v>
+      </c>
+      <c r="D15" s="1">
+        <f>SUM(D5:D14)</f>
+        <v>174</v>
+      </c>
+      <c r="E15" s="32">
+        <f>SUM(E5:E14)</f>
+        <v>85</v>
+      </c>
+      <c r="F15" s="32">
+        <f>SUM(F5:F14)</f>
+        <v>409</v>
+      </c>
+      <c r="G15" s="1">
+        <f>SUM(G5:G14)</f>
+        <v>36</v>
+      </c>
+      <c r="H15" s="1">
+        <f>SUM(H5:H14)</f>
+        <v>16</v>
+      </c>
+      <c r="I15" s="1">
+        <f>SUM(I5:I14)</f>
+        <v>15</v>
+      </c>
+      <c r="J15" s="32">
+        <f>SUM(J5:J14)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="K27" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R27" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="S27" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="91">
+        <v>1</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="92">
+        <v>34</v>
+      </c>
+      <c r="D28" s="91">
+        <v>18</v>
+      </c>
+      <c r="E28" s="29">
+        <v>15</v>
+      </c>
+      <c r="F28" s="29">
+        <v>67</v>
+      </c>
+      <c r="G28" s="91">
+        <v>2</v>
+      </c>
+      <c r="H28" s="91">
+        <v>2</v>
+      </c>
+      <c r="I28" s="96">
+        <v>0</v>
+      </c>
+      <c r="J28" s="20">
+        <v>3</v>
+      </c>
+      <c r="K28" s="36">
+        <v>1</v>
+      </c>
+      <c r="L28" s="92">
+        <v>5</v>
+      </c>
+      <c r="M28" s="92">
+        <v>2</v>
+      </c>
+      <c r="N28" s="92">
+        <v>1</v>
+      </c>
+      <c r="O28" s="92">
+        <v>8</v>
+      </c>
+      <c r="P28" s="92">
+        <v>6</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>10</v>
+      </c>
+      <c r="R28" s="34">
+        <f>SUM(K28:Q28)/6</f>
+        <v>5.5</v>
+      </c>
+      <c r="S28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="87">
+        <v>2</v>
+      </c>
+      <c r="B29" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="89">
+        <v>8</v>
+      </c>
+      <c r="D29" s="90">
+        <v>21</v>
+      </c>
+      <c r="E29" s="44">
+        <v>8</v>
+      </c>
+      <c r="F29" s="44">
+        <v>37</v>
+      </c>
+      <c r="G29" s="90">
+        <v>1</v>
+      </c>
+      <c r="H29" s="90">
+        <v>1</v>
+      </c>
+      <c r="I29" s="93">
+        <v>1</v>
+      </c>
+      <c r="J29" s="47">
+        <v>2</v>
+      </c>
+      <c r="K29" s="48">
+        <v>7</v>
+      </c>
+      <c r="L29" s="88">
+        <v>3</v>
+      </c>
+      <c r="M29" s="88">
+        <v>5</v>
+      </c>
+      <c r="N29" s="88">
+        <v>6</v>
+      </c>
+      <c r="O29" s="88">
+        <v>10</v>
+      </c>
+      <c r="P29" s="88">
+        <v>10</v>
+      </c>
+      <c r="Q29" s="50">
+        <v>8</v>
+      </c>
+      <c r="R29" s="51">
+        <f>SUM(K29:Q29)/6</f>
+        <v>8.1666666666666661</v>
+      </c>
+      <c r="S29" s="50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="91">
+        <v>3</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="92">
+        <v>12</v>
+      </c>
+      <c r="D30" s="91">
+        <v>12</v>
+      </c>
+      <c r="E30" s="29">
+        <v>0</v>
+      </c>
+      <c r="F30" s="29">
+        <v>24</v>
+      </c>
+      <c r="G30" s="91">
+        <v>2</v>
+      </c>
+      <c r="H30" s="91">
+        <v>2</v>
+      </c>
+      <c r="I30" s="95">
+        <v>4</v>
+      </c>
+      <c r="J30" s="22">
+        <v>2</v>
+      </c>
+      <c r="K30" s="35">
+        <v>5</v>
+      </c>
+      <c r="L30" s="92">
+        <v>7</v>
+      </c>
+      <c r="M30" s="92">
+        <v>10</v>
+      </c>
+      <c r="N30" s="92">
+        <v>9</v>
+      </c>
+      <c r="O30" s="92">
+        <v>7</v>
+      </c>
+      <c r="P30" s="92">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>1</v>
+      </c>
+      <c r="R30" s="34">
+        <f>SUM(K30:Q30)/6</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="S30" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="87">
+        <v>4</v>
+      </c>
+      <c r="B31" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="89">
+        <v>4</v>
+      </c>
+      <c r="D31" s="90">
+        <v>12</v>
+      </c>
+      <c r="E31" s="44">
+        <v>3</v>
+      </c>
+      <c r="F31" s="44">
+        <v>19</v>
+      </c>
+      <c r="G31" s="58">
+        <v>8</v>
+      </c>
+      <c r="H31" s="90">
+        <v>1</v>
+      </c>
+      <c r="I31" s="93">
+        <v>2</v>
+      </c>
+      <c r="J31" s="47">
+        <v>2</v>
+      </c>
+      <c r="K31" s="48">
+        <v>9</v>
+      </c>
+      <c r="L31" s="88">
+        <v>8</v>
+      </c>
+      <c r="M31" s="88">
+        <v>8</v>
+      </c>
+      <c r="N31" s="88">
+        <v>10</v>
+      </c>
+      <c r="O31" s="88">
+        <v>1</v>
+      </c>
+      <c r="P31" s="88">
+        <v>9</v>
+      </c>
+      <c r="Q31" s="50">
+        <v>5</v>
+      </c>
+      <c r="R31" s="51">
+        <f>SUM(K31:Q31)/6</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="S31" s="50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="32">
+        <v>5</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="5">
+        <v>6</v>
+      </c>
+      <c r="D32" s="16">
+        <v>14</v>
+      </c>
+      <c r="E32" s="14">
+        <v>8</v>
+      </c>
+      <c r="F32" s="14">
+        <v>28</v>
+      </c>
+      <c r="G32" s="15">
+        <v>5</v>
+      </c>
+      <c r="H32" s="16">
+        <v>2</v>
+      </c>
+      <c r="I32" s="96">
+        <v>1</v>
+      </c>
+      <c r="J32" s="21">
+        <v>2</v>
+      </c>
+      <c r="K32" s="35">
+        <v>8</v>
+      </c>
+      <c r="L32" s="1">
+        <v>6</v>
+      </c>
+      <c r="M32" s="1">
+        <v>4</v>
+      </c>
+      <c r="N32" s="1">
+        <v>7</v>
+      </c>
+      <c r="O32" s="1">
+        <v>3</v>
+      </c>
+      <c r="P32" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>7</v>
+      </c>
+      <c r="R32" s="34">
+        <f>SUM(K32:Q32)/6</f>
+        <v>6.5</v>
+      </c>
+      <c r="S32" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="87">
+        <v>6</v>
+      </c>
+      <c r="B33" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="88">
+        <v>2</v>
+      </c>
+      <c r="D33" s="87">
+        <v>23</v>
+      </c>
+      <c r="E33" s="58">
+        <v>3</v>
+      </c>
+      <c r="F33" s="44">
+        <v>28</v>
+      </c>
+      <c r="G33" s="97">
+        <v>1</v>
+      </c>
+      <c r="H33" s="87">
+        <v>1</v>
+      </c>
+      <c r="I33" s="98">
+        <v>2</v>
+      </c>
+      <c r="J33" s="57">
+        <v>2</v>
+      </c>
+      <c r="K33" s="48">
+        <v>10</v>
+      </c>
+      <c r="L33" s="88">
+        <v>2</v>
+      </c>
+      <c r="M33" s="88">
+        <v>9</v>
+      </c>
+      <c r="N33" s="88">
+        <v>8</v>
+      </c>
+      <c r="O33" s="88">
+        <v>9</v>
+      </c>
+      <c r="P33" s="88">
+        <v>8</v>
+      </c>
+      <c r="Q33" s="50">
+        <v>4</v>
+      </c>
+      <c r="R33" s="51">
+        <f>SUM(K33:Q33)/6</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="S33" s="50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="32">
+        <v>7</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="1">
+        <v>30</v>
+      </c>
+      <c r="D34" s="32">
+        <v>9</v>
+      </c>
+      <c r="E34" s="15">
+        <v>5</v>
+      </c>
+      <c r="F34" s="14">
+        <v>44</v>
+      </c>
+      <c r="G34" s="94">
+        <v>6</v>
+      </c>
+      <c r="H34" s="32">
+        <v>2</v>
+      </c>
+      <c r="I34" s="95">
+        <v>2</v>
+      </c>
+      <c r="J34" s="22">
+        <v>2</v>
+      </c>
+      <c r="K34" s="35">
+        <v>2</v>
+      </c>
+      <c r="L34" s="1">
+        <v>9</v>
+      </c>
+      <c r="M34" s="1">
+        <v>6</v>
+      </c>
+      <c r="N34" s="1">
+        <v>4</v>
+      </c>
+      <c r="O34" s="1">
+        <v>2</v>
+      </c>
+      <c r="P34" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>2</v>
+      </c>
+      <c r="R34" s="34">
+        <f>SUM(K34:Q34)/6</f>
+        <v>4.5</v>
+      </c>
+      <c r="S34" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="87">
+        <v>8</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="89">
+        <v>28</v>
+      </c>
+      <c r="D35" s="90">
+        <v>6</v>
+      </c>
+      <c r="E35" s="58">
+        <v>4</v>
+      </c>
+      <c r="F35" s="44">
+        <v>38</v>
+      </c>
+      <c r="G35" s="44">
+        <v>4</v>
+      </c>
+      <c r="H35" s="90">
+        <v>1</v>
+      </c>
+      <c r="I35" s="93">
+        <v>2</v>
+      </c>
+      <c r="J35" s="60">
+        <v>2</v>
+      </c>
+      <c r="K35" s="48">
+        <v>3</v>
+      </c>
+      <c r="L35" s="88">
+        <v>10</v>
+      </c>
+      <c r="M35" s="88">
+        <v>7</v>
+      </c>
+      <c r="N35" s="88">
+        <v>5</v>
+      </c>
+      <c r="O35" s="88">
+        <v>4</v>
+      </c>
+      <c r="P35" s="88">
+        <v>7</v>
+      </c>
+      <c r="Q35" s="50">
+        <v>3</v>
+      </c>
+      <c r="R35" s="51">
+        <f>SUM(K35:Q35)/6</f>
+        <v>6.5</v>
+      </c>
+      <c r="S35" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="32">
+        <v>9</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="1">
+        <v>10</v>
+      </c>
+      <c r="D36" s="32">
+        <v>20</v>
+      </c>
+      <c r="E36" s="25">
+        <v>30</v>
+      </c>
+      <c r="F36" s="29">
+        <v>60</v>
+      </c>
+      <c r="G36" s="99">
+        <v>3</v>
+      </c>
+      <c r="H36" s="32">
+        <v>2</v>
+      </c>
+      <c r="I36" s="96">
+        <v>0</v>
+      </c>
+      <c r="J36" s="22">
+        <v>2</v>
+      </c>
+      <c r="K36" s="35">
+        <v>6</v>
+      </c>
+      <c r="L36" s="1">
+        <v>4</v>
+      </c>
+      <c r="M36" s="1">
+        <v>1</v>
+      </c>
+      <c r="N36" s="1">
+        <v>3</v>
+      </c>
+      <c r="O36" s="1">
+        <v>6</v>
+      </c>
+      <c r="P36" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>9</v>
+      </c>
+      <c r="R36" s="34">
+        <f>SUM(K36:Q36)/6</f>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="S36" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="61">
+        <v>10</v>
+      </c>
+      <c r="B37" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="63">
+        <v>16</v>
+      </c>
+      <c r="D37" s="86">
+        <v>39</v>
+      </c>
+      <c r="E37" s="64">
+        <v>9</v>
+      </c>
+      <c r="F37" s="65">
+        <v>64</v>
+      </c>
+      <c r="G37" s="100">
+        <v>4</v>
+      </c>
+      <c r="H37" s="86">
+        <v>2</v>
+      </c>
+      <c r="I37" s="61">
+        <v>1</v>
+      </c>
+      <c r="J37" s="68">
+        <v>3</v>
+      </c>
+      <c r="K37" s="69">
+        <v>4</v>
+      </c>
+      <c r="L37" s="63">
+        <v>1</v>
+      </c>
+      <c r="M37" s="63">
+        <v>3</v>
+      </c>
+      <c r="N37" s="63">
+        <v>2</v>
+      </c>
+      <c r="O37" s="63">
+        <v>5</v>
+      </c>
+      <c r="P37" s="63">
+        <v>3</v>
+      </c>
+      <c r="Q37" s="67">
+        <v>6</v>
+      </c>
+      <c r="R37" s="74">
+        <f>SUM(K37:Q37)/6</f>
+        <v>4</v>
+      </c>
+      <c r="S37" s="71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A28:S37">
+    <sortCondition ref="A28:A37"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="C3:I3"/>

</xml_diff>

<commit_message>
Summary InDesign model adds & updates, resource adds & updates Actions: UPDATE Professions-Hi-Tech InDesign model and idml UPDATE Professions-Hi-Tech resources/JazzAge/Bootlegger UPDATE TimeMachine-JazzAge InDesign model & idml UPDATE JazzAge v1 and v2 InDesign models ADD TimeMachine-JazzAge resource files UPDATE JazzAge resource files
Problems
</commit_message>
<xml_diff>
--- a/docs/edition_points.xlsx
+++ b/docs/edition_points.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Compile\careers\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369773E6-AFDB-466B-89DE-7578F7870C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8460152F-881F-4BCB-9B75-41C608772D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4350" yWindow="960" windowWidth="24075" windowHeight="13500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="75">
   <si>
     <t>Occupation</t>
   </si>
@@ -457,7 +457,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -656,6 +656,54 @@
     <xf numFmtId="37" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -663,72 +711,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1038,27 +1020,27 @@
   <sheetData>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="76" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="78"/>
+      <c r="C3" s="92" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="94"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="76" t="s">
+      <c r="K3" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="77"/>
-      <c r="S3" s="78"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="94"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -1985,7 +1967,7 @@
   <dimension ref="A3:T40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2006,27 +1988,27 @@
   <sheetData>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="76" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="78"/>
+      <c r="C3" s="92" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="94"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="76" t="s">
+      <c r="K3" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="77"/>
-      <c r="S3" s="78"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="94"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -2209,14 +2191,14 @@
         <v>9</v>
       </c>
       <c r="R6" s="51">
-        <f t="shared" ref="R5:R14" si="1">SUM(K6:Q6)/6</f>
+        <f t="shared" ref="R6:R14" si="1">SUM(K6:Q6)/6</f>
         <v>7.833333333333333</v>
       </c>
       <c r="S6" s="50">
         <v>9</v>
       </c>
       <c r="T6" s="1">
-        <f t="shared" ref="T5:T14" si="2">SUM(K6:Q6)</f>
+        <f t="shared" ref="T6:T14" si="2">SUM(K6:Q6)</f>
         <v>47</v>
       </c>
     </row>
@@ -2838,6 +2820,11 @@
         <v>25</v>
       </c>
     </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="30" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
         <v>49</v>
@@ -2898,29 +2885,29 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="91">
+      <c r="A31" s="32">
         <v>1</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="92">
+      <c r="C31" s="1">
         <v>34</v>
       </c>
-      <c r="D31" s="92">
+      <c r="D31" s="1">
         <v>24</v>
       </c>
       <c r="E31" s="29">
         <v>15</v>
       </c>
       <c r="F31" s="29">
-        <f>SUM(C31:E31)</f>
+        <f t="shared" ref="F31:F40" si="4">SUM(C31:E31)</f>
         <v>73</v>
       </c>
       <c r="G31" s="26">
         <v>2</v>
       </c>
-      <c r="H31" s="92">
+      <c r="H31" s="1">
         <v>2</v>
       </c>
       <c r="I31" s="7">
@@ -2932,26 +2919,26 @@
       <c r="K31" s="36">
         <v>3</v>
       </c>
-      <c r="L31" s="92">
-        <v>2</v>
-      </c>
-      <c r="M31" s="92">
-        <v>2</v>
-      </c>
-      <c r="N31" s="92">
-        <v>1</v>
-      </c>
-      <c r="O31" s="92">
-        <v>7</v>
-      </c>
-      <c r="P31" s="92">
+      <c r="L31" s="1">
+        <v>2</v>
+      </c>
+      <c r="M31" s="1">
+        <v>2</v>
+      </c>
+      <c r="N31" s="1">
+        <v>1</v>
+      </c>
+      <c r="O31" s="1">
+        <v>7</v>
+      </c>
+      <c r="P31" s="1">
         <v>8</v>
       </c>
       <c r="Q31" s="4">
         <v>10</v>
       </c>
       <c r="R31" s="34">
-        <f>(O31+SUM(K31:M31))/4</f>
+        <f t="shared" ref="R31:R40" si="5">(O31+SUM(K31:M31))/4</f>
         <v>3.5</v>
       </c>
       <c r="S31" s="4">
@@ -2975,7 +2962,7 @@
         <v>8</v>
       </c>
       <c r="F32" s="52">
-        <f>SUM(C32:E32)</f>
+        <f t="shared" si="4"/>
         <v>44</v>
       </c>
       <c r="G32" s="53">
@@ -3012,7 +2999,7 @@
         <v>9</v>
       </c>
       <c r="R32" s="51">
-        <f>(O32+SUM(K32:M32))/4</f>
+        <f t="shared" si="5"/>
         <v>5.5</v>
       </c>
       <c r="S32" s="50">
@@ -3036,7 +3023,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="14">
-        <f>SUM(C33:E33)</f>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="G33" s="13">
@@ -3073,7 +3060,7 @@
         <v>1</v>
       </c>
       <c r="R33" s="34">
-        <f>(O33+SUM(K33:M33))/4</f>
+        <f t="shared" si="5"/>
         <v>8.25</v>
       </c>
       <c r="S33" s="4">
@@ -3097,7 +3084,7 @@
         <v>6</v>
       </c>
       <c r="F34" s="52">
-        <f>SUM(C34:E34)</f>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="G34" s="53">
@@ -3134,7 +3121,7 @@
         <v>2</v>
       </c>
       <c r="R34" s="51">
-        <f>(O34+SUM(K34:M34))/4</f>
+        <f t="shared" si="5"/>
         <v>5.75</v>
       </c>
       <c r="S34" s="50">
@@ -3158,7 +3145,7 @@
         <v>8</v>
       </c>
       <c r="F35" s="14">
-        <f>SUM(C35:E35)</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="G35" s="6">
@@ -3195,7 +3182,7 @@
         <v>7</v>
       </c>
       <c r="R35" s="34">
-        <f>(O35+SUM(K35:M35))/4</f>
+        <f t="shared" si="5"/>
         <v>5.5</v>
       </c>
       <c r="S35" s="4">
@@ -3219,7 +3206,7 @@
         <v>3</v>
       </c>
       <c r="F36" s="52">
-        <f>SUM(C36:E36)</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="G36" s="56">
@@ -3256,7 +3243,7 @@
         <v>5</v>
       </c>
       <c r="R36" s="51">
-        <f>(O36+SUM(K36:M36))/4</f>
+        <f t="shared" si="5"/>
         <v>8.25</v>
       </c>
       <c r="S36" s="50">
@@ -3280,7 +3267,7 @@
         <v>5</v>
       </c>
       <c r="F37" s="14">
-        <f>SUM(C37:E37)</f>
+        <f t="shared" si="4"/>
         <v>49</v>
       </c>
       <c r="G37" s="13">
@@ -3317,7 +3304,7 @@
         <v>4</v>
       </c>
       <c r="R37" s="34">
-        <f>(O37+SUM(K37:M37))/4</f>
+        <f t="shared" si="5"/>
         <v>4.75</v>
       </c>
       <c r="S37" s="4">
@@ -3341,7 +3328,7 @@
         <v>7</v>
       </c>
       <c r="F38" s="52">
-        <f>SUM(C38:E38)</f>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="G38" s="73">
@@ -3378,7 +3365,7 @@
         <v>6</v>
       </c>
       <c r="R38" s="51">
-        <f>(O38+SUM(K38:M38))/4</f>
+        <f t="shared" si="5"/>
         <v>5.75</v>
       </c>
       <c r="S38" s="50">
@@ -3402,7 +3389,7 @@
         <v>30</v>
       </c>
       <c r="F39" s="14">
-        <f>SUM(C39:E39)</f>
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
       <c r="G39" s="13">
@@ -3439,7 +3426,7 @@
         <v>3</v>
       </c>
       <c r="R39" s="34">
-        <f>(O39+SUM(K39:M39))/4</f>
+        <f t="shared" si="5"/>
         <v>3.75</v>
       </c>
       <c r="S39" s="4">
@@ -3463,7 +3450,7 @@
         <v>4</v>
       </c>
       <c r="F40" s="65">
-        <f>SUM(C40:E40)</f>
+        <f t="shared" si="4"/>
         <v>66</v>
       </c>
       <c r="G40" s="66">
@@ -3500,7 +3487,7 @@
         <v>8</v>
       </c>
       <c r="R40" s="74">
-        <f>(O40+SUM(K40:M40))/4</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="S40" s="71">
@@ -3525,7 +3512,7 @@
   <dimension ref="A3:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3541,27 +3528,27 @@
   <sheetData>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="76" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="78"/>
+      <c r="C3" s="92" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="94"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="76" t="s">
+      <c r="K3" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="77"/>
-      <c r="S3" s="78"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="94"/>
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
@@ -3634,7 +3621,7 @@
         <v>55</v>
       </c>
       <c r="C5" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D5" s="32">
         <v>18</v>
@@ -3644,7 +3631,7 @@
       </c>
       <c r="F5" s="29">
         <f>SUM(C5:E5)</f>
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G5" s="1">
         <v>2</v>
@@ -3701,7 +3688,7 @@
       <c r="C6" s="43">
         <v>8</v>
       </c>
-      <c r="D6" s="85">
+      <c r="D6" s="82">
         <v>21</v>
       </c>
       <c r="E6" s="44">
@@ -3721,7 +3708,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6" s="48">
         <v>7</v>
@@ -3752,7 +3739,7 @@
         <v>6</v>
       </c>
       <c r="T6" s="1">
-        <f t="shared" ref="T5:T14" si="1">SUM(K6:Q6)</f>
+        <f t="shared" ref="T6:T14" si="1">SUM(K6:Q6)</f>
         <v>49</v>
       </c>
     </row>
@@ -3831,7 +3818,7 @@
       <c r="C8" s="43">
         <v>4</v>
       </c>
-      <c r="D8" s="85">
+      <c r="D8" s="82">
         <v>12</v>
       </c>
       <c r="E8" s="44">
@@ -3906,7 +3893,7 @@
         <f t="shared" ref="F9:F14" si="2">SUM(C9:E9)</f>
         <v>28</v>
       </c>
-      <c r="G9" s="79">
+      <c r="G9" s="76">
         <v>5</v>
       </c>
       <c r="H9" s="5">
@@ -3971,7 +3958,7 @@
         <f>SUM(C10:E10)</f>
         <v>28</v>
       </c>
-      <c r="G10" s="80">
+      <c r="G10" s="77">
         <v>1</v>
       </c>
       <c r="H10" s="49">
@@ -4036,7 +4023,7 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="G11" s="81">
+      <c r="G11" s="78">
         <v>6</v>
       </c>
       <c r="H11" s="1">
@@ -4091,7 +4078,7 @@
       <c r="C12" s="43">
         <v>28</v>
       </c>
-      <c r="D12" s="85">
+      <c r="D12" s="82">
         <v>6</v>
       </c>
       <c r="E12" s="58">
@@ -4101,7 +4088,7 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="G12" s="82">
+      <c r="G12" s="79">
         <v>4</v>
       </c>
       <c r="H12" s="43">
@@ -4166,7 +4153,7 @@
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="G13" s="83">
+      <c r="G13" s="80">
         <v>3</v>
       </c>
       <c r="H13" s="1">
@@ -4221,7 +4208,7 @@
       <c r="C14" s="63">
         <v>16</v>
       </c>
-      <c r="D14" s="86">
+      <c r="D14" s="83">
         <v>39</v>
       </c>
       <c r="E14" s="64">
@@ -4231,7 +4218,7 @@
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="G14" s="84">
+      <c r="G14" s="81">
         <v>4</v>
       </c>
       <c r="H14" s="63">
@@ -4281,36 +4268,36 @@
         <v>65</v>
       </c>
       <c r="C15" s="1">
-        <f>SUM(C5:C14)</f>
-        <v>150</v>
+        <f t="shared" ref="C15:J15" si="3">SUM(C5:C14)</f>
+        <v>154</v>
       </c>
       <c r="D15" s="1">
-        <f>SUM(D5:D14)</f>
+        <f t="shared" si="3"/>
         <v>174</v>
       </c>
       <c r="E15" s="32">
-        <f>SUM(E5:E14)</f>
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
       <c r="F15" s="32">
-        <f>SUM(F5:F14)</f>
-        <v>409</v>
+        <f t="shared" si="3"/>
+        <v>413</v>
       </c>
       <c r="G15" s="1">
-        <f>SUM(G5:G14)</f>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="H15" s="1">
-        <f>SUM(H5:H14)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="I15" s="1">
-        <f>SUM(I5:I14)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="J15" s="32">
-        <f>SUM(J5:J14)</f>
-        <v>22</v>
+        <f t="shared" si="3"/>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -4450,16 +4437,16 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="91">
+      <c r="A28" s="32">
         <v>1</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="92">
-        <v>34</v>
-      </c>
-      <c r="D28" s="91">
+      <c r="C28" s="1">
+        <v>38</v>
+      </c>
+      <c r="D28" s="32">
         <v>18</v>
       </c>
       <c r="E28" s="29">
@@ -4468,13 +4455,13 @@
       <c r="F28" s="29">
         <v>67</v>
       </c>
-      <c r="G28" s="91">
-        <v>2</v>
-      </c>
-      <c r="H28" s="91">
-        <v>2</v>
-      </c>
-      <c r="I28" s="96">
+      <c r="G28" s="32">
+        <v>2</v>
+      </c>
+      <c r="H28" s="32">
+        <v>2</v>
+      </c>
+      <c r="I28" s="87">
         <v>0</v>
       </c>
       <c r="J28" s="20">
@@ -4483,26 +4470,26 @@
       <c r="K28" s="36">
         <v>1</v>
       </c>
-      <c r="L28" s="92">
-        <v>5</v>
-      </c>
-      <c r="M28" s="92">
-        <v>2</v>
-      </c>
-      <c r="N28" s="92">
-        <v>1</v>
-      </c>
-      <c r="O28" s="92">
-        <v>8</v>
-      </c>
-      <c r="P28" s="92">
+      <c r="L28" s="1">
+        <v>5</v>
+      </c>
+      <c r="M28" s="1">
+        <v>2</v>
+      </c>
+      <c r="N28" s="1">
+        <v>1</v>
+      </c>
+      <c r="O28" s="1">
+        <v>8</v>
+      </c>
+      <c r="P28" s="1">
         <v>6</v>
       </c>
       <c r="Q28" s="4">
         <v>10</v>
       </c>
       <c r="R28" s="34">
-        <f>SUM(K28:Q28)/6</f>
+        <f t="shared" ref="R28:R37" si="4">SUM(K28:Q28)/6</f>
         <v>5.5</v>
       </c>
       <c r="S28" s="4">
@@ -4510,16 +4497,16 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="87">
+      <c r="A29" s="41">
         <v>2</v>
       </c>
       <c r="B29" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="89">
-        <v>8</v>
-      </c>
-      <c r="D29" s="90">
+      <c r="C29" s="43">
+        <v>8</v>
+      </c>
+      <c r="D29" s="82">
         <v>21</v>
       </c>
       <c r="E29" s="44">
@@ -4528,41 +4515,41 @@
       <c r="F29" s="44">
         <v>37</v>
       </c>
-      <c r="G29" s="90">
-        <v>1</v>
-      </c>
-      <c r="H29" s="90">
-        <v>1</v>
-      </c>
-      <c r="I29" s="93">
+      <c r="G29" s="82">
+        <v>1</v>
+      </c>
+      <c r="H29" s="82">
+        <v>1</v>
+      </c>
+      <c r="I29" s="84">
         <v>1</v>
       </c>
       <c r="J29" s="47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K29" s="48">
         <v>7</v>
       </c>
-      <c r="L29" s="88">
-        <v>3</v>
-      </c>
-      <c r="M29" s="88">
-        <v>5</v>
-      </c>
-      <c r="N29" s="88">
-        <v>6</v>
-      </c>
-      <c r="O29" s="88">
-        <v>10</v>
-      </c>
-      <c r="P29" s="88">
+      <c r="L29" s="49">
+        <v>3</v>
+      </c>
+      <c r="M29" s="49">
+        <v>5</v>
+      </c>
+      <c r="N29" s="49">
+        <v>6</v>
+      </c>
+      <c r="O29" s="49">
+        <v>10</v>
+      </c>
+      <c r="P29" s="49">
         <v>10</v>
       </c>
       <c r="Q29" s="50">
         <v>8</v>
       </c>
       <c r="R29" s="51">
-        <f>SUM(K29:Q29)/6</f>
+        <f t="shared" si="4"/>
         <v>8.1666666666666661</v>
       </c>
       <c r="S29" s="50">
@@ -4570,16 +4557,16 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="91">
+      <c r="A30" s="32">
         <v>3</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="92">
+      <c r="C30" s="1">
         <v>12</v>
       </c>
-      <c r="D30" s="91">
+      <c r="D30" s="32">
         <v>12</v>
       </c>
       <c r="E30" s="29">
@@ -4588,13 +4575,13 @@
       <c r="F30" s="29">
         <v>24</v>
       </c>
-      <c r="G30" s="91">
-        <v>2</v>
-      </c>
-      <c r="H30" s="91">
-        <v>2</v>
-      </c>
-      <c r="I30" s="95">
+      <c r="G30" s="32">
+        <v>2</v>
+      </c>
+      <c r="H30" s="32">
+        <v>2</v>
+      </c>
+      <c r="I30" s="86">
         <v>4</v>
       </c>
       <c r="J30" s="22">
@@ -4603,26 +4590,26 @@
       <c r="K30" s="35">
         <v>5</v>
       </c>
-      <c r="L30" s="92">
-        <v>7</v>
-      </c>
-      <c r="M30" s="92">
-        <v>10</v>
-      </c>
-      <c r="N30" s="92">
-        <v>9</v>
-      </c>
-      <c r="O30" s="92">
-        <v>7</v>
-      </c>
-      <c r="P30" s="92">
+      <c r="L30" s="1">
+        <v>7</v>
+      </c>
+      <c r="M30" s="1">
+        <v>10</v>
+      </c>
+      <c r="N30" s="1">
+        <v>9</v>
+      </c>
+      <c r="O30" s="1">
+        <v>7</v>
+      </c>
+      <c r="P30" s="1">
         <v>1</v>
       </c>
       <c r="Q30" s="4">
         <v>1</v>
       </c>
       <c r="R30" s="34">
-        <f>SUM(K30:Q30)/6</f>
+        <f t="shared" si="4"/>
         <v>6.666666666666667</v>
       </c>
       <c r="S30" s="4">
@@ -4630,16 +4617,16 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="87">
+      <c r="A31" s="41">
         <v>4</v>
       </c>
       <c r="B31" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="89">
-        <v>4</v>
-      </c>
-      <c r="D31" s="90">
+      <c r="C31" s="43">
+        <v>4</v>
+      </c>
+      <c r="D31" s="82">
         <v>12</v>
       </c>
       <c r="E31" s="44">
@@ -4651,10 +4638,10 @@
       <c r="G31" s="58">
         <v>8</v>
       </c>
-      <c r="H31" s="90">
-        <v>1</v>
-      </c>
-      <c r="I31" s="93">
+      <c r="H31" s="82">
+        <v>1</v>
+      </c>
+      <c r="I31" s="84">
         <v>2</v>
       </c>
       <c r="J31" s="47">
@@ -4663,26 +4650,26 @@
       <c r="K31" s="48">
         <v>9</v>
       </c>
-      <c r="L31" s="88">
-        <v>8</v>
-      </c>
-      <c r="M31" s="88">
-        <v>8</v>
-      </c>
-      <c r="N31" s="88">
-        <v>10</v>
-      </c>
-      <c r="O31" s="88">
-        <v>1</v>
-      </c>
-      <c r="P31" s="88">
+      <c r="L31" s="49">
+        <v>8</v>
+      </c>
+      <c r="M31" s="49">
+        <v>8</v>
+      </c>
+      <c r="N31" s="49">
+        <v>10</v>
+      </c>
+      <c r="O31" s="49">
+        <v>1</v>
+      </c>
+      <c r="P31" s="49">
         <v>9</v>
       </c>
       <c r="Q31" s="50">
         <v>5</v>
       </c>
       <c r="R31" s="51">
-        <f>SUM(K31:Q31)/6</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333339</v>
       </c>
       <c r="S31" s="50">
@@ -4714,7 +4701,7 @@
       <c r="H32" s="16">
         <v>2</v>
       </c>
-      <c r="I32" s="96">
+      <c r="I32" s="87">
         <v>1</v>
       </c>
       <c r="J32" s="21">
@@ -4742,7 +4729,7 @@
         <v>7</v>
       </c>
       <c r="R32" s="34">
-        <f>SUM(K32:Q32)/6</f>
+        <f t="shared" si="4"/>
         <v>6.5</v>
       </c>
       <c r="S32" s="4">
@@ -4750,16 +4737,16 @@
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="87">
+      <c r="A33" s="41">
         <v>6</v>
       </c>
       <c r="B33" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="88">
-        <v>2</v>
-      </c>
-      <c r="D33" s="87">
+      <c r="C33" s="49">
+        <v>2</v>
+      </c>
+      <c r="D33" s="41">
         <v>23</v>
       </c>
       <c r="E33" s="58">
@@ -4768,13 +4755,13 @@
       <c r="F33" s="44">
         <v>28</v>
       </c>
-      <c r="G33" s="97">
-        <v>1</v>
-      </c>
-      <c r="H33" s="87">
-        <v>1</v>
-      </c>
-      <c r="I33" s="98">
+      <c r="G33" s="88">
+        <v>1</v>
+      </c>
+      <c r="H33" s="41">
+        <v>1</v>
+      </c>
+      <c r="I33" s="89">
         <v>2</v>
       </c>
       <c r="J33" s="57">
@@ -4783,26 +4770,26 @@
       <c r="K33" s="48">
         <v>10</v>
       </c>
-      <c r="L33" s="88">
-        <v>2</v>
-      </c>
-      <c r="M33" s="88">
-        <v>9</v>
-      </c>
-      <c r="N33" s="88">
-        <v>8</v>
-      </c>
-      <c r="O33" s="88">
-        <v>9</v>
-      </c>
-      <c r="P33" s="88">
+      <c r="L33" s="49">
+        <v>2</v>
+      </c>
+      <c r="M33" s="49">
+        <v>9</v>
+      </c>
+      <c r="N33" s="49">
+        <v>8</v>
+      </c>
+      <c r="O33" s="49">
+        <v>9</v>
+      </c>
+      <c r="P33" s="49">
         <v>8</v>
       </c>
       <c r="Q33" s="50">
         <v>4</v>
       </c>
       <c r="R33" s="51">
-        <f>SUM(K33:Q33)/6</f>
+        <f t="shared" si="4"/>
         <v>8.3333333333333339</v>
       </c>
       <c r="S33" s="50">
@@ -4828,13 +4815,13 @@
       <c r="F34" s="14">
         <v>44</v>
       </c>
-      <c r="G34" s="94">
+      <c r="G34" s="85">
         <v>6</v>
       </c>
       <c r="H34" s="32">
         <v>2</v>
       </c>
-      <c r="I34" s="95">
+      <c r="I34" s="86">
         <v>2</v>
       </c>
       <c r="J34" s="22">
@@ -4862,7 +4849,7 @@
         <v>2</v>
       </c>
       <c r="R34" s="34">
-        <f>SUM(K34:Q34)/6</f>
+        <f t="shared" si="4"/>
         <v>4.5</v>
       </c>
       <c r="S34" s="4">
@@ -4870,16 +4857,16 @@
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="87">
+      <c r="A35" s="41">
         <v>8</v>
       </c>
       <c r="B35" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="89">
+      <c r="C35" s="43">
         <v>28</v>
       </c>
-      <c r="D35" s="90">
+      <c r="D35" s="82">
         <v>6</v>
       </c>
       <c r="E35" s="58">
@@ -4891,10 +4878,10 @@
       <c r="G35" s="44">
         <v>4</v>
       </c>
-      <c r="H35" s="90">
-        <v>1</v>
-      </c>
-      <c r="I35" s="93">
+      <c r="H35" s="82">
+        <v>1</v>
+      </c>
+      <c r="I35" s="84">
         <v>2</v>
       </c>
       <c r="J35" s="60">
@@ -4903,26 +4890,26 @@
       <c r="K35" s="48">
         <v>3</v>
       </c>
-      <c r="L35" s="88">
-        <v>10</v>
-      </c>
-      <c r="M35" s="88">
-        <v>7</v>
-      </c>
-      <c r="N35" s="88">
-        <v>5</v>
-      </c>
-      <c r="O35" s="88">
-        <v>4</v>
-      </c>
-      <c r="P35" s="88">
+      <c r="L35" s="49">
+        <v>10</v>
+      </c>
+      <c r="M35" s="49">
+        <v>7</v>
+      </c>
+      <c r="N35" s="49">
+        <v>5</v>
+      </c>
+      <c r="O35" s="49">
+        <v>4</v>
+      </c>
+      <c r="P35" s="49">
         <v>7</v>
       </c>
       <c r="Q35" s="50">
         <v>3</v>
       </c>
       <c r="R35" s="51">
-        <f>SUM(K35:Q35)/6</f>
+        <f t="shared" si="4"/>
         <v>6.5</v>
       </c>
       <c r="S35" s="50">
@@ -4948,13 +4935,13 @@
       <c r="F36" s="29">
         <v>60</v>
       </c>
-      <c r="G36" s="99">
+      <c r="G36" s="90">
         <v>3</v>
       </c>
       <c r="H36" s="32">
         <v>2</v>
       </c>
-      <c r="I36" s="96">
+      <c r="I36" s="87">
         <v>0</v>
       </c>
       <c r="J36" s="22">
@@ -4982,7 +4969,7 @@
         <v>9</v>
       </c>
       <c r="R36" s="34">
-        <f>SUM(K36:Q36)/6</f>
+        <f t="shared" si="4"/>
         <v>5.666666666666667</v>
       </c>
       <c r="S36" s="4">
@@ -4999,7 +4986,7 @@
       <c r="C37" s="63">
         <v>16</v>
       </c>
-      <c r="D37" s="86">
+      <c r="D37" s="83">
         <v>39</v>
       </c>
       <c r="E37" s="64">
@@ -5008,10 +4995,10 @@
       <c r="F37" s="65">
         <v>64</v>
       </c>
-      <c r="G37" s="100">
-        <v>4</v>
-      </c>
-      <c r="H37" s="86">
+      <c r="G37" s="91">
+        <v>4</v>
+      </c>
+      <c r="H37" s="83">
         <v>2</v>
       </c>
       <c r="I37" s="61">
@@ -5042,7 +5029,7 @@
         <v>6</v>
       </c>
       <c r="R37" s="74">
-        <f>SUM(K37:Q37)/6</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="S37" s="71">

</xml_diff>

<commit_message>
Summary Updated computer player logic Actions: ADD Rankings for Destination London edition Problems
</commit_message>
<xml_diff>
--- a/docs/edition_points.xlsx
+++ b/docs/edition_points.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Compile\careers\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8460152F-881F-4BCB-9B75-41C608772D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB470DF-0EFC-486C-83A6-FC4DB1C31A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4350" yWindow="960" windowWidth="24075" windowHeight="13500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4185" yWindow="1005" windowWidth="24075" windowHeight="13500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hi-Tech v1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hi-Tech v2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hi-Tech Jobs" sheetId="1" r:id="rId1"/>
+    <sheet name="Hi-Tech Professions" sheetId="2" r:id="rId2"/>
     <sheet name="Jazz Age" sheetId="3" r:id="rId3"/>
+    <sheet name="Destination London" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="91">
   <si>
     <t>Occupation</t>
   </si>
@@ -263,6 +264,54 @@
   </si>
   <si>
     <t>Roosevelt College, Prohibition Agent</t>
+  </si>
+  <si>
+    <t>Guinness</t>
+  </si>
+  <si>
+    <t>Bunch of Grapes</t>
+  </si>
+  <si>
+    <t>Oxford</t>
+  </si>
+  <si>
+    <t>Harrods</t>
+  </si>
+  <si>
+    <t>Westminster</t>
+  </si>
+  <si>
+    <t>Stonehenge</t>
+  </si>
+  <si>
+    <t>Houses of Parliament</t>
+  </si>
+  <si>
+    <t>Buckingham Palace</t>
+  </si>
+  <si>
+    <t>Tower of London</t>
+  </si>
+  <si>
+    <t>Sightseeing Tour</t>
+  </si>
+  <si>
+    <t>Ranking Total</t>
+  </si>
+  <si>
+    <t>Guiness, Sightseeing Tour</t>
+  </si>
+  <si>
+    <t>Guiness, Houses of Parliament</t>
+  </si>
+  <si>
+    <t>Tower of London, Guiness</t>
+  </si>
+  <si>
+    <t>Harrods, Houses of Parliament</t>
+  </si>
+  <si>
+    <t>Oxford, Stonehenge</t>
   </si>
 </sst>
 </file>
@@ -457,7 +506,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -711,6 +760,61 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1967,7 +2071,7 @@
   <dimension ref="A3:T40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3511,14 +3615,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66559D5-1C3E-471D-81A3-258D37D68792}">
   <dimension ref="A3:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="8" width="10.28515625" customWidth="1"/>
+    <col min="3" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="8" width="10.28515625" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" customWidth="1"/>
@@ -3667,7 +3773,7 @@
         <v>10</v>
       </c>
       <c r="R5" s="34">
-        <f t="shared" ref="R5:R14" si="0">SUM(K5:Q5)/6</f>
+        <f>SUM(K5:Q5)/6</f>
         <v>5.5</v>
       </c>
       <c r="S5" s="4">
@@ -3732,7 +3838,7 @@
         <v>8</v>
       </c>
       <c r="R6" s="51">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="R5:R14" si="0">SUM(K6:Q6)/6</f>
         <v>8.1666666666666661</v>
       </c>
       <c r="S6" s="50">
@@ -5052,4 +5158,1550 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5E5147-5992-4431-822F-ABC86F78CFE9}">
+  <dimension ref="A3:T43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="12"/>
+      <c r="C3" s="92" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="92" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="94"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="S4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="T4" s="28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44</v>
+      </c>
+      <c r="D5" s="32">
+        <v>24</v>
+      </c>
+      <c r="E5" s="29">
+        <v>10</v>
+      </c>
+      <c r="F5" s="29">
+        <f>SUM(C5:E5)</f>
+        <v>78</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="20">
+        <v>3</v>
+      </c>
+      <c r="K5" s="103">
+        <v>1</v>
+      </c>
+      <c r="L5" s="32">
+        <v>1</v>
+      </c>
+      <c r="M5" s="32">
+        <v>2</v>
+      </c>
+      <c r="N5" s="32">
+        <v>1</v>
+      </c>
+      <c r="O5" s="32">
+        <v>9</v>
+      </c>
+      <c r="P5" s="32">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="86">
+        <v>9</v>
+      </c>
+      <c r="R5" s="34">
+        <v>4.833333333333333</v>
+      </c>
+      <c r="S5" s="86">
+        <v>1</v>
+      </c>
+      <c r="T5" s="32">
+        <f>SUM(K5:Q5)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="41">
+        <v>2</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="43">
+        <v>10</v>
+      </c>
+      <c r="D6" s="82">
+        <v>21</v>
+      </c>
+      <c r="E6" s="44">
+        <v>8</v>
+      </c>
+      <c r="F6" s="44">
+        <f>SUM(C6:E6)</f>
+        <v>39</v>
+      </c>
+      <c r="G6" s="43">
+        <v>1</v>
+      </c>
+      <c r="H6" s="43">
+        <v>1</v>
+      </c>
+      <c r="I6" s="46">
+        <v>1</v>
+      </c>
+      <c r="J6" s="47">
+        <v>1</v>
+      </c>
+      <c r="K6" s="105">
+        <v>8</v>
+      </c>
+      <c r="L6" s="95">
+        <v>4</v>
+      </c>
+      <c r="M6" s="95">
+        <v>5</v>
+      </c>
+      <c r="N6" s="95">
+        <v>6</v>
+      </c>
+      <c r="O6" s="95">
+        <v>10</v>
+      </c>
+      <c r="P6" s="95">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="89">
+        <v>8</v>
+      </c>
+      <c r="R6" s="51">
+        <v>8.5</v>
+      </c>
+      <c r="S6" s="89">
+        <v>6</v>
+      </c>
+      <c r="T6" s="1">
+        <f t="shared" ref="T6:T14" si="0">SUM(K6:Q6)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="32">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="1">
+        <v>12</v>
+      </c>
+      <c r="D7" s="32">
+        <v>12</v>
+      </c>
+      <c r="E7" s="29">
+        <v>0</v>
+      </c>
+      <c r="F7" s="29">
+        <f>SUM(C7:E7)</f>
+        <v>24</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="4">
+        <v>4</v>
+      </c>
+      <c r="J7" s="22">
+        <v>2</v>
+      </c>
+      <c r="K7" s="107">
+        <v>7</v>
+      </c>
+      <c r="L7" s="114">
+        <v>7</v>
+      </c>
+      <c r="M7" s="114">
+        <v>10</v>
+      </c>
+      <c r="N7" s="114">
+        <v>9</v>
+      </c>
+      <c r="O7" s="114">
+        <v>7</v>
+      </c>
+      <c r="P7" s="114">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="86">
+        <v>1</v>
+      </c>
+      <c r="R7" s="34">
+        <v>7</v>
+      </c>
+      <c r="S7" s="86">
+        <v>9</v>
+      </c>
+      <c r="T7" s="1">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="41">
+        <v>4</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="43">
+        <v>4</v>
+      </c>
+      <c r="D8" s="82">
+        <v>12</v>
+      </c>
+      <c r="E8" s="44">
+        <v>3</v>
+      </c>
+      <c r="F8" s="44">
+        <f>SUM(C8:E8)</f>
+        <v>19</v>
+      </c>
+      <c r="G8" s="75">
+        <v>8</v>
+      </c>
+      <c r="H8" s="43">
+        <v>1</v>
+      </c>
+      <c r="I8" s="46">
+        <v>2</v>
+      </c>
+      <c r="J8" s="47">
+        <v>2</v>
+      </c>
+      <c r="K8" s="105">
+        <v>9</v>
+      </c>
+      <c r="L8" s="95">
+        <v>8</v>
+      </c>
+      <c r="M8" s="95">
+        <v>8</v>
+      </c>
+      <c r="N8" s="95">
+        <v>10</v>
+      </c>
+      <c r="O8" s="95">
+        <v>1</v>
+      </c>
+      <c r="P8" s="95">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="89">
+        <v>4</v>
+      </c>
+      <c r="R8" s="51">
+        <v>8</v>
+      </c>
+      <c r="S8" s="89">
+        <v>10</v>
+      </c>
+      <c r="T8" s="1">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="32">
+        <v>5</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="5">
+        <v>16</v>
+      </c>
+      <c r="D9" s="16">
+        <v>12</v>
+      </c>
+      <c r="E9" s="14">
+        <v>8</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" ref="F9:F14" si="1">SUM(C9:E9)</f>
+        <v>36</v>
+      </c>
+      <c r="G9" s="76">
+        <v>5</v>
+      </c>
+      <c r="H9" s="5">
+        <v>2</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1</v>
+      </c>
+      <c r="J9" s="21">
+        <v>2</v>
+      </c>
+      <c r="K9" s="107">
+        <v>5</v>
+      </c>
+      <c r="L9" s="32">
+        <v>6</v>
+      </c>
+      <c r="M9" s="32">
+        <v>4</v>
+      </c>
+      <c r="N9" s="32">
+        <v>7</v>
+      </c>
+      <c r="O9" s="32">
+        <v>4</v>
+      </c>
+      <c r="P9" s="32">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="86">
+        <v>6</v>
+      </c>
+      <c r="R9" s="34">
+        <v>6</v>
+      </c>
+      <c r="S9" s="115">
+        <v>7</v>
+      </c>
+      <c r="T9" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="41">
+        <v>6</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="49">
+        <v>2</v>
+      </c>
+      <c r="D10" s="41">
+        <v>23</v>
+      </c>
+      <c r="E10" s="58">
+        <v>3</v>
+      </c>
+      <c r="F10" s="44">
+        <f>SUM(C10:E10)</f>
+        <v>28</v>
+      </c>
+      <c r="G10" s="77">
+        <v>2</v>
+      </c>
+      <c r="H10" s="49">
+        <v>2</v>
+      </c>
+      <c r="I10" s="50">
+        <v>2</v>
+      </c>
+      <c r="J10" s="57">
+        <v>2</v>
+      </c>
+      <c r="K10" s="105">
+        <v>10</v>
+      </c>
+      <c r="L10" s="95">
+        <v>3</v>
+      </c>
+      <c r="M10" s="95">
+        <v>9</v>
+      </c>
+      <c r="N10" s="95">
+        <v>8</v>
+      </c>
+      <c r="O10" s="95">
+        <v>8</v>
+      </c>
+      <c r="P10" s="95">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="89">
+        <v>2</v>
+      </c>
+      <c r="R10" s="51">
+        <v>7</v>
+      </c>
+      <c r="S10" s="89">
+        <v>8</v>
+      </c>
+      <c r="T10" s="1">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="32">
+        <v>7</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="1">
+        <v>38</v>
+      </c>
+      <c r="D11" s="32">
+        <v>6</v>
+      </c>
+      <c r="E11" s="15">
+        <v>5</v>
+      </c>
+      <c r="F11" s="14">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="G11" s="78">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2</v>
+      </c>
+      <c r="I11" s="4">
+        <v>2</v>
+      </c>
+      <c r="J11" s="22">
+        <v>2</v>
+      </c>
+      <c r="K11" s="107">
+        <v>2</v>
+      </c>
+      <c r="L11" s="32">
+        <v>9</v>
+      </c>
+      <c r="M11" s="32">
+        <v>6</v>
+      </c>
+      <c r="N11" s="32">
+        <v>4</v>
+      </c>
+      <c r="O11" s="32">
+        <v>2</v>
+      </c>
+      <c r="P11" s="32">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="86">
+        <v>3</v>
+      </c>
+      <c r="R11" s="34">
+        <v>4.833333333333333</v>
+      </c>
+      <c r="S11" s="86">
+        <v>4</v>
+      </c>
+      <c r="T11" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="41">
+        <v>8</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="43">
+        <v>30</v>
+      </c>
+      <c r="D12" s="82">
+        <v>6</v>
+      </c>
+      <c r="E12" s="58">
+        <v>4</v>
+      </c>
+      <c r="F12" s="44">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="G12" s="79">
+        <v>5</v>
+      </c>
+      <c r="H12" s="43">
+        <v>1</v>
+      </c>
+      <c r="I12" s="46">
+        <v>2</v>
+      </c>
+      <c r="J12" s="60">
+        <v>2</v>
+      </c>
+      <c r="K12" s="105">
+        <v>4</v>
+      </c>
+      <c r="L12" s="95">
+        <v>10</v>
+      </c>
+      <c r="M12" s="95">
+        <v>7</v>
+      </c>
+      <c r="N12" s="95">
+        <v>5</v>
+      </c>
+      <c r="O12" s="95">
+        <v>3</v>
+      </c>
+      <c r="P12" s="95">
+        <v>9</v>
+      </c>
+      <c r="Q12" s="89">
+        <v>5</v>
+      </c>
+      <c r="R12" s="51">
+        <v>7.166666666666667</v>
+      </c>
+      <c r="S12" s="89">
+        <v>5</v>
+      </c>
+      <c r="T12" s="1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="32">
+        <v>9</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="1">
+        <v>12</v>
+      </c>
+      <c r="D13" s="32">
+        <v>20</v>
+      </c>
+      <c r="E13" s="25">
+        <v>30</v>
+      </c>
+      <c r="F13" s="29">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="G13" s="80">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0</v>
+      </c>
+      <c r="J13" s="22">
+        <v>2</v>
+      </c>
+      <c r="K13" s="107">
+        <v>6</v>
+      </c>
+      <c r="L13" s="114">
+        <v>5</v>
+      </c>
+      <c r="M13" s="114">
+        <v>1</v>
+      </c>
+      <c r="N13" s="114">
+        <v>3</v>
+      </c>
+      <c r="O13" s="114">
+        <v>6</v>
+      </c>
+      <c r="P13" s="114">
+        <v>7</v>
+      </c>
+      <c r="Q13" s="86">
+        <v>10</v>
+      </c>
+      <c r="R13" s="34">
+        <v>6.333333333333333</v>
+      </c>
+      <c r="S13" s="86">
+        <v>3</v>
+      </c>
+      <c r="T13" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="61">
+        <v>10</v>
+      </c>
+      <c r="B14" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="63">
+        <v>34</v>
+      </c>
+      <c r="D14" s="83">
+        <v>23</v>
+      </c>
+      <c r="E14" s="64">
+        <v>9</v>
+      </c>
+      <c r="F14" s="65">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="G14" s="81">
+        <v>4</v>
+      </c>
+      <c r="H14" s="63">
+        <v>2</v>
+      </c>
+      <c r="I14" s="67">
+        <v>1</v>
+      </c>
+      <c r="J14" s="68">
+        <v>3</v>
+      </c>
+      <c r="K14" s="109">
+        <v>3</v>
+      </c>
+      <c r="L14" s="83">
+        <v>2</v>
+      </c>
+      <c r="M14" s="83">
+        <v>3</v>
+      </c>
+      <c r="N14" s="83">
+        <v>2</v>
+      </c>
+      <c r="O14" s="83">
+        <v>5</v>
+      </c>
+      <c r="P14" s="83">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="61">
+        <v>7</v>
+      </c>
+      <c r="R14" s="74">
+        <v>4.5</v>
+      </c>
+      <c r="S14" s="110">
+        <v>2</v>
+      </c>
+      <c r="T14" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" ref="C15:J15" si="2">SUM(C5:C14)</f>
+        <v>202</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="E15" s="32">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="F15" s="32">
+        <f t="shared" si="2"/>
+        <v>441</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="J15" s="32">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="98" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="99" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="99" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="98" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="98" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="100" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30" s="101" t="s">
+        <v>24</v>
+      </c>
+      <c r="K30" s="102" t="s">
+        <v>37</v>
+      </c>
+      <c r="L30" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="M30" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="N30" s="98" t="s">
+        <v>10</v>
+      </c>
+      <c r="O30" s="98" t="s">
+        <v>4</v>
+      </c>
+      <c r="P30" s="98" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q30" s="100" t="s">
+        <v>7</v>
+      </c>
+      <c r="R30" s="100" t="s">
+        <v>50</v>
+      </c>
+      <c r="S30" s="101" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="32">
+        <v>1</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="32">
+        <v>44</v>
+      </c>
+      <c r="D31" s="32">
+        <v>24</v>
+      </c>
+      <c r="E31" s="29">
+        <v>10</v>
+      </c>
+      <c r="F31" s="29">
+        <v>78</v>
+      </c>
+      <c r="G31" s="32">
+        <v>2</v>
+      </c>
+      <c r="H31" s="32">
+        <v>2</v>
+      </c>
+      <c r="I31" s="87">
+        <v>0</v>
+      </c>
+      <c r="J31" s="20">
+        <v>3</v>
+      </c>
+      <c r="K31" s="103">
+        <v>1</v>
+      </c>
+      <c r="L31" s="32">
+        <v>1</v>
+      </c>
+      <c r="M31" s="32">
+        <v>2</v>
+      </c>
+      <c r="N31" s="32">
+        <v>1</v>
+      </c>
+      <c r="O31" s="32">
+        <v>9</v>
+      </c>
+      <c r="P31" s="32">
+        <v>6</v>
+      </c>
+      <c r="Q31" s="86">
+        <v>9</v>
+      </c>
+      <c r="R31" s="34">
+        <f>SUM(K31:Q31)/6</f>
+        <v>4.833333333333333</v>
+      </c>
+      <c r="S31" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="95">
+        <v>2</v>
+      </c>
+      <c r="B32" s="106" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="113">
+        <v>10</v>
+      </c>
+      <c r="D32" s="113">
+        <v>21</v>
+      </c>
+      <c r="E32" s="44">
+        <v>8</v>
+      </c>
+      <c r="F32" s="44">
+        <v>39</v>
+      </c>
+      <c r="G32" s="113">
+        <v>1</v>
+      </c>
+      <c r="H32" s="113">
+        <v>1</v>
+      </c>
+      <c r="I32" s="84">
+        <v>1</v>
+      </c>
+      <c r="J32" s="47">
+        <v>1</v>
+      </c>
+      <c r="K32" s="105">
+        <v>8</v>
+      </c>
+      <c r="L32" s="95">
+        <v>4</v>
+      </c>
+      <c r="M32" s="95">
+        <v>5</v>
+      </c>
+      <c r="N32" s="95">
+        <v>6</v>
+      </c>
+      <c r="O32" s="95">
+        <v>10</v>
+      </c>
+      <c r="P32" s="95">
+        <v>10</v>
+      </c>
+      <c r="Q32" s="89">
+        <v>8</v>
+      </c>
+      <c r="R32" s="51">
+        <f>SUM(K32:Q32)/6</f>
+        <v>8.5</v>
+      </c>
+      <c r="S32" s="89">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="114">
+        <v>3</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="114">
+        <v>12</v>
+      </c>
+      <c r="D33" s="114">
+        <v>12</v>
+      </c>
+      <c r="E33" s="29">
+        <v>0</v>
+      </c>
+      <c r="F33" s="29">
+        <v>24</v>
+      </c>
+      <c r="G33" s="114">
+        <v>2</v>
+      </c>
+      <c r="H33" s="114">
+        <v>2</v>
+      </c>
+      <c r="I33" s="86">
+        <v>4</v>
+      </c>
+      <c r="J33" s="22">
+        <v>2</v>
+      </c>
+      <c r="K33" s="107">
+        <v>7</v>
+      </c>
+      <c r="L33" s="114">
+        <v>7</v>
+      </c>
+      <c r="M33" s="114">
+        <v>10</v>
+      </c>
+      <c r="N33" s="114">
+        <v>9</v>
+      </c>
+      <c r="O33" s="114">
+        <v>7</v>
+      </c>
+      <c r="P33" s="114">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="86">
+        <v>1</v>
+      </c>
+      <c r="R33" s="34">
+        <f>SUM(K33:Q33)/6</f>
+        <v>7</v>
+      </c>
+      <c r="S33" s="86">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="95">
+        <v>4</v>
+      </c>
+      <c r="B34" s="106" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="113">
+        <v>4</v>
+      </c>
+      <c r="D34" s="113">
+        <v>12</v>
+      </c>
+      <c r="E34" s="44">
+        <v>3</v>
+      </c>
+      <c r="F34" s="44">
+        <v>19</v>
+      </c>
+      <c r="G34" s="58">
+        <v>8</v>
+      </c>
+      <c r="H34" s="113">
+        <v>1</v>
+      </c>
+      <c r="I34" s="84">
+        <v>2</v>
+      </c>
+      <c r="J34" s="47">
+        <v>2</v>
+      </c>
+      <c r="K34" s="105">
+        <v>9</v>
+      </c>
+      <c r="L34" s="95">
+        <v>8</v>
+      </c>
+      <c r="M34" s="95">
+        <v>8</v>
+      </c>
+      <c r="N34" s="95">
+        <v>10</v>
+      </c>
+      <c r="O34" s="95">
+        <v>1</v>
+      </c>
+      <c r="P34" s="95">
+        <v>8</v>
+      </c>
+      <c r="Q34" s="89">
+        <v>4</v>
+      </c>
+      <c r="R34" s="51">
+        <f>SUM(K34:Q34)/6</f>
+        <v>8</v>
+      </c>
+      <c r="S34" s="89">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="32">
+        <v>5</v>
+      </c>
+      <c r="B35" s="108" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="16">
+        <v>16</v>
+      </c>
+      <c r="D35" s="16">
+        <v>12</v>
+      </c>
+      <c r="E35" s="14">
+        <v>8</v>
+      </c>
+      <c r="F35" s="14">
+        <v>36</v>
+      </c>
+      <c r="G35" s="15">
+        <v>5</v>
+      </c>
+      <c r="H35" s="16">
+        <v>2</v>
+      </c>
+      <c r="I35" s="87">
+        <v>1</v>
+      </c>
+      <c r="J35" s="21">
+        <v>2</v>
+      </c>
+      <c r="K35" s="107">
+        <v>5</v>
+      </c>
+      <c r="L35" s="32">
+        <v>6</v>
+      </c>
+      <c r="M35" s="32">
+        <v>4</v>
+      </c>
+      <c r="N35" s="32">
+        <v>7</v>
+      </c>
+      <c r="O35" s="32">
+        <v>4</v>
+      </c>
+      <c r="P35" s="32">
+        <v>4</v>
+      </c>
+      <c r="Q35" s="86">
+        <v>6</v>
+      </c>
+      <c r="R35" s="34">
+        <f>SUM(K35:Q35)/6</f>
+        <v>6</v>
+      </c>
+      <c r="S35" s="115">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="95">
+        <v>6</v>
+      </c>
+      <c r="B36" s="104" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="95">
+        <v>2</v>
+      </c>
+      <c r="D36" s="95">
+        <v>23</v>
+      </c>
+      <c r="E36" s="58">
+        <v>3</v>
+      </c>
+      <c r="F36" s="44">
+        <v>28</v>
+      </c>
+      <c r="G36" s="88">
+        <v>2</v>
+      </c>
+      <c r="H36" s="95">
+        <v>2</v>
+      </c>
+      <c r="I36" s="89">
+        <v>2</v>
+      </c>
+      <c r="J36" s="57">
+        <v>2</v>
+      </c>
+      <c r="K36" s="105">
+        <v>10</v>
+      </c>
+      <c r="L36" s="95">
+        <v>3</v>
+      </c>
+      <c r="M36" s="95">
+        <v>9</v>
+      </c>
+      <c r="N36" s="95">
+        <v>8</v>
+      </c>
+      <c r="O36" s="95">
+        <v>8</v>
+      </c>
+      <c r="P36" s="95">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="89">
+        <v>2</v>
+      </c>
+      <c r="R36" s="51">
+        <f>SUM(K36:Q36)/6</f>
+        <v>7</v>
+      </c>
+      <c r="S36" s="89">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="32">
+        <v>7</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="32">
+        <v>38</v>
+      </c>
+      <c r="D37" s="32">
+        <v>6</v>
+      </c>
+      <c r="E37" s="15">
+        <v>5</v>
+      </c>
+      <c r="F37" s="14">
+        <v>49</v>
+      </c>
+      <c r="G37" s="85">
+        <v>6</v>
+      </c>
+      <c r="H37" s="32">
+        <v>2</v>
+      </c>
+      <c r="I37" s="86">
+        <v>2</v>
+      </c>
+      <c r="J37" s="22">
+        <v>2</v>
+      </c>
+      <c r="K37" s="107">
+        <v>2</v>
+      </c>
+      <c r="L37" s="32">
+        <v>9</v>
+      </c>
+      <c r="M37" s="32">
+        <v>6</v>
+      </c>
+      <c r="N37" s="32">
+        <v>4</v>
+      </c>
+      <c r="O37" s="32">
+        <v>2</v>
+      </c>
+      <c r="P37" s="32">
+        <v>3</v>
+      </c>
+      <c r="Q37" s="86">
+        <v>3</v>
+      </c>
+      <c r="R37" s="34">
+        <f>SUM(K37:Q37)/6</f>
+        <v>4.833333333333333</v>
+      </c>
+      <c r="S37" s="86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="95">
+        <v>8</v>
+      </c>
+      <c r="B38" s="106" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="113">
+        <v>30</v>
+      </c>
+      <c r="D38" s="113">
+        <v>6</v>
+      </c>
+      <c r="E38" s="58">
+        <v>4</v>
+      </c>
+      <c r="F38" s="44">
+        <v>40</v>
+      </c>
+      <c r="G38" s="44">
+        <v>5</v>
+      </c>
+      <c r="H38" s="113">
+        <v>1</v>
+      </c>
+      <c r="I38" s="84">
+        <v>2</v>
+      </c>
+      <c r="J38" s="60">
+        <v>2</v>
+      </c>
+      <c r="K38" s="105">
+        <v>4</v>
+      </c>
+      <c r="L38" s="95">
+        <v>10</v>
+      </c>
+      <c r="M38" s="95">
+        <v>7</v>
+      </c>
+      <c r="N38" s="95">
+        <v>5</v>
+      </c>
+      <c r="O38" s="95">
+        <v>3</v>
+      </c>
+      <c r="P38" s="95">
+        <v>9</v>
+      </c>
+      <c r="Q38" s="89">
+        <v>5</v>
+      </c>
+      <c r="R38" s="51">
+        <f>SUM(K38:Q38)/6</f>
+        <v>7.166666666666667</v>
+      </c>
+      <c r="S38" s="89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="114">
+        <v>9</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="114">
+        <v>12</v>
+      </c>
+      <c r="D39" s="114">
+        <v>20</v>
+      </c>
+      <c r="E39" s="25">
+        <v>30</v>
+      </c>
+      <c r="F39" s="29">
+        <v>62</v>
+      </c>
+      <c r="G39" s="90">
+        <v>4</v>
+      </c>
+      <c r="H39" s="114">
+        <v>2</v>
+      </c>
+      <c r="I39" s="87">
+        <v>0</v>
+      </c>
+      <c r="J39" s="22">
+        <v>2</v>
+      </c>
+      <c r="K39" s="107">
+        <v>6</v>
+      </c>
+      <c r="L39" s="114">
+        <v>5</v>
+      </c>
+      <c r="M39" s="114">
+        <v>1</v>
+      </c>
+      <c r="N39" s="114">
+        <v>3</v>
+      </c>
+      <c r="O39" s="114">
+        <v>6</v>
+      </c>
+      <c r="P39" s="114">
+        <v>7</v>
+      </c>
+      <c r="Q39" s="86">
+        <v>10</v>
+      </c>
+      <c r="R39" s="34">
+        <f>SUM(K39:Q39)/6</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="S39" s="86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" s="61">
+        <v>10</v>
+      </c>
+      <c r="B40" s="112" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="83">
+        <v>34</v>
+      </c>
+      <c r="D40" s="83">
+        <v>23</v>
+      </c>
+      <c r="E40" s="64">
+        <v>9</v>
+      </c>
+      <c r="F40" s="65">
+        <v>66</v>
+      </c>
+      <c r="G40" s="91">
+        <v>4</v>
+      </c>
+      <c r="H40" s="83">
+        <v>2</v>
+      </c>
+      <c r="I40" s="61">
+        <v>1</v>
+      </c>
+      <c r="J40" s="68">
+        <v>3</v>
+      </c>
+      <c r="K40" s="109">
+        <v>3</v>
+      </c>
+      <c r="L40" s="83">
+        <v>2</v>
+      </c>
+      <c r="M40" s="83">
+        <v>3</v>
+      </c>
+      <c r="N40" s="83">
+        <v>2</v>
+      </c>
+      <c r="O40" s="83">
+        <v>5</v>
+      </c>
+      <c r="P40" s="83">
+        <v>5</v>
+      </c>
+      <c r="Q40" s="61">
+        <v>7</v>
+      </c>
+      <c r="R40" s="74">
+        <f>SUM(K40:Q40)/6</f>
+        <v>4.5</v>
+      </c>
+      <c r="S40" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C41" s="111">
+        <f>SUM(C31:C40)</f>
+        <v>202</v>
+      </c>
+      <c r="D41" s="111">
+        <f>SUM(D31:D40)</f>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A31:S40">
+    <sortCondition ref="A31:A40"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="K3:S3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Summary Updated models, resources. Added functionality. Actions: UPDATE InDesign models, removing corner_square type, adding payday_square, hospital_square, unemployment_square, holiday_square UPDATE engine code and resources for the 4 new border square types ADD Wormhole functionality. Used in Professions-Hi-Tech for 6 professions. ADD Rectangle connecting Westminster Abbey to Houses of Parliament - InDesign model only.
Problems
</commit_message>
<xml_diff>
--- a/docs/edition_points.xlsx
+++ b/docs/edition_points.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Compile\careers\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB470DF-0EFC-486C-83A6-FC4DB1C31A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4CEA3D-60DA-440F-B470-3FF5A1565E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="1005" windowWidth="24075" windowHeight="13500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="765" windowWidth="24900" windowHeight="13545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hi-Tech Jobs" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Jazz Age" sheetId="3" r:id="rId3"/>
     <sheet name="Destination London" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Hi-Tech Professions'!$A$30:$Q$40</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="95">
   <si>
     <t>Occupation</t>
   </si>
@@ -312,6 +315,18 @@
   </si>
   <si>
     <t>Oxford, Stonehenge</t>
+  </si>
+  <si>
+    <t>Aerospace Engineering, Pharmaceutical Sciences</t>
+  </si>
+  <si>
+    <t>Aerospace Engineering, Patent Attorney</t>
+  </si>
+  <si>
+    <t>Quantum Computing, Patent Attorney</t>
+  </si>
+  <si>
+    <t>Average Rank</t>
   </si>
 </sst>
 </file>
@@ -506,7 +521,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -650,10 +665,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -696,9 +707,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -751,18 +759,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -808,15 +804,37 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1124,27 +1142,27 @@
   <sheetData>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="92" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="94"/>
+      <c r="C3" s="107" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="109"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="92" t="s">
+      <c r="K3" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="93"/>
-      <c r="S3" s="94"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="108"/>
+      <c r="R3" s="108"/>
+      <c r="S3" s="109"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -1546,14 +1564,14 @@
       <c r="D10" s="49">
         <v>23</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="56">
         <v>3</v>
       </c>
       <c r="F10" s="44">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="G10" s="72">
+      <c r="G10" s="70">
         <v>2</v>
       </c>
       <c r="H10" s="49">
@@ -1562,7 +1580,7 @@
       <c r="I10" s="50">
         <v>2</v>
       </c>
-      <c r="J10" s="57">
+      <c r="J10" s="55">
         <v>2</v>
       </c>
       <c r="K10" s="48">
@@ -1676,14 +1694,14 @@
       <c r="D12" s="43">
         <v>6</v>
       </c>
-      <c r="E12" s="58">
+      <c r="E12" s="56">
         <v>6</v>
       </c>
       <c r="F12" s="44">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="G12" s="59">
+      <c r="G12" s="57">
         <v>5</v>
       </c>
       <c r="H12" s="43">
@@ -1692,7 +1710,7 @@
       <c r="I12" s="46">
         <v>2</v>
       </c>
-      <c r="J12" s="60">
+      <c r="J12" s="58">
         <v>2</v>
       </c>
       <c r="K12" s="48">
@@ -1794,63 +1812,63 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="61">
-        <v>10</v>
-      </c>
-      <c r="B14" s="62" t="s">
+      <c r="A14" s="59">
+        <v>10</v>
+      </c>
+      <c r="B14" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="63">
+      <c r="C14" s="61">
         <v>34</v>
       </c>
-      <c r="D14" s="63">
+      <c r="D14" s="61">
         <v>23</v>
       </c>
-      <c r="E14" s="64">
-        <v>8</v>
-      </c>
-      <c r="F14" s="65">
+      <c r="E14" s="62">
+        <v>8</v>
+      </c>
+      <c r="F14" s="63">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="G14" s="66">
-        <v>4</v>
-      </c>
-      <c r="H14" s="63">
-        <v>2</v>
-      </c>
-      <c r="I14" s="67">
-        <v>1</v>
-      </c>
-      <c r="J14" s="68">
-        <v>3</v>
-      </c>
-      <c r="K14" s="69">
-        <v>3</v>
-      </c>
-      <c r="L14" s="63">
-        <v>2</v>
-      </c>
-      <c r="M14" s="63">
-        <v>4</v>
-      </c>
-      <c r="N14" s="63">
-        <v>3</v>
-      </c>
-      <c r="O14" s="63">
-        <v>5</v>
-      </c>
-      <c r="P14" s="63">
-        <v>6</v>
-      </c>
-      <c r="Q14" s="67">
-        <v>7</v>
-      </c>
-      <c r="R14" s="70">
+      <c r="G14" s="64">
+        <v>4</v>
+      </c>
+      <c r="H14" s="61">
+        <v>2</v>
+      </c>
+      <c r="I14" s="65">
+        <v>1</v>
+      </c>
+      <c r="J14" s="66">
+        <v>3</v>
+      </c>
+      <c r="K14" s="67">
+        <v>3</v>
+      </c>
+      <c r="L14" s="61">
+        <v>2</v>
+      </c>
+      <c r="M14" s="61">
+        <v>4</v>
+      </c>
+      <c r="N14" s="61">
+        <v>3</v>
+      </c>
+      <c r="O14" s="61">
+        <v>5</v>
+      </c>
+      <c r="P14" s="61">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="65">
+        <v>7</v>
+      </c>
+      <c r="R14" s="68">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="S14" s="71">
+      <c r="S14" s="69">
         <v>2</v>
       </c>
       <c r="T14" s="1">
@@ -2068,10 +2086,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2731D533-3189-49BB-AE83-771387574D8F}">
-  <dimension ref="A3:T40"/>
+  <dimension ref="A3:T52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2079,7 +2097,7 @@
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -2092,27 +2110,27 @@
   <sheetData>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="92" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="94"/>
+      <c r="C3" s="107" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="109"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="92" t="s">
+      <c r="K3" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="93"/>
-      <c r="S3" s="94"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="108"/>
+      <c r="R3" s="108"/>
+      <c r="S3" s="109"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -2177,29 +2195,29 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="32">
+      <c r="A5" s="112">
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="1">
-        <v>34</v>
-      </c>
-      <c r="D5" s="1">
-        <v>24</v>
+      <c r="C5" s="113">
+        <v>44</v>
+      </c>
+      <c r="D5" s="113">
+        <v>32</v>
       </c>
       <c r="E5" s="29">
         <v>15</v>
       </c>
       <c r="F5" s="29">
-        <f t="shared" ref="F5:F14" si="0">SUM(C5:E5)</f>
-        <v>73</v>
+        <f>SUM(C5:E5)</f>
+        <v>91</v>
       </c>
       <c r="G5" s="26">
         <v>2</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="113">
         <v>2</v>
       </c>
       <c r="I5" s="7">
@@ -2209,32 +2227,32 @@
         <v>3</v>
       </c>
       <c r="K5" s="36">
-        <v>3</v>
-      </c>
-      <c r="L5" s="1">
-        <v>2</v>
-      </c>
-      <c r="M5" s="1">
-        <v>2</v>
-      </c>
-      <c r="N5" s="1">
-        <v>1</v>
-      </c>
-      <c r="O5" s="1">
-        <v>7</v>
-      </c>
-      <c r="P5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="113">
+        <v>1</v>
+      </c>
+      <c r="M5" s="113">
+        <v>2</v>
+      </c>
+      <c r="N5" s="113">
+        <v>1</v>
+      </c>
+      <c r="O5" s="113">
+        <v>10</v>
+      </c>
+      <c r="P5" s="113">
         <v>8</v>
       </c>
       <c r="Q5" s="4">
         <v>10</v>
       </c>
       <c r="R5" s="34">
-        <f>SUM(K5:Q5)/6</f>
-        <v>5.5</v>
+        <f>(O5+SUM(K5:M5))/4</f>
+        <v>3.5</v>
       </c>
       <c r="S5" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T5" s="1">
         <f>SUM(K5:Q5)</f>
@@ -2252,124 +2270,124 @@
         <v>13</v>
       </c>
       <c r="D6" s="43">
-        <v>23</v>
-      </c>
-      <c r="E6" s="44">
+        <v>21</v>
+      </c>
+      <c r="E6" s="52">
         <v>8</v>
       </c>
       <c r="F6" s="44">
+        <f>SUM(C6:E6)</f>
+        <v>42</v>
+      </c>
+      <c r="G6" s="53">
+        <v>2</v>
+      </c>
+      <c r="H6" s="43">
+        <v>1</v>
+      </c>
+      <c r="I6" s="46">
+        <v>1</v>
+      </c>
+      <c r="J6" s="47">
+        <v>2</v>
+      </c>
+      <c r="K6" s="48">
+        <v>7</v>
+      </c>
+      <c r="L6" s="49">
+        <v>5</v>
+      </c>
+      <c r="M6" s="49">
+        <v>4</v>
+      </c>
+      <c r="N6" s="49">
+        <v>6</v>
+      </c>
+      <c r="O6" s="49">
+        <v>9</v>
+      </c>
+      <c r="P6" s="49">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="50">
+        <v>9</v>
+      </c>
+      <c r="R6" s="51">
+        <f>(O6+SUM(K6:M6))/4</f>
+        <v>6.25</v>
+      </c>
+      <c r="S6" s="50">
+        <v>6</v>
+      </c>
+      <c r="T6" s="1">
+        <f t="shared" ref="T6:T14" si="0">SUM(K6:Q6)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="32">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="113">
+        <v>12</v>
+      </c>
+      <c r="D7" s="113">
+        <v>12</v>
+      </c>
+      <c r="E7" s="29">
+        <v>0</v>
+      </c>
+      <c r="F7" s="29">
+        <f>SUM(C7:E7)</f>
+        <v>24</v>
+      </c>
+      <c r="G7" s="26">
+        <v>2</v>
+      </c>
+      <c r="H7" s="113">
+        <v>2</v>
+      </c>
+      <c r="I7" s="4">
+        <v>4</v>
+      </c>
+      <c r="J7" s="22">
+        <v>2</v>
+      </c>
+      <c r="K7" s="35">
+        <v>8</v>
+      </c>
+      <c r="L7" s="113">
+        <v>7</v>
+      </c>
+      <c r="M7" s="113">
+        <v>10</v>
+      </c>
+      <c r="N7" s="113">
+        <v>9</v>
+      </c>
+      <c r="O7" s="113">
+        <v>7</v>
+      </c>
+      <c r="P7" s="113">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>1</v>
+      </c>
+      <c r="R7" s="34">
+        <f>(O7+SUM(K7:M7))/4</f>
+        <v>8</v>
+      </c>
+      <c r="S7" s="115">
+        <v>9</v>
+      </c>
+      <c r="T7" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="G6" s="45">
-        <v>2</v>
-      </c>
-      <c r="H6" s="43">
-        <v>1</v>
-      </c>
-      <c r="I6" s="46">
-        <v>1</v>
-      </c>
-      <c r="J6" s="47">
-        <v>2</v>
-      </c>
-      <c r="K6" s="48">
-        <v>6</v>
-      </c>
-      <c r="L6" s="49">
-        <v>4</v>
-      </c>
-      <c r="M6" s="49">
-        <v>4</v>
-      </c>
-      <c r="N6" s="49">
-        <v>6</v>
-      </c>
-      <c r="O6" s="49">
-        <v>8</v>
-      </c>
-      <c r="P6" s="49">
-        <v>10</v>
-      </c>
-      <c r="Q6" s="50">
-        <v>9</v>
-      </c>
-      <c r="R6" s="51">
-        <f t="shared" ref="R6:R14" si="1">SUM(K6:Q6)/6</f>
-        <v>7.833333333333333</v>
-      </c>
-      <c r="S6" s="50">
-        <v>9</v>
-      </c>
-      <c r="T6" s="1">
-        <f t="shared" ref="T6:T14" si="2">SUM(K6:Q6)</f>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="32">
-        <v>3</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="1">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1">
-        <v>12</v>
-      </c>
-      <c r="E7" s="29">
-        <v>0</v>
-      </c>
-      <c r="F7" s="29">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="G7" s="26">
-        <v>2</v>
-      </c>
-      <c r="H7" s="1">
-        <v>2</v>
-      </c>
-      <c r="I7" s="4">
-        <v>4</v>
-      </c>
-      <c r="J7" s="22">
-        <v>2</v>
-      </c>
-      <c r="K7" s="35">
-        <v>7</v>
-      </c>
-      <c r="L7" s="1">
-        <v>6</v>
-      </c>
-      <c r="M7" s="1">
-        <v>10</v>
-      </c>
-      <c r="N7" s="1">
-        <v>9</v>
-      </c>
-      <c r="O7" s="1">
-        <v>10</v>
-      </c>
-      <c r="P7" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>1</v>
-      </c>
-      <c r="R7" s="34">
-        <f t="shared" si="1"/>
-        <v>7.5</v>
-      </c>
-      <c r="S7" s="4">
-        <v>8</v>
-      </c>
-      <c r="T7" s="1">
-        <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="41">
@@ -2378,62 +2396,62 @@
       <c r="B8" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="43">
-        <v>4</v>
-      </c>
-      <c r="D8" s="43">
+      <c r="C8" s="114">
+        <v>4</v>
+      </c>
+      <c r="D8" s="114">
         <v>12</v>
       </c>
       <c r="E8" s="44">
         <v>6</v>
       </c>
       <c r="F8" s="44">
+        <f>SUM(C8:E8)</f>
+        <v>22</v>
+      </c>
+      <c r="G8" s="45">
+        <v>8</v>
+      </c>
+      <c r="H8" s="114">
+        <v>3</v>
+      </c>
+      <c r="I8" s="46">
+        <v>2</v>
+      </c>
+      <c r="J8" s="47">
+        <v>2</v>
+      </c>
+      <c r="K8" s="48">
+        <v>9</v>
+      </c>
+      <c r="L8" s="111">
+        <v>6</v>
+      </c>
+      <c r="M8" s="111">
+        <v>5</v>
+      </c>
+      <c r="N8" s="111">
+        <v>10</v>
+      </c>
+      <c r="O8" s="111">
+        <v>1</v>
+      </c>
+      <c r="P8" s="111">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="50">
+        <v>2</v>
+      </c>
+      <c r="R8" s="51">
+        <f>(O8+SUM(K8:M8))/4</f>
+        <v>5.25</v>
+      </c>
+      <c r="S8" s="50">
+        <v>10</v>
+      </c>
+      <c r="T8" s="1">
         <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="G8" s="45">
-        <v>8</v>
-      </c>
-      <c r="H8" s="43">
-        <v>3</v>
-      </c>
-      <c r="I8" s="46">
-        <v>2</v>
-      </c>
-      <c r="J8" s="47">
-        <v>2</v>
-      </c>
-      <c r="K8" s="48">
-        <v>9</v>
-      </c>
-      <c r="L8" s="49">
-        <v>7</v>
-      </c>
-      <c r="M8" s="49">
-        <v>6</v>
-      </c>
-      <c r="N8" s="49">
-        <v>10</v>
-      </c>
-      <c r="O8" s="49">
-        <v>1</v>
-      </c>
-      <c r="P8" s="49">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="50">
-        <v>2</v>
-      </c>
-      <c r="R8" s="51">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="S8" s="50">
-        <v>5</v>
-      </c>
-      <c r="T8" s="1">
-        <f t="shared" si="2"/>
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -2444,61 +2462,61 @@
         <v>31</v>
       </c>
       <c r="C9" s="5">
+        <v>14</v>
+      </c>
+      <c r="D9" s="5">
         <v>12</v>
       </c>
-      <c r="D9" s="5">
-        <v>8</v>
-      </c>
       <c r="E9" s="14">
         <v>8</v>
       </c>
       <c r="F9" s="14">
+        <f>SUM(C9:E9)</f>
+        <v>34</v>
+      </c>
+      <c r="G9" s="6">
+        <v>5</v>
+      </c>
+      <c r="H9" s="5">
+        <v>2</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1</v>
+      </c>
+      <c r="J9" s="21">
+        <v>2</v>
+      </c>
+      <c r="K9" s="35">
+        <v>6</v>
+      </c>
+      <c r="L9" s="1">
+        <v>8</v>
+      </c>
+      <c r="M9" s="1">
+        <v>3</v>
+      </c>
+      <c r="N9" s="1">
+        <v>8</v>
+      </c>
+      <c r="O9" s="1">
+        <v>4</v>
+      </c>
+      <c r="P9" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>7</v>
+      </c>
+      <c r="R9" s="34">
+        <f>(O9+SUM(K9:M9))/4</f>
+        <v>5.25</v>
+      </c>
+      <c r="S9" s="115">
+        <v>7</v>
+      </c>
+      <c r="T9" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="G9" s="6">
-        <v>5</v>
-      </c>
-      <c r="H9" s="5">
-        <v>2</v>
-      </c>
-      <c r="I9" s="7">
-        <v>1</v>
-      </c>
-      <c r="J9" s="21">
-        <v>2</v>
-      </c>
-      <c r="K9" s="35">
-        <v>8</v>
-      </c>
-      <c r="L9" s="1">
-        <v>8</v>
-      </c>
-      <c r="M9" s="1">
-        <v>3</v>
-      </c>
-      <c r="N9" s="1">
-        <v>8</v>
-      </c>
-      <c r="O9" s="1">
-        <v>3</v>
-      </c>
-      <c r="P9" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>7</v>
-      </c>
-      <c r="R9" s="34">
-        <f t="shared" si="1"/>
-        <v>7.166666666666667</v>
-      </c>
-      <c r="S9" s="4">
-        <v>6</v>
-      </c>
-      <c r="T9" s="1">
-        <f t="shared" si="2"/>
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -2508,62 +2526,62 @@
       <c r="B10" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="49">
-        <v>2</v>
-      </c>
-      <c r="D10" s="49">
+      <c r="C10" s="111">
+        <v>2</v>
+      </c>
+      <c r="D10" s="111">
         <v>23</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="56">
         <v>3</v>
       </c>
       <c r="F10" s="44">
+        <f>SUM(C10:E10)</f>
+        <v>28</v>
+      </c>
+      <c r="G10" s="70">
+        <v>2</v>
+      </c>
+      <c r="H10" s="111">
+        <v>2</v>
+      </c>
+      <c r="I10" s="50">
+        <v>2</v>
+      </c>
+      <c r="J10" s="55">
+        <v>2</v>
+      </c>
+      <c r="K10" s="48">
+        <v>10</v>
+      </c>
+      <c r="L10" s="111">
+        <v>4</v>
+      </c>
+      <c r="M10" s="111">
+        <v>9</v>
+      </c>
+      <c r="N10" s="111">
+        <v>7</v>
+      </c>
+      <c r="O10" s="111">
+        <v>8</v>
+      </c>
+      <c r="P10" s="111">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="50">
+        <v>5</v>
+      </c>
+      <c r="R10" s="51">
+        <f>(O10+SUM(K10:M10))/4</f>
+        <v>7.75</v>
+      </c>
+      <c r="S10" s="50">
+        <v>8</v>
+      </c>
+      <c r="T10" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="G10" s="72">
-        <v>2</v>
-      </c>
-      <c r="H10" s="49">
-        <v>2</v>
-      </c>
-      <c r="I10" s="50">
-        <v>2</v>
-      </c>
-      <c r="J10" s="57">
-        <v>2</v>
-      </c>
-      <c r="K10" s="48">
-        <v>10</v>
-      </c>
-      <c r="L10" s="49">
-        <v>5</v>
-      </c>
-      <c r="M10" s="49">
-        <v>9</v>
-      </c>
-      <c r="N10" s="49">
-        <v>7</v>
-      </c>
-      <c r="O10" s="49">
-        <v>9</v>
-      </c>
-      <c r="P10" s="49">
-        <v>5</v>
-      </c>
-      <c r="Q10" s="50">
-        <v>5</v>
-      </c>
-      <c r="R10" s="51">
-        <f t="shared" si="1"/>
-        <v>8.3333333333333339</v>
-      </c>
-      <c r="S10" s="50">
-        <v>10</v>
-      </c>
-      <c r="T10" s="1">
-        <f t="shared" si="2"/>
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -2573,62 +2591,62 @@
       <c r="B11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="113">
         <v>38</v>
       </c>
-      <c r="D11" s="1">
-        <v>6</v>
-      </c>
-      <c r="E11" s="15">
+      <c r="D11" s="113">
+        <v>6</v>
+      </c>
+      <c r="E11" s="25">
         <v>5</v>
       </c>
       <c r="F11" s="14">
+        <f>SUM(C11:E11)</f>
+        <v>49</v>
+      </c>
+      <c r="G11" s="26">
+        <v>6</v>
+      </c>
+      <c r="H11" s="113">
+        <v>2</v>
+      </c>
+      <c r="I11" s="4">
+        <v>2</v>
+      </c>
+      <c r="J11" s="22">
+        <v>2</v>
+      </c>
+      <c r="K11" s="35">
+        <v>2</v>
+      </c>
+      <c r="L11" s="113">
+        <v>10</v>
+      </c>
+      <c r="M11" s="113">
+        <v>6</v>
+      </c>
+      <c r="N11" s="113">
+        <v>4</v>
+      </c>
+      <c r="O11" s="113">
+        <v>2</v>
+      </c>
+      <c r="P11" s="113">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>4</v>
+      </c>
+      <c r="R11" s="34">
+        <f>(O11+SUM(K11:M11))/4</f>
+        <v>5</v>
+      </c>
+      <c r="S11" s="115">
+        <v>4</v>
+      </c>
+      <c r="T11" s="1">
         <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="G11" s="13">
-        <v>6</v>
-      </c>
-      <c r="H11" s="1">
-        <v>2</v>
-      </c>
-      <c r="I11" s="4">
-        <v>2</v>
-      </c>
-      <c r="J11" s="22">
-        <v>2</v>
-      </c>
-      <c r="K11" s="35">
-        <v>1</v>
-      </c>
-      <c r="L11" s="1">
-        <v>9</v>
-      </c>
-      <c r="M11" s="1">
-        <v>7</v>
-      </c>
-      <c r="N11" s="1">
-        <v>4</v>
-      </c>
-      <c r="O11" s="1">
-        <v>2</v>
-      </c>
-      <c r="P11" s="1">
-        <v>4</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>4</v>
-      </c>
-      <c r="R11" s="34">
-        <f t="shared" si="1"/>
-        <v>5.166666666666667</v>
-      </c>
-      <c r="S11" s="4">
-        <v>2</v>
-      </c>
-      <c r="T11" s="1">
-        <f t="shared" si="2"/>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -2644,55 +2662,55 @@
       <c r="D12" s="43">
         <v>6</v>
       </c>
-      <c r="E12" s="58">
-        <v>7</v>
+      <c r="E12" s="56">
+        <v>4</v>
       </c>
       <c r="F12" s="44">
+        <f>SUM(C12:E12)</f>
+        <v>42</v>
+      </c>
+      <c r="G12" s="57">
+        <v>5</v>
+      </c>
+      <c r="H12" s="43">
+        <v>1</v>
+      </c>
+      <c r="I12" s="46">
+        <v>2</v>
+      </c>
+      <c r="J12" s="58">
+        <v>2</v>
+      </c>
+      <c r="K12" s="48">
+        <v>4</v>
+      </c>
+      <c r="L12" s="49">
+        <v>9</v>
+      </c>
+      <c r="M12" s="49">
+        <v>7</v>
+      </c>
+      <c r="N12" s="49">
+        <v>5</v>
+      </c>
+      <c r="O12" s="49">
+        <v>3</v>
+      </c>
+      <c r="P12" s="49">
+        <v>9</v>
+      </c>
+      <c r="Q12" s="50">
+        <v>6</v>
+      </c>
+      <c r="R12" s="51">
+        <f>(O12+SUM(K12:M12))/4</f>
+        <v>5.75</v>
+      </c>
+      <c r="S12" s="50">
+        <v>5</v>
+      </c>
+      <c r="T12" s="1">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="G12" s="59">
-        <v>5</v>
-      </c>
-      <c r="H12" s="43">
-        <v>1</v>
-      </c>
-      <c r="I12" s="46">
-        <v>2</v>
-      </c>
-      <c r="J12" s="60">
-        <v>2</v>
-      </c>
-      <c r="K12" s="48">
-        <v>4</v>
-      </c>
-      <c r="L12" s="49">
-        <v>10</v>
-      </c>
-      <c r="M12" s="49">
-        <v>5</v>
-      </c>
-      <c r="N12" s="49">
-        <v>5</v>
-      </c>
-      <c r="O12" s="49">
-        <v>4</v>
-      </c>
-      <c r="P12" s="49">
-        <v>9</v>
-      </c>
-      <c r="Q12" s="50">
-        <v>6</v>
-      </c>
-      <c r="R12" s="51">
-        <f t="shared" si="1"/>
-        <v>7.166666666666667</v>
-      </c>
-      <c r="S12" s="50">
-        <v>7</v>
-      </c>
-      <c r="T12" s="1">
-        <f t="shared" si="2"/>
         <v>43</v>
       </c>
     </row>
@@ -2704,156 +2722,156 @@
         <v>35</v>
       </c>
       <c r="C13" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1">
         <v>24</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="15">
         <v>30</v>
       </c>
       <c r="F13" s="29">
+        <f>SUM(C13:E13)</f>
+        <v>68</v>
+      </c>
+      <c r="G13" s="13">
+        <v>3</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2</v>
+      </c>
+      <c r="I13" s="7">
+        <v>2</v>
+      </c>
+      <c r="J13" s="22">
+        <v>2</v>
+      </c>
+      <c r="K13" s="35">
+        <v>5</v>
+      </c>
+      <c r="L13" s="1">
+        <v>3</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>2</v>
+      </c>
+      <c r="O13" s="1">
+        <v>6</v>
+      </c>
+      <c r="P13" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>3</v>
+      </c>
+      <c r="R13" s="34">
+        <f>(O13+SUM(K13:M13))/4</f>
+        <v>3.75</v>
+      </c>
+      <c r="S13" s="115">
+        <v>2</v>
+      </c>
+      <c r="T13" s="1">
         <f t="shared" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="G13" s="26">
-        <v>3</v>
-      </c>
-      <c r="H13" s="1">
-        <v>2</v>
-      </c>
-      <c r="I13" s="7">
-        <v>2</v>
-      </c>
-      <c r="J13" s="22">
-        <v>2</v>
-      </c>
-      <c r="K13" s="35">
-        <v>5</v>
-      </c>
-      <c r="L13" s="1">
-        <v>3</v>
-      </c>
-      <c r="M13" s="1">
-        <v>1</v>
-      </c>
-      <c r="N13" s="1">
-        <v>2</v>
-      </c>
-      <c r="O13" s="1">
-        <v>6</v>
-      </c>
-      <c r="P13" s="1">
-        <v>3</v>
-      </c>
-      <c r="Q13" s="4">
-        <v>3</v>
-      </c>
-      <c r="R13" s="34">
-        <f t="shared" si="1"/>
-        <v>3.8333333333333335</v>
-      </c>
-      <c r="S13" s="4">
-        <v>1</v>
-      </c>
-      <c r="T13" s="1">
-        <f t="shared" si="2"/>
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="61">
-        <v>10</v>
-      </c>
-      <c r="B14" s="62" t="s">
+      <c r="A14" s="59">
+        <v>10</v>
+      </c>
+      <c r="B14" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="63">
+      <c r="C14" s="61">
         <v>34</v>
       </c>
-      <c r="D14" s="63">
+      <c r="D14" s="61">
         <v>28</v>
       </c>
-      <c r="E14" s="64">
-        <v>4</v>
-      </c>
-      <c r="F14" s="65">
+      <c r="E14" s="62">
+        <v>4</v>
+      </c>
+      <c r="F14" s="63">
+        <f>SUM(C14:E14)</f>
+        <v>66</v>
+      </c>
+      <c r="G14" s="64">
+        <v>4</v>
+      </c>
+      <c r="H14" s="61">
+        <v>2</v>
+      </c>
+      <c r="I14" s="65">
+        <v>1</v>
+      </c>
+      <c r="J14" s="66">
+        <v>3</v>
+      </c>
+      <c r="K14" s="67">
+        <v>3</v>
+      </c>
+      <c r="L14" s="61">
+        <v>2</v>
+      </c>
+      <c r="M14" s="61">
+        <v>8</v>
+      </c>
+      <c r="N14" s="61">
+        <v>3</v>
+      </c>
+      <c r="O14" s="61">
+        <v>5</v>
+      </c>
+      <c r="P14" s="61">
+        <v>7</v>
+      </c>
+      <c r="Q14" s="65">
+        <v>8</v>
+      </c>
+      <c r="R14" s="71">
+        <f>(O14+SUM(K14:M14))/4</f>
+        <v>4.5</v>
+      </c>
+      <c r="S14" s="69">
+        <v>3</v>
+      </c>
+      <c r="T14" s="1">
         <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="G14" s="66">
-        <v>4</v>
-      </c>
-      <c r="H14" s="63">
-        <v>2</v>
-      </c>
-      <c r="I14" s="67">
-        <v>1</v>
-      </c>
-      <c r="J14" s="68">
-        <v>3</v>
-      </c>
-      <c r="K14" s="69">
-        <v>2</v>
-      </c>
-      <c r="L14" s="63">
-        <v>1</v>
-      </c>
-      <c r="M14" s="63">
-        <v>8</v>
-      </c>
-      <c r="N14" s="63">
-        <v>3</v>
-      </c>
-      <c r="O14" s="63">
-        <v>5</v>
-      </c>
-      <c r="P14" s="63">
-        <v>7</v>
-      </c>
-      <c r="Q14" s="67">
-        <v>8</v>
-      </c>
-      <c r="R14" s="74">
-        <f t="shared" si="1"/>
-        <v>5.666666666666667</v>
-      </c>
-      <c r="S14" s="71">
-        <v>4</v>
-      </c>
-      <c r="T14" s="1">
-        <f t="shared" si="2"/>
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:I15" si="3">SUM(C5:C14)</f>
-        <v>194</v>
+        <f>SUM(C5:C14)</f>
+        <v>207</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="3"/>
-        <v>166</v>
+        <f t="shared" ref="D15:I15" si="1">SUM(D5:D14)</f>
+        <v>176</v>
       </c>
       <c r="E15" s="16">
-        <f t="shared" si="3"/>
-        <v>86</v>
+        <f t="shared" si="1"/>
+        <v>83</v>
       </c>
       <c r="F15" s="16">
         <f>SUM(F5:F14)</f>
-        <v>446</v>
+        <v>466</v>
       </c>
       <c r="G15" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="J15" s="23"/>
@@ -2863,9 +2881,9 @@
         <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2874,9 +2892,9 @@
         <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2885,9 +2903,9 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2896,9 +2914,9 @@
         <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2909,7 +2927,7 @@
       <c r="C23" t="s">
         <v>54</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2920,7 +2938,7 @@
       <c r="C24" t="s">
         <v>30</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2929,6 +2947,29 @@
         <v>67</v>
       </c>
     </row>
+    <row r="29" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C29" s="107" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="108"/>
+      <c r="E29" s="108"/>
+      <c r="F29" s="108"/>
+      <c r="G29" s="108"/>
+      <c r="H29" s="108"/>
+      <c r="I29" s="109"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="107" t="s">
+        <v>38</v>
+      </c>
+      <c r="L29" s="108"/>
+      <c r="M29" s="108"/>
+      <c r="N29" s="108"/>
+      <c r="O29" s="108"/>
+      <c r="P29" s="108"/>
+      <c r="Q29" s="108"/>
+      <c r="R29" s="108"/>
+      <c r="S29" s="109"/>
+    </row>
     <row r="30" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
         <v>49</v>
@@ -2981,37 +3022,36 @@
       <c r="Q30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="R30" s="3" t="s">
-        <v>50</v>
+      <c r="R30" s="33" t="s">
+        <v>94</v>
       </c>
       <c r="S30" s="19" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="32">
+      <c r="A31" s="112">
         <v>1</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="1">
-        <v>34</v>
-      </c>
-      <c r="D31" s="1">
-        <v>24</v>
+      <c r="C31" s="113">
+        <v>44</v>
+      </c>
+      <c r="D31" s="113">
+        <v>32</v>
       </c>
       <c r="E31" s="29">
         <v>15</v>
       </c>
       <c r="F31" s="29">
-        <f t="shared" ref="F31:F40" si="4">SUM(C31:E31)</f>
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="G31" s="26">
         <v>2</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31" s="113">
         <v>2</v>
       </c>
       <c r="I31" s="7">
@@ -3021,32 +3061,32 @@
         <v>3</v>
       </c>
       <c r="K31" s="36">
-        <v>3</v>
-      </c>
-      <c r="L31" s="1">
-        <v>2</v>
-      </c>
-      <c r="M31" s="1">
-        <v>2</v>
-      </c>
-      <c r="N31" s="1">
-        <v>1</v>
-      </c>
-      <c r="O31" s="1">
-        <v>7</v>
-      </c>
-      <c r="P31" s="1">
+        <v>1</v>
+      </c>
+      <c r="L31" s="113">
+        <v>1</v>
+      </c>
+      <c r="M31" s="113">
+        <v>2</v>
+      </c>
+      <c r="N31" s="113">
+        <v>1</v>
+      </c>
+      <c r="O31" s="113">
+        <v>10</v>
+      </c>
+      <c r="P31" s="113">
         <v>8</v>
       </c>
       <c r="Q31" s="4">
         <v>10</v>
       </c>
       <c r="R31" s="34">
-        <f t="shared" ref="R31:R40" si="5">(O31+SUM(K31:M31))/4</f>
+        <f>(O31+SUM(K31:M31))/4</f>
         <v>3.5</v>
       </c>
       <c r="S31" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -3060,14 +3100,13 @@
         <v>13</v>
       </c>
       <c r="D32" s="43">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E32" s="52">
         <v>8</v>
       </c>
       <c r="F32" s="52">
-        <f t="shared" si="4"/>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G32" s="53">
         <v>2</v>
@@ -3082,10 +3121,10 @@
         <v>2</v>
       </c>
       <c r="K32" s="48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L32" s="49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M32" s="49">
         <v>4</v>
@@ -3094,7 +3133,7 @@
         <v>6</v>
       </c>
       <c r="O32" s="49">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P32" s="49">
         <v>10</v>
@@ -3103,37 +3142,36 @@
         <v>9</v>
       </c>
       <c r="R32" s="51">
-        <f t="shared" si="5"/>
-        <v>5.5</v>
+        <f>(O32+SUM(K32:M32))/4</f>
+        <v>6.25</v>
       </c>
       <c r="S32" s="50">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="32">
+      <c r="A33" s="112">
         <v>3</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="113">
         <v>12</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="113">
         <v>12</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="29">
         <v>0</v>
       </c>
-      <c r="F33" s="14">
-        <f t="shared" si="4"/>
+      <c r="F33" s="29">
         <v>24</v>
       </c>
-      <c r="G33" s="13">
-        <v>2</v>
-      </c>
-      <c r="H33" s="1">
+      <c r="G33" s="26">
+        <v>2</v>
+      </c>
+      <c r="H33" s="113">
         <v>2</v>
       </c>
       <c r="I33" s="4">
@@ -3143,58 +3181,57 @@
         <v>2</v>
       </c>
       <c r="K33" s="35">
-        <v>7</v>
-      </c>
-      <c r="L33" s="1">
-        <v>6</v>
-      </c>
-      <c r="M33" s="1">
-        <v>10</v>
-      </c>
-      <c r="N33" s="1">
-        <v>9</v>
-      </c>
-      <c r="O33" s="1">
-        <v>10</v>
-      </c>
-      <c r="P33" s="1">
+        <v>8</v>
+      </c>
+      <c r="L33" s="113">
+        <v>7</v>
+      </c>
+      <c r="M33" s="113">
+        <v>10</v>
+      </c>
+      <c r="N33" s="113">
+        <v>9</v>
+      </c>
+      <c r="O33" s="113">
+        <v>7</v>
+      </c>
+      <c r="P33" s="113">
         <v>2</v>
       </c>
       <c r="Q33" s="4">
         <v>1</v>
       </c>
       <c r="R33" s="34">
-        <f t="shared" si="5"/>
-        <v>8.25</v>
-      </c>
-      <c r="S33" s="4">
-        <v>1</v>
+        <f>(O33+SUM(K33:M33))/4</f>
+        <v>8</v>
+      </c>
+      <c r="S33" s="115">
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="41">
+      <c r="A34" s="110">
         <v>4</v>
       </c>
       <c r="B34" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="43">
-        <v>4</v>
-      </c>
-      <c r="D34" s="43">
+      <c r="C34" s="114">
+        <v>4</v>
+      </c>
+      <c r="D34" s="114">
         <v>12</v>
       </c>
-      <c r="E34" s="52">
-        <v>6</v>
-      </c>
-      <c r="F34" s="52">
-        <f t="shared" si="4"/>
+      <c r="E34" s="44">
+        <v>6</v>
+      </c>
+      <c r="F34" s="44">
         <v>22</v>
       </c>
-      <c r="G34" s="53">
-        <v>8</v>
-      </c>
-      <c r="H34" s="43">
+      <c r="G34" s="45">
+        <v>8</v>
+      </c>
+      <c r="H34" s="114">
         <v>3</v>
       </c>
       <c r="I34" s="46">
@@ -3206,30 +3243,30 @@
       <c r="K34" s="48">
         <v>9</v>
       </c>
-      <c r="L34" s="49">
-        <v>7</v>
-      </c>
-      <c r="M34" s="49">
-        <v>6</v>
-      </c>
-      <c r="N34" s="49">
-        <v>10</v>
-      </c>
-      <c r="O34" s="49">
-        <v>1</v>
-      </c>
-      <c r="P34" s="49">
+      <c r="L34" s="111">
+        <v>6</v>
+      </c>
+      <c r="M34" s="111">
+        <v>5</v>
+      </c>
+      <c r="N34" s="111">
+        <v>10</v>
+      </c>
+      <c r="O34" s="111">
+        <v>1</v>
+      </c>
+      <c r="P34" s="111">
         <v>1</v>
       </c>
       <c r="Q34" s="50">
         <v>2</v>
       </c>
       <c r="R34" s="51">
-        <f t="shared" si="5"/>
-        <v>5.75</v>
+        <f>(O34+SUM(K34:M34))/4</f>
+        <v>5.25</v>
       </c>
       <c r="S34" s="50">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -3240,17 +3277,16 @@
         <v>31</v>
       </c>
       <c r="C35" s="5">
+        <v>14</v>
+      </c>
+      <c r="D35" s="5">
         <v>12</v>
       </c>
-      <c r="D35" s="5">
-        <v>8</v>
-      </c>
       <c r="E35" s="14">
         <v>8</v>
       </c>
       <c r="F35" s="14">
-        <f t="shared" si="4"/>
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G35" s="6">
         <v>5</v>
@@ -3265,7 +3301,7 @@
         <v>2</v>
       </c>
       <c r="K35" s="35">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L35" s="1">
         <v>8</v>
@@ -3277,7 +3313,7 @@
         <v>8</v>
       </c>
       <c r="O35" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P35" s="1">
         <v>6</v>
@@ -3286,98 +3322,96 @@
         <v>7</v>
       </c>
       <c r="R35" s="34">
-        <f t="shared" si="5"/>
-        <v>5.5</v>
-      </c>
-      <c r="S35" s="4">
-        <v>6</v>
+        <f>(O35+SUM(K35:M35))/4</f>
+        <v>5.25</v>
+      </c>
+      <c r="S35" s="115">
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="41">
+      <c r="A36" s="110">
         <v>6</v>
       </c>
       <c r="B36" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="49">
-        <v>2</v>
-      </c>
-      <c r="D36" s="49">
+      <c r="C36" s="111">
+        <v>2</v>
+      </c>
+      <c r="D36" s="111">
         <v>23</v>
       </c>
-      <c r="E36" s="55">
-        <v>3</v>
-      </c>
-      <c r="F36" s="52">
-        <f t="shared" si="4"/>
+      <c r="E36" s="56">
+        <v>3</v>
+      </c>
+      <c r="F36" s="44">
         <v>28</v>
       </c>
-      <c r="G36" s="56">
-        <v>2</v>
-      </c>
-      <c r="H36" s="49">
+      <c r="G36" s="70">
+        <v>2</v>
+      </c>
+      <c r="H36" s="111">
         <v>2</v>
       </c>
       <c r="I36" s="50">
         <v>2</v>
       </c>
-      <c r="J36" s="57">
+      <c r="J36" s="55">
         <v>2</v>
       </c>
       <c r="K36" s="48">
         <v>10</v>
       </c>
-      <c r="L36" s="49">
-        <v>5</v>
-      </c>
-      <c r="M36" s="49">
-        <v>9</v>
-      </c>
-      <c r="N36" s="49">
-        <v>7</v>
-      </c>
-      <c r="O36" s="49">
-        <v>9</v>
-      </c>
-      <c r="P36" s="49">
+      <c r="L36" s="111">
+        <v>4</v>
+      </c>
+      <c r="M36" s="111">
+        <v>9</v>
+      </c>
+      <c r="N36" s="111">
+        <v>7</v>
+      </c>
+      <c r="O36" s="111">
+        <v>8</v>
+      </c>
+      <c r="P36" s="111">
         <v>5</v>
       </c>
       <c r="Q36" s="50">
         <v>5</v>
       </c>
       <c r="R36" s="51">
-        <f t="shared" si="5"/>
-        <v>8.25</v>
+        <f>(O36+SUM(K36:M36))/4</f>
+        <v>7.75</v>
       </c>
       <c r="S36" s="50">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="32">
+      <c r="A37" s="112">
         <v>7</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="113">
         <v>38</v>
       </c>
-      <c r="D37" s="1">
-        <v>6</v>
-      </c>
-      <c r="E37" s="15">
-        <v>5</v>
-      </c>
-      <c r="F37" s="14">
-        <f t="shared" si="4"/>
+      <c r="D37" s="113">
+        <v>6</v>
+      </c>
+      <c r="E37" s="25">
+        <v>5</v>
+      </c>
+      <c r="F37" s="29">
         <v>49</v>
       </c>
-      <c r="G37" s="13">
-        <v>6</v>
-      </c>
-      <c r="H37" s="1">
+      <c r="G37" s="26">
+        <v>6</v>
+      </c>
+      <c r="H37" s="113">
         <v>2</v>
       </c>
       <c r="I37" s="4">
@@ -3387,32 +3421,32 @@
         <v>2</v>
       </c>
       <c r="K37" s="35">
-        <v>1</v>
-      </c>
-      <c r="L37" s="1">
-        <v>9</v>
-      </c>
-      <c r="M37" s="1">
-        <v>7</v>
-      </c>
-      <c r="N37" s="1">
-        <v>4</v>
-      </c>
-      <c r="O37" s="1">
-        <v>2</v>
-      </c>
-      <c r="P37" s="1">
+        <v>2</v>
+      </c>
+      <c r="L37" s="113">
+        <v>10</v>
+      </c>
+      <c r="M37" s="113">
+        <v>6</v>
+      </c>
+      <c r="N37" s="113">
+        <v>4</v>
+      </c>
+      <c r="O37" s="113">
+        <v>2</v>
+      </c>
+      <c r="P37" s="113">
         <v>4</v>
       </c>
       <c r="Q37" s="4">
         <v>4</v>
       </c>
       <c r="R37" s="34">
-        <f t="shared" si="5"/>
-        <v>4.75</v>
-      </c>
-      <c r="S37" s="4">
-        <v>7</v>
+        <f>(O37+SUM(K37:M37))/4</f>
+        <v>5</v>
+      </c>
+      <c r="S37" s="115">
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -3428,14 +3462,13 @@
       <c r="D38" s="43">
         <v>6</v>
       </c>
-      <c r="E38" s="55">
-        <v>7</v>
-      </c>
-      <c r="F38" s="52">
-        <f t="shared" si="4"/>
-        <v>45</v>
-      </c>
-      <c r="G38" s="73">
+      <c r="E38" s="56">
+        <v>4</v>
+      </c>
+      <c r="F38" s="44">
+        <v>42</v>
+      </c>
+      <c r="G38" s="57">
         <v>5</v>
       </c>
       <c r="H38" s="43">
@@ -3444,23 +3477,23 @@
       <c r="I38" s="46">
         <v>2</v>
       </c>
-      <c r="J38" s="60">
+      <c r="J38" s="58">
         <v>2</v>
       </c>
       <c r="K38" s="48">
         <v>4</v>
       </c>
       <c r="L38" s="49">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M38" s="49">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N38" s="49">
         <v>5</v>
       </c>
       <c r="O38" s="49">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P38" s="49">
         <v>9</v>
@@ -3469,11 +3502,11 @@
         <v>6</v>
       </c>
       <c r="R38" s="51">
-        <f t="shared" si="5"/>
+        <f>(O38+SUM(K38:M38))/4</f>
         <v>5.75</v>
       </c>
       <c r="S38" s="50">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -3484,7 +3517,7 @@
         <v>35</v>
       </c>
       <c r="C39" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D39" s="1">
         <v>24</v>
@@ -3493,8 +3526,7 @@
         <v>30</v>
       </c>
       <c r="F39" s="14">
-        <f t="shared" si="4"/>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G39" s="13">
         <v>3</v>
@@ -3530,81 +3562,115 @@
         <v>3</v>
       </c>
       <c r="R39" s="34">
-        <f t="shared" si="5"/>
+        <f>(O39+SUM(K39:M39))/4</f>
         <v>3.75</v>
       </c>
-      <c r="S39" s="4">
-        <v>9</v>
+      <c r="S39" s="115">
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="61">
-        <v>10</v>
-      </c>
-      <c r="B40" s="62" t="s">
+      <c r="A40" s="59">
+        <v>10</v>
+      </c>
+      <c r="B40" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="63">
+      <c r="C40" s="61">
         <v>34</v>
       </c>
-      <c r="D40" s="63">
+      <c r="D40" s="61">
         <v>28</v>
       </c>
-      <c r="E40" s="64">
-        <v>4</v>
-      </c>
-      <c r="F40" s="65">
-        <f t="shared" si="4"/>
+      <c r="E40" s="62">
+        <v>4</v>
+      </c>
+      <c r="F40" s="63">
         <v>66</v>
       </c>
-      <c r="G40" s="66">
-        <v>4</v>
-      </c>
-      <c r="H40" s="63">
-        <v>2</v>
-      </c>
-      <c r="I40" s="67">
-        <v>1</v>
-      </c>
-      <c r="J40" s="68">
-        <v>3</v>
-      </c>
-      <c r="K40" s="69">
-        <v>2</v>
-      </c>
-      <c r="L40" s="63">
-        <v>1</v>
-      </c>
-      <c r="M40" s="63">
-        <v>8</v>
-      </c>
-      <c r="N40" s="63">
-        <v>3</v>
-      </c>
-      <c r="O40" s="63">
-        <v>5</v>
-      </c>
-      <c r="P40" s="63">
-        <v>7</v>
-      </c>
-      <c r="Q40" s="67">
-        <v>8</v>
-      </c>
-      <c r="R40" s="74">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="S40" s="71">
-        <v>8</v>
-      </c>
+      <c r="G40" s="64">
+        <v>4</v>
+      </c>
+      <c r="H40" s="61">
+        <v>2</v>
+      </c>
+      <c r="I40" s="65">
+        <v>1</v>
+      </c>
+      <c r="J40" s="66">
+        <v>3</v>
+      </c>
+      <c r="K40" s="67">
+        <v>3</v>
+      </c>
+      <c r="L40" s="61">
+        <v>2</v>
+      </c>
+      <c r="M40" s="61">
+        <v>8</v>
+      </c>
+      <c r="N40" s="61">
+        <v>3</v>
+      </c>
+      <c r="O40" s="61">
+        <v>5</v>
+      </c>
+      <c r="P40" s="61">
+        <v>7</v>
+      </c>
+      <c r="Q40" s="65">
+        <v>8</v>
+      </c>
+      <c r="R40" s="71">
+        <f>(O40+SUM(K40:M40))/4</f>
+        <v>4.5</v>
+      </c>
+      <c r="S40" s="69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F42" s="116"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F43" s="116"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F44" s="116"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F45" s="116"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F46" s="116"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F47" s="116"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F48" s="116"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="116"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="116"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="116"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="116"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A31:S40">
     <sortCondition ref="A31:A40"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C3:I3"/>
     <mergeCell ref="K3:S3"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="K29:S29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3634,27 +3700,27 @@
   <sheetData>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="92" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="94"/>
+      <c r="C3" s="107" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="109"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="92" t="s">
+      <c r="K3" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="93"/>
-      <c r="S3" s="94"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="108"/>
+      <c r="R3" s="108"/>
+      <c r="S3" s="109"/>
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
@@ -3794,7 +3860,7 @@
       <c r="C6" s="43">
         <v>8</v>
       </c>
-      <c r="D6" s="82">
+      <c r="D6" s="79">
         <v>21</v>
       </c>
       <c r="E6" s="44">
@@ -3838,7 +3904,7 @@
         <v>8</v>
       </c>
       <c r="R6" s="51">
-        <f t="shared" ref="R5:R14" si="0">SUM(K6:Q6)/6</f>
+        <f t="shared" ref="R6:R14" si="0">SUM(K6:Q6)/6</f>
         <v>8.1666666666666661</v>
       </c>
       <c r="S6" s="50">
@@ -3924,7 +3990,7 @@
       <c r="C8" s="43">
         <v>4</v>
       </c>
-      <c r="D8" s="82">
+      <c r="D8" s="79">
         <v>12</v>
       </c>
       <c r="E8" s="44">
@@ -3934,7 +4000,7 @@
         <f>SUM(C8:E8)</f>
         <v>19</v>
       </c>
-      <c r="G8" s="75">
+      <c r="G8" s="72">
         <v>8</v>
       </c>
       <c r="H8" s="43">
@@ -3999,7 +4065,7 @@
         <f t="shared" ref="F9:F14" si="2">SUM(C9:E9)</f>
         <v>28</v>
       </c>
-      <c r="G9" s="76">
+      <c r="G9" s="73">
         <v>5</v>
       </c>
       <c r="H9" s="5">
@@ -4057,14 +4123,14 @@
       <c r="D10" s="41">
         <v>23</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="56">
         <v>3</v>
       </c>
       <c r="F10" s="44">
         <f>SUM(C10:E10)</f>
         <v>28</v>
       </c>
-      <c r="G10" s="77">
+      <c r="G10" s="74">
         <v>1</v>
       </c>
       <c r="H10" s="49">
@@ -4073,7 +4139,7 @@
       <c r="I10" s="50">
         <v>2</v>
       </c>
-      <c r="J10" s="57">
+      <c r="J10" s="55">
         <v>2</v>
       </c>
       <c r="K10" s="48">
@@ -4129,7 +4195,7 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="G11" s="78">
+      <c r="G11" s="75">
         <v>6</v>
       </c>
       <c r="H11" s="1">
@@ -4184,17 +4250,17 @@
       <c r="C12" s="43">
         <v>28</v>
       </c>
-      <c r="D12" s="82">
-        <v>6</v>
-      </c>
-      <c r="E12" s="58">
+      <c r="D12" s="79">
+        <v>6</v>
+      </c>
+      <c r="E12" s="56">
         <v>4</v>
       </c>
       <c r="F12" s="44">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="G12" s="79">
+      <c r="G12" s="76">
         <v>4</v>
       </c>
       <c r="H12" s="43">
@@ -4203,7 +4269,7 @@
       <c r="I12" s="46">
         <v>2</v>
       </c>
-      <c r="J12" s="60">
+      <c r="J12" s="58">
         <v>2</v>
       </c>
       <c r="K12" s="48">
@@ -4259,7 +4325,7 @@
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="G13" s="80">
+      <c r="G13" s="77">
         <v>3</v>
       </c>
       <c r="H13" s="1">
@@ -4305,63 +4371,63 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="61">
-        <v>10</v>
-      </c>
-      <c r="B14" s="62" t="s">
+      <c r="A14" s="59">
+        <v>10</v>
+      </c>
+      <c r="B14" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="63">
+      <c r="C14" s="61">
         <v>16</v>
       </c>
-      <c r="D14" s="83">
+      <c r="D14" s="80">
         <v>39</v>
       </c>
-      <c r="E14" s="64">
-        <v>9</v>
-      </c>
-      <c r="F14" s="65">
+      <c r="E14" s="62">
+        <v>9</v>
+      </c>
+      <c r="F14" s="63">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="G14" s="81">
-        <v>4</v>
-      </c>
-      <c r="H14" s="63">
-        <v>2</v>
-      </c>
-      <c r="I14" s="67">
-        <v>1</v>
-      </c>
-      <c r="J14" s="68">
-        <v>3</v>
-      </c>
-      <c r="K14" s="69">
-        <v>4</v>
-      </c>
-      <c r="L14" s="63">
-        <v>1</v>
-      </c>
-      <c r="M14" s="63">
-        <v>3</v>
-      </c>
-      <c r="N14" s="63">
-        <v>2</v>
-      </c>
-      <c r="O14" s="63">
-        <v>5</v>
-      </c>
-      <c r="P14" s="63">
-        <v>3</v>
-      </c>
-      <c r="Q14" s="67">
-        <v>6</v>
-      </c>
-      <c r="R14" s="74">
+      <c r="G14" s="78">
+        <v>4</v>
+      </c>
+      <c r="H14" s="61">
+        <v>2</v>
+      </c>
+      <c r="I14" s="65">
+        <v>1</v>
+      </c>
+      <c r="J14" s="66">
+        <v>3</v>
+      </c>
+      <c r="K14" s="67">
+        <v>4</v>
+      </c>
+      <c r="L14" s="61">
+        <v>1</v>
+      </c>
+      <c r="M14" s="61">
+        <v>3</v>
+      </c>
+      <c r="N14" s="61">
+        <v>2</v>
+      </c>
+      <c r="O14" s="61">
+        <v>5</v>
+      </c>
+      <c r="P14" s="61">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="65">
+        <v>6</v>
+      </c>
+      <c r="R14" s="71">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="S14" s="71">
+      <c r="S14" s="69">
         <v>2</v>
       </c>
       <c r="T14" s="1">
@@ -4567,7 +4633,7 @@
       <c r="H28" s="32">
         <v>2</v>
       </c>
-      <c r="I28" s="87">
+      <c r="I28" s="84">
         <v>0</v>
       </c>
       <c r="J28" s="20">
@@ -4612,7 +4678,7 @@
       <c r="C29" s="43">
         <v>8</v>
       </c>
-      <c r="D29" s="82">
+      <c r="D29" s="79">
         <v>21</v>
       </c>
       <c r="E29" s="44">
@@ -4621,13 +4687,13 @@
       <c r="F29" s="44">
         <v>37</v>
       </c>
-      <c r="G29" s="82">
-        <v>1</v>
-      </c>
-      <c r="H29" s="82">
-        <v>1</v>
-      </c>
-      <c r="I29" s="84">
+      <c r="G29" s="79">
+        <v>1</v>
+      </c>
+      <c r="H29" s="79">
+        <v>1</v>
+      </c>
+      <c r="I29" s="81">
         <v>1</v>
       </c>
       <c r="J29" s="47">
@@ -4687,7 +4753,7 @@
       <c r="H30" s="32">
         <v>2</v>
       </c>
-      <c r="I30" s="86">
+      <c r="I30" s="83">
         <v>4</v>
       </c>
       <c r="J30" s="22">
@@ -4732,7 +4798,7 @@
       <c r="C31" s="43">
         <v>4</v>
       </c>
-      <c r="D31" s="82">
+      <c r="D31" s="79">
         <v>12</v>
       </c>
       <c r="E31" s="44">
@@ -4741,13 +4807,13 @@
       <c r="F31" s="44">
         <v>19</v>
       </c>
-      <c r="G31" s="58">
-        <v>8</v>
-      </c>
-      <c r="H31" s="82">
-        <v>1</v>
-      </c>
-      <c r="I31" s="84">
+      <c r="G31" s="56">
+        <v>8</v>
+      </c>
+      <c r="H31" s="79">
+        <v>1</v>
+      </c>
+      <c r="I31" s="81">
         <v>2</v>
       </c>
       <c r="J31" s="47">
@@ -4807,7 +4873,7 @@
       <c r="H32" s="16">
         <v>2</v>
       </c>
-      <c r="I32" s="87">
+      <c r="I32" s="84">
         <v>1</v>
       </c>
       <c r="J32" s="21">
@@ -4855,22 +4921,22 @@
       <c r="D33" s="41">
         <v>23</v>
       </c>
-      <c r="E33" s="58">
+      <c r="E33" s="56">
         <v>3</v>
       </c>
       <c r="F33" s="44">
         <v>28</v>
       </c>
-      <c r="G33" s="88">
+      <c r="G33" s="85">
         <v>1</v>
       </c>
       <c r="H33" s="41">
         <v>1</v>
       </c>
-      <c r="I33" s="89">
-        <v>2</v>
-      </c>
-      <c r="J33" s="57">
+      <c r="I33" s="86">
+        <v>2</v>
+      </c>
+      <c r="J33" s="55">
         <v>2</v>
       </c>
       <c r="K33" s="48">
@@ -4921,13 +4987,13 @@
       <c r="F34" s="14">
         <v>44</v>
       </c>
-      <c r="G34" s="85">
+      <c r="G34" s="82">
         <v>6</v>
       </c>
       <c r="H34" s="32">
         <v>2</v>
       </c>
-      <c r="I34" s="86">
+      <c r="I34" s="83">
         <v>2</v>
       </c>
       <c r="J34" s="22">
@@ -4972,10 +5038,10 @@
       <c r="C35" s="43">
         <v>28</v>
       </c>
-      <c r="D35" s="82">
-        <v>6</v>
-      </c>
-      <c r="E35" s="58">
+      <c r="D35" s="79">
+        <v>6</v>
+      </c>
+      <c r="E35" s="56">
         <v>4</v>
       </c>
       <c r="F35" s="44">
@@ -4984,13 +5050,13 @@
       <c r="G35" s="44">
         <v>4</v>
       </c>
-      <c r="H35" s="82">
-        <v>1</v>
-      </c>
-      <c r="I35" s="84">
-        <v>2</v>
-      </c>
-      <c r="J35" s="60">
+      <c r="H35" s="79">
+        <v>1</v>
+      </c>
+      <c r="I35" s="81">
+        <v>2</v>
+      </c>
+      <c r="J35" s="58">
         <v>2</v>
       </c>
       <c r="K35" s="48">
@@ -5041,13 +5107,13 @@
       <c r="F36" s="29">
         <v>60</v>
       </c>
-      <c r="G36" s="90">
+      <c r="G36" s="87">
         <v>3</v>
       </c>
       <c r="H36" s="32">
         <v>2</v>
       </c>
-      <c r="I36" s="87">
+      <c r="I36" s="84">
         <v>0</v>
       </c>
       <c r="J36" s="22">
@@ -5083,62 +5149,62 @@
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="61">
-        <v>10</v>
-      </c>
-      <c r="B37" s="62" t="s">
+      <c r="A37" s="59">
+        <v>10</v>
+      </c>
+      <c r="B37" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="63">
+      <c r="C37" s="61">
         <v>16</v>
       </c>
-      <c r="D37" s="83">
+      <c r="D37" s="80">
         <v>39</v>
       </c>
-      <c r="E37" s="64">
-        <v>9</v>
-      </c>
-      <c r="F37" s="65">
+      <c r="E37" s="62">
+        <v>9</v>
+      </c>
+      <c r="F37" s="63">
         <v>64</v>
       </c>
-      <c r="G37" s="91">
-        <v>4</v>
-      </c>
-      <c r="H37" s="83">
-        <v>2</v>
-      </c>
-      <c r="I37" s="61">
-        <v>1</v>
-      </c>
-      <c r="J37" s="68">
-        <v>3</v>
-      </c>
-      <c r="K37" s="69">
-        <v>4</v>
-      </c>
-      <c r="L37" s="63">
-        <v>1</v>
-      </c>
-      <c r="M37" s="63">
-        <v>3</v>
-      </c>
-      <c r="N37" s="63">
-        <v>2</v>
-      </c>
-      <c r="O37" s="63">
-        <v>5</v>
-      </c>
-      <c r="P37" s="63">
-        <v>3</v>
-      </c>
-      <c r="Q37" s="67">
-        <v>6</v>
-      </c>
-      <c r="R37" s="74">
+      <c r="G37" s="88">
+        <v>4</v>
+      </c>
+      <c r="H37" s="80">
+        <v>2</v>
+      </c>
+      <c r="I37" s="59">
+        <v>1</v>
+      </c>
+      <c r="J37" s="66">
+        <v>3</v>
+      </c>
+      <c r="K37" s="67">
+        <v>4</v>
+      </c>
+      <c r="L37" s="61">
+        <v>1</v>
+      </c>
+      <c r="M37" s="61">
+        <v>3</v>
+      </c>
+      <c r="N37" s="61">
+        <v>2</v>
+      </c>
+      <c r="O37" s="61">
+        <v>5</v>
+      </c>
+      <c r="P37" s="61">
+        <v>3</v>
+      </c>
+      <c r="Q37" s="65">
+        <v>6</v>
+      </c>
+      <c r="R37" s="71">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="S37" s="71">
+      <c r="S37" s="69">
         <v>2</v>
       </c>
     </row>
@@ -5164,7 +5230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5E5147-5992-4431-822F-ABC86F78CFE9}">
   <dimension ref="A3:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -5180,27 +5246,27 @@
   <sheetData>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="92" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="94"/>
+      <c r="C3" s="107" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="109"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="92" t="s">
+      <c r="K3" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="93"/>
-      <c r="S3" s="94"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="108"/>
+      <c r="R3" s="108"/>
+      <c r="S3" s="109"/>
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
@@ -5297,7 +5363,7 @@
       <c r="J5" s="20">
         <v>3</v>
       </c>
-      <c r="K5" s="103">
+      <c r="K5" s="96">
         <v>1</v>
       </c>
       <c r="L5" s="32">
@@ -5315,13 +5381,13 @@
       <c r="P5" s="32">
         <v>6</v>
       </c>
-      <c r="Q5" s="86">
+      <c r="Q5" s="83">
         <v>9</v>
       </c>
       <c r="R5" s="34">
         <v>4.833333333333333</v>
       </c>
-      <c r="S5" s="86">
+      <c r="S5" s="83">
         <v>1</v>
       </c>
       <c r="T5" s="32">
@@ -5339,7 +5405,7 @@
       <c r="C6" s="43">
         <v>10</v>
       </c>
-      <c r="D6" s="82">
+      <c r="D6" s="79">
         <v>21</v>
       </c>
       <c r="E6" s="44">
@@ -5361,31 +5427,31 @@
       <c r="J6" s="47">
         <v>1</v>
       </c>
-      <c r="K6" s="105">
-        <v>8</v>
-      </c>
-      <c r="L6" s="95">
-        <v>4</v>
-      </c>
-      <c r="M6" s="95">
-        <v>5</v>
-      </c>
-      <c r="N6" s="95">
-        <v>6</v>
-      </c>
-      <c r="O6" s="95">
-        <v>10</v>
-      </c>
-      <c r="P6" s="95">
-        <v>10</v>
-      </c>
-      <c r="Q6" s="89">
+      <c r="K6" s="98">
+        <v>8</v>
+      </c>
+      <c r="L6" s="41">
+        <v>4</v>
+      </c>
+      <c r="M6" s="41">
+        <v>5</v>
+      </c>
+      <c r="N6" s="41">
+        <v>6</v>
+      </c>
+      <c r="O6" s="41">
+        <v>10</v>
+      </c>
+      <c r="P6" s="41">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="86">
         <v>8</v>
       </c>
       <c r="R6" s="51">
         <v>8.5</v>
       </c>
-      <c r="S6" s="89">
+      <c r="S6" s="86">
         <v>6</v>
       </c>
       <c r="T6" s="1">
@@ -5425,31 +5491,31 @@
       <c r="J7" s="22">
         <v>2</v>
       </c>
-      <c r="K7" s="107">
-        <v>7</v>
-      </c>
-      <c r="L7" s="114">
-        <v>7</v>
-      </c>
-      <c r="M7" s="114">
-        <v>10</v>
-      </c>
-      <c r="N7" s="114">
-        <v>9</v>
-      </c>
-      <c r="O7" s="114">
-        <v>7</v>
-      </c>
-      <c r="P7" s="114">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="86">
+      <c r="K7" s="100">
+        <v>7</v>
+      </c>
+      <c r="L7" s="32">
+        <v>7</v>
+      </c>
+      <c r="M7" s="32">
+        <v>10</v>
+      </c>
+      <c r="N7" s="32">
+        <v>9</v>
+      </c>
+      <c r="O7" s="32">
+        <v>7</v>
+      </c>
+      <c r="P7" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="83">
         <v>1</v>
       </c>
       <c r="R7" s="34">
         <v>7</v>
       </c>
-      <c r="S7" s="86">
+      <c r="S7" s="83">
         <v>9</v>
       </c>
       <c r="T7" s="1">
@@ -5467,7 +5533,7 @@
       <c r="C8" s="43">
         <v>4</v>
       </c>
-      <c r="D8" s="82">
+      <c r="D8" s="79">
         <v>12</v>
       </c>
       <c r="E8" s="44">
@@ -5477,7 +5543,7 @@
         <f>SUM(C8:E8)</f>
         <v>19</v>
       </c>
-      <c r="G8" s="75">
+      <c r="G8" s="72">
         <v>8</v>
       </c>
       <c r="H8" s="43">
@@ -5489,31 +5555,31 @@
       <c r="J8" s="47">
         <v>2</v>
       </c>
-      <c r="K8" s="105">
-        <v>9</v>
-      </c>
-      <c r="L8" s="95">
-        <v>8</v>
-      </c>
-      <c r="M8" s="95">
-        <v>8</v>
-      </c>
-      <c r="N8" s="95">
-        <v>10</v>
-      </c>
-      <c r="O8" s="95">
-        <v>1</v>
-      </c>
-      <c r="P8" s="95">
-        <v>8</v>
-      </c>
-      <c r="Q8" s="89">
+      <c r="K8" s="98">
+        <v>9</v>
+      </c>
+      <c r="L8" s="41">
+        <v>8</v>
+      </c>
+      <c r="M8" s="41">
+        <v>8</v>
+      </c>
+      <c r="N8" s="41">
+        <v>10</v>
+      </c>
+      <c r="O8" s="41">
+        <v>1</v>
+      </c>
+      <c r="P8" s="41">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="86">
         <v>4</v>
       </c>
       <c r="R8" s="51">
         <v>8</v>
       </c>
-      <c r="S8" s="89">
+      <c r="S8" s="86">
         <v>10</v>
       </c>
       <c r="T8" s="1">
@@ -5541,7 +5607,7 @@
         <f t="shared" ref="F9:F14" si="1">SUM(C9:E9)</f>
         <v>36</v>
       </c>
-      <c r="G9" s="76">
+      <c r="G9" s="73">
         <v>5</v>
       </c>
       <c r="H9" s="5">
@@ -5553,7 +5619,7 @@
       <c r="J9" s="21">
         <v>2</v>
       </c>
-      <c r="K9" s="107">
+      <c r="K9" s="100">
         <v>5</v>
       </c>
       <c r="L9" s="32">
@@ -5571,13 +5637,13 @@
       <c r="P9" s="32">
         <v>4</v>
       </c>
-      <c r="Q9" s="86">
+      <c r="Q9" s="83">
         <v>6</v>
       </c>
       <c r="R9" s="34">
         <v>6</v>
       </c>
-      <c r="S9" s="115">
+      <c r="S9" s="106">
         <v>7</v>
       </c>
       <c r="T9" s="1">
@@ -5598,14 +5664,14 @@
       <c r="D10" s="41">
         <v>23</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="56">
         <v>3</v>
       </c>
       <c r="F10" s="44">
         <f>SUM(C10:E10)</f>
         <v>28</v>
       </c>
-      <c r="G10" s="77">
+      <c r="G10" s="74">
         <v>2</v>
       </c>
       <c r="H10" s="49">
@@ -5614,34 +5680,34 @@
       <c r="I10" s="50">
         <v>2</v>
       </c>
-      <c r="J10" s="57">
-        <v>2</v>
-      </c>
-      <c r="K10" s="105">
-        <v>10</v>
-      </c>
-      <c r="L10" s="95">
-        <v>3</v>
-      </c>
-      <c r="M10" s="95">
-        <v>9</v>
-      </c>
-      <c r="N10" s="95">
-        <v>8</v>
-      </c>
-      <c r="O10" s="95">
-        <v>8</v>
-      </c>
-      <c r="P10" s="95">
-        <v>2</v>
-      </c>
-      <c r="Q10" s="89">
+      <c r="J10" s="55">
+        <v>2</v>
+      </c>
+      <c r="K10" s="98">
+        <v>10</v>
+      </c>
+      <c r="L10" s="41">
+        <v>3</v>
+      </c>
+      <c r="M10" s="41">
+        <v>9</v>
+      </c>
+      <c r="N10" s="41">
+        <v>8</v>
+      </c>
+      <c r="O10" s="41">
+        <v>8</v>
+      </c>
+      <c r="P10" s="41">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="86">
         <v>2</v>
       </c>
       <c r="R10" s="51">
         <v>7</v>
       </c>
-      <c r="S10" s="89">
+      <c r="S10" s="86">
         <v>8</v>
       </c>
       <c r="T10" s="1">
@@ -5669,7 +5735,7 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="G11" s="78">
+      <c r="G11" s="75">
         <v>6</v>
       </c>
       <c r="H11" s="1">
@@ -5681,7 +5747,7 @@
       <c r="J11" s="22">
         <v>2</v>
       </c>
-      <c r="K11" s="107">
+      <c r="K11" s="100">
         <v>2</v>
       </c>
       <c r="L11" s="32">
@@ -5699,13 +5765,13 @@
       <c r="P11" s="32">
         <v>3</v>
       </c>
-      <c r="Q11" s="86">
+      <c r="Q11" s="83">
         <v>3</v>
       </c>
       <c r="R11" s="34">
         <v>4.833333333333333</v>
       </c>
-      <c r="S11" s="86">
+      <c r="S11" s="83">
         <v>4</v>
       </c>
       <c r="T11" s="1">
@@ -5723,17 +5789,17 @@
       <c r="C12" s="43">
         <v>30</v>
       </c>
-      <c r="D12" s="82">
-        <v>6</v>
-      </c>
-      <c r="E12" s="58">
+      <c r="D12" s="79">
+        <v>6</v>
+      </c>
+      <c r="E12" s="56">
         <v>4</v>
       </c>
       <c r="F12" s="44">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="G12" s="79">
+      <c r="G12" s="76">
         <v>5</v>
       </c>
       <c r="H12" s="43">
@@ -5742,34 +5808,34 @@
       <c r="I12" s="46">
         <v>2</v>
       </c>
-      <c r="J12" s="60">
-        <v>2</v>
-      </c>
-      <c r="K12" s="105">
-        <v>4</v>
-      </c>
-      <c r="L12" s="95">
-        <v>10</v>
-      </c>
-      <c r="M12" s="95">
-        <v>7</v>
-      </c>
-      <c r="N12" s="95">
-        <v>5</v>
-      </c>
-      <c r="O12" s="95">
-        <v>3</v>
-      </c>
-      <c r="P12" s="95">
-        <v>9</v>
-      </c>
-      <c r="Q12" s="89">
+      <c r="J12" s="58">
+        <v>2</v>
+      </c>
+      <c r="K12" s="98">
+        <v>4</v>
+      </c>
+      <c r="L12" s="41">
+        <v>10</v>
+      </c>
+      <c r="M12" s="41">
+        <v>7</v>
+      </c>
+      <c r="N12" s="41">
+        <v>5</v>
+      </c>
+      <c r="O12" s="41">
+        <v>3</v>
+      </c>
+      <c r="P12" s="41">
+        <v>9</v>
+      </c>
+      <c r="Q12" s="86">
         <v>5</v>
       </c>
       <c r="R12" s="51">
         <v>7.166666666666667</v>
       </c>
-      <c r="S12" s="89">
+      <c r="S12" s="86">
         <v>5</v>
       </c>
       <c r="T12" s="1">
@@ -5797,7 +5863,7 @@
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="G13" s="80">
+      <c r="G13" s="77">
         <v>4</v>
       </c>
       <c r="H13" s="1">
@@ -5809,31 +5875,31 @@
       <c r="J13" s="22">
         <v>2</v>
       </c>
-      <c r="K13" s="107">
-        <v>6</v>
-      </c>
-      <c r="L13" s="114">
-        <v>5</v>
-      </c>
-      <c r="M13" s="114">
-        <v>1</v>
-      </c>
-      <c r="N13" s="114">
-        <v>3</v>
-      </c>
-      <c r="O13" s="114">
-        <v>6</v>
-      </c>
-      <c r="P13" s="114">
-        <v>7</v>
-      </c>
-      <c r="Q13" s="86">
+      <c r="K13" s="100">
+        <v>6</v>
+      </c>
+      <c r="L13" s="32">
+        <v>5</v>
+      </c>
+      <c r="M13" s="32">
+        <v>1</v>
+      </c>
+      <c r="N13" s="32">
+        <v>3</v>
+      </c>
+      <c r="O13" s="32">
+        <v>6</v>
+      </c>
+      <c r="P13" s="32">
+        <v>7</v>
+      </c>
+      <c r="Q13" s="83">
         <v>10</v>
       </c>
       <c r="R13" s="34">
         <v>6.333333333333333</v>
       </c>
-      <c r="S13" s="86">
+      <c r="S13" s="83">
         <v>3</v>
       </c>
       <c r="T13" s="1">
@@ -5842,62 +5908,62 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="61">
-        <v>10</v>
-      </c>
-      <c r="B14" s="62" t="s">
+      <c r="A14" s="59">
+        <v>10</v>
+      </c>
+      <c r="B14" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="63">
+      <c r="C14" s="61">
         <v>34</v>
       </c>
-      <c r="D14" s="83">
+      <c r="D14" s="80">
         <v>23</v>
       </c>
-      <c r="E14" s="64">
-        <v>9</v>
-      </c>
-      <c r="F14" s="65">
+      <c r="E14" s="62">
+        <v>9</v>
+      </c>
+      <c r="F14" s="63">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
-      <c r="G14" s="81">
-        <v>4</v>
-      </c>
-      <c r="H14" s="63">
-        <v>2</v>
-      </c>
-      <c r="I14" s="67">
-        <v>1</v>
-      </c>
-      <c r="J14" s="68">
-        <v>3</v>
-      </c>
-      <c r="K14" s="109">
-        <v>3</v>
-      </c>
-      <c r="L14" s="83">
-        <v>2</v>
-      </c>
-      <c r="M14" s="83">
-        <v>3</v>
-      </c>
-      <c r="N14" s="83">
-        <v>2</v>
-      </c>
-      <c r="O14" s="83">
-        <v>5</v>
-      </c>
-      <c r="P14" s="83">
-        <v>5</v>
-      </c>
-      <c r="Q14" s="61">
-        <v>7</v>
-      </c>
-      <c r="R14" s="74">
+      <c r="G14" s="78">
+        <v>4</v>
+      </c>
+      <c r="H14" s="61">
+        <v>2</v>
+      </c>
+      <c r="I14" s="65">
+        <v>1</v>
+      </c>
+      <c r="J14" s="66">
+        <v>3</v>
+      </c>
+      <c r="K14" s="102">
+        <v>3</v>
+      </c>
+      <c r="L14" s="80">
+        <v>2</v>
+      </c>
+      <c r="M14" s="80">
+        <v>3</v>
+      </c>
+      <c r="N14" s="80">
+        <v>2</v>
+      </c>
+      <c r="O14" s="80">
+        <v>5</v>
+      </c>
+      <c r="P14" s="80">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="59">
+        <v>7</v>
+      </c>
+      <c r="R14" s="71">
         <v>4.5</v>
       </c>
-      <c r="S14" s="110">
+      <c r="S14" s="103">
         <v>2</v>
       </c>
       <c r="T14" s="1">
@@ -6020,61 +6086,61 @@
       </c>
     </row>
     <row r="30" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="96" t="s">
+      <c r="A30" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="97" t="s">
+      <c r="B30" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="98" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="98" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="99" t="s">
-        <v>1</v>
-      </c>
-      <c r="F30" s="99" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="98" t="s">
-        <v>4</v>
-      </c>
-      <c r="H30" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="I30" s="100" t="s">
-        <v>7</v>
-      </c>
-      <c r="J30" s="101" t="s">
+      <c r="C30" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="92" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="92" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="91" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="93" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="K30" s="102" t="s">
+      <c r="K30" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="L30" s="98" t="s">
-        <v>2</v>
-      </c>
-      <c r="M30" s="98" t="s">
-        <v>1</v>
-      </c>
-      <c r="N30" s="98" t="s">
-        <v>10</v>
-      </c>
-      <c r="O30" s="98" t="s">
-        <v>4</v>
-      </c>
-      <c r="P30" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q30" s="100" t="s">
-        <v>7</v>
-      </c>
-      <c r="R30" s="100" t="s">
+      <c r="L30" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="M30" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="N30" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="O30" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="P30" s="91" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q30" s="93" t="s">
+        <v>7</v>
+      </c>
+      <c r="R30" s="93" t="s">
         <v>50</v>
       </c>
-      <c r="S30" s="101" t="s">
+      <c r="S30" s="94" t="s">
         <v>51</v>
       </c>
     </row>
@@ -6103,13 +6169,13 @@
       <c r="H31" s="32">
         <v>2</v>
       </c>
-      <c r="I31" s="87">
+      <c r="I31" s="84">
         <v>0</v>
       </c>
       <c r="J31" s="20">
         <v>3</v>
       </c>
-      <c r="K31" s="103">
+      <c r="K31" s="96">
         <v>1</v>
       </c>
       <c r="L31" s="32">
@@ -6127,28 +6193,28 @@
       <c r="P31" s="32">
         <v>6</v>
       </c>
-      <c r="Q31" s="86">
+      <c r="Q31" s="83">
         <v>9</v>
       </c>
       <c r="R31" s="34">
-        <f>SUM(K31:Q31)/6</f>
+        <f t="shared" ref="R31:R40" si="3">SUM(K31:Q31)/6</f>
         <v>4.833333333333333</v>
       </c>
-      <c r="S31" s="86">
+      <c r="S31" s="83">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="95">
-        <v>2</v>
-      </c>
-      <c r="B32" s="106" t="s">
+      <c r="A32" s="41">
+        <v>2</v>
+      </c>
+      <c r="B32" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="113">
-        <v>10</v>
-      </c>
-      <c r="D32" s="113">
+      <c r="C32" s="79">
+        <v>10</v>
+      </c>
+      <c r="D32" s="79">
         <v>21</v>
       </c>
       <c r="E32" s="44">
@@ -6157,58 +6223,58 @@
       <c r="F32" s="44">
         <v>39</v>
       </c>
-      <c r="G32" s="113">
-        <v>1</v>
-      </c>
-      <c r="H32" s="113">
-        <v>1</v>
-      </c>
-      <c r="I32" s="84">
+      <c r="G32" s="79">
+        <v>1</v>
+      </c>
+      <c r="H32" s="79">
+        <v>1</v>
+      </c>
+      <c r="I32" s="81">
         <v>1</v>
       </c>
       <c r="J32" s="47">
         <v>1</v>
       </c>
-      <c r="K32" s="105">
-        <v>8</v>
-      </c>
-      <c r="L32" s="95">
-        <v>4</v>
-      </c>
-      <c r="M32" s="95">
-        <v>5</v>
-      </c>
-      <c r="N32" s="95">
-        <v>6</v>
-      </c>
-      <c r="O32" s="95">
-        <v>10</v>
-      </c>
-      <c r="P32" s="95">
-        <v>10</v>
-      </c>
-      <c r="Q32" s="89">
+      <c r="K32" s="98">
+        <v>8</v>
+      </c>
+      <c r="L32" s="41">
+        <v>4</v>
+      </c>
+      <c r="M32" s="41">
+        <v>5</v>
+      </c>
+      <c r="N32" s="41">
+        <v>6</v>
+      </c>
+      <c r="O32" s="41">
+        <v>10</v>
+      </c>
+      <c r="P32" s="41">
+        <v>10</v>
+      </c>
+      <c r="Q32" s="86">
         <v>8</v>
       </c>
       <c r="R32" s="51">
-        <f>SUM(K32:Q32)/6</f>
+        <f t="shared" si="3"/>
         <v>8.5</v>
       </c>
-      <c r="S32" s="89">
+      <c r="S32" s="86">
         <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="114">
+      <c r="A33" s="32">
         <v>3</v>
       </c>
       <c r="B33" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="114">
+      <c r="C33" s="32">
         <v>12</v>
       </c>
-      <c r="D33" s="114">
+      <c r="D33" s="32">
         <v>12</v>
       </c>
       <c r="E33" s="29">
@@ -6217,58 +6283,58 @@
       <c r="F33" s="29">
         <v>24</v>
       </c>
-      <c r="G33" s="114">
-        <v>2</v>
-      </c>
-      <c r="H33" s="114">
-        <v>2</v>
-      </c>
-      <c r="I33" s="86">
+      <c r="G33" s="32">
+        <v>2</v>
+      </c>
+      <c r="H33" s="32">
+        <v>2</v>
+      </c>
+      <c r="I33" s="83">
         <v>4</v>
       </c>
       <c r="J33" s="22">
         <v>2</v>
       </c>
-      <c r="K33" s="107">
-        <v>7</v>
-      </c>
-      <c r="L33" s="114">
-        <v>7</v>
-      </c>
-      <c r="M33" s="114">
-        <v>10</v>
-      </c>
-      <c r="N33" s="114">
-        <v>9</v>
-      </c>
-      <c r="O33" s="114">
-        <v>7</v>
-      </c>
-      <c r="P33" s="114">
-        <v>1</v>
-      </c>
-      <c r="Q33" s="86">
+      <c r="K33" s="100">
+        <v>7</v>
+      </c>
+      <c r="L33" s="32">
+        <v>7</v>
+      </c>
+      <c r="M33" s="32">
+        <v>10</v>
+      </c>
+      <c r="N33" s="32">
+        <v>9</v>
+      </c>
+      <c r="O33" s="32">
+        <v>7</v>
+      </c>
+      <c r="P33" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="83">
         <v>1</v>
       </c>
       <c r="R33" s="34">
-        <f>SUM(K33:Q33)/6</f>
-        <v>7</v>
-      </c>
-      <c r="S33" s="86">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="S33" s="83">
         <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="95">
-        <v>4</v>
-      </c>
-      <c r="B34" s="106" t="s">
+      <c r="A34" s="41">
+        <v>4</v>
+      </c>
+      <c r="B34" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="113">
-        <v>4</v>
-      </c>
-      <c r="D34" s="113">
+      <c r="C34" s="79">
+        <v>4</v>
+      </c>
+      <c r="D34" s="79">
         <v>12</v>
       </c>
       <c r="E34" s="44">
@@ -6277,44 +6343,44 @@
       <c r="F34" s="44">
         <v>19</v>
       </c>
-      <c r="G34" s="58">
-        <v>8</v>
-      </c>
-      <c r="H34" s="113">
-        <v>1</v>
-      </c>
-      <c r="I34" s="84">
+      <c r="G34" s="56">
+        <v>8</v>
+      </c>
+      <c r="H34" s="79">
+        <v>1</v>
+      </c>
+      <c r="I34" s="81">
         <v>2</v>
       </c>
       <c r="J34" s="47">
         <v>2</v>
       </c>
-      <c r="K34" s="105">
-        <v>9</v>
-      </c>
-      <c r="L34" s="95">
-        <v>8</v>
-      </c>
-      <c r="M34" s="95">
-        <v>8</v>
-      </c>
-      <c r="N34" s="95">
-        <v>10</v>
-      </c>
-      <c r="O34" s="95">
-        <v>1</v>
-      </c>
-      <c r="P34" s="95">
-        <v>8</v>
-      </c>
-      <c r="Q34" s="89">
+      <c r="K34" s="98">
+        <v>9</v>
+      </c>
+      <c r="L34" s="41">
+        <v>8</v>
+      </c>
+      <c r="M34" s="41">
+        <v>8</v>
+      </c>
+      <c r="N34" s="41">
+        <v>10</v>
+      </c>
+      <c r="O34" s="41">
+        <v>1</v>
+      </c>
+      <c r="P34" s="41">
+        <v>8</v>
+      </c>
+      <c r="Q34" s="86">
         <v>4</v>
       </c>
       <c r="R34" s="51">
-        <f>SUM(K34:Q34)/6</f>
-        <v>8</v>
-      </c>
-      <c r="S34" s="89">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="S34" s="86">
         <v>10</v>
       </c>
     </row>
@@ -6322,7 +6388,7 @@
       <c r="A35" s="32">
         <v>5</v>
       </c>
-      <c r="B35" s="108" t="s">
+      <c r="B35" s="101" t="s">
         <v>79</v>
       </c>
       <c r="C35" s="16">
@@ -6343,13 +6409,13 @@
       <c r="H35" s="16">
         <v>2</v>
       </c>
-      <c r="I35" s="87">
+      <c r="I35" s="84">
         <v>1</v>
       </c>
       <c r="J35" s="21">
         <v>2</v>
       </c>
-      <c r="K35" s="107">
+      <c r="K35" s="100">
         <v>5</v>
       </c>
       <c r="L35" s="32">
@@ -6367,74 +6433,74 @@
       <c r="P35" s="32">
         <v>4</v>
       </c>
-      <c r="Q35" s="86">
+      <c r="Q35" s="83">
         <v>6</v>
       </c>
       <c r="R35" s="34">
-        <f>SUM(K35:Q35)/6</f>
-        <v>6</v>
-      </c>
-      <c r="S35" s="115">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="S35" s="106">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="95">
-        <v>6</v>
-      </c>
-      <c r="B36" s="104" t="s">
+      <c r="A36" s="41">
+        <v>6</v>
+      </c>
+      <c r="B36" s="97" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="95">
-        <v>2</v>
-      </c>
-      <c r="D36" s="95">
+      <c r="C36" s="41">
+        <v>2</v>
+      </c>
+      <c r="D36" s="41">
         <v>23</v>
       </c>
-      <c r="E36" s="58">
+      <c r="E36" s="56">
         <v>3</v>
       </c>
       <c r="F36" s="44">
         <v>28</v>
       </c>
-      <c r="G36" s="88">
-        <v>2</v>
-      </c>
-      <c r="H36" s="95">
-        <v>2</v>
-      </c>
-      <c r="I36" s="89">
-        <v>2</v>
-      </c>
-      <c r="J36" s="57">
-        <v>2</v>
-      </c>
-      <c r="K36" s="105">
-        <v>10</v>
-      </c>
-      <c r="L36" s="95">
-        <v>3</v>
-      </c>
-      <c r="M36" s="95">
-        <v>9</v>
-      </c>
-      <c r="N36" s="95">
-        <v>8</v>
-      </c>
-      <c r="O36" s="95">
-        <v>8</v>
-      </c>
-      <c r="P36" s="95">
-        <v>2</v>
-      </c>
-      <c r="Q36" s="89">
+      <c r="G36" s="85">
+        <v>2</v>
+      </c>
+      <c r="H36" s="41">
+        <v>2</v>
+      </c>
+      <c r="I36" s="86">
+        <v>2</v>
+      </c>
+      <c r="J36" s="55">
+        <v>2</v>
+      </c>
+      <c r="K36" s="98">
+        <v>10</v>
+      </c>
+      <c r="L36" s="41">
+        <v>3</v>
+      </c>
+      <c r="M36" s="41">
+        <v>9</v>
+      </c>
+      <c r="N36" s="41">
+        <v>8</v>
+      </c>
+      <c r="O36" s="41">
+        <v>8</v>
+      </c>
+      <c r="P36" s="41">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="86">
         <v>2</v>
       </c>
       <c r="R36" s="51">
-        <f>SUM(K36:Q36)/6</f>
-        <v>7</v>
-      </c>
-      <c r="S36" s="89">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="S36" s="86">
         <v>8</v>
       </c>
     </row>
@@ -6457,19 +6523,19 @@
       <c r="F37" s="14">
         <v>49</v>
       </c>
-      <c r="G37" s="85">
+      <c r="G37" s="82">
         <v>6</v>
       </c>
       <c r="H37" s="32">
         <v>2</v>
       </c>
-      <c r="I37" s="86">
+      <c r="I37" s="83">
         <v>2</v>
       </c>
       <c r="J37" s="22">
         <v>2</v>
       </c>
-      <c r="K37" s="107">
+      <c r="K37" s="100">
         <v>2</v>
       </c>
       <c r="L37" s="32">
@@ -6487,31 +6553,31 @@
       <c r="P37" s="32">
         <v>3</v>
       </c>
-      <c r="Q37" s="86">
+      <c r="Q37" s="83">
         <v>3</v>
       </c>
       <c r="R37" s="34">
-        <f>SUM(K37:Q37)/6</f>
+        <f t="shared" si="3"/>
         <v>4.833333333333333</v>
       </c>
-      <c r="S37" s="86">
+      <c r="S37" s="83">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="95">
-        <v>8</v>
-      </c>
-      <c r="B38" s="106" t="s">
+      <c r="A38" s="41">
+        <v>8</v>
+      </c>
+      <c r="B38" s="99" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="113">
+      <c r="C38" s="79">
         <v>30</v>
       </c>
-      <c r="D38" s="113">
-        <v>6</v>
-      </c>
-      <c r="E38" s="58">
+      <c r="D38" s="79">
+        <v>6</v>
+      </c>
+      <c r="E38" s="56">
         <v>4</v>
       </c>
       <c r="F38" s="44">
@@ -6520,55 +6586,55 @@
       <c r="G38" s="44">
         <v>5</v>
       </c>
-      <c r="H38" s="113">
-        <v>1</v>
-      </c>
-      <c r="I38" s="84">
-        <v>2</v>
-      </c>
-      <c r="J38" s="60">
-        <v>2</v>
-      </c>
-      <c r="K38" s="105">
-        <v>4</v>
-      </c>
-      <c r="L38" s="95">
-        <v>10</v>
-      </c>
-      <c r="M38" s="95">
-        <v>7</v>
-      </c>
-      <c r="N38" s="95">
-        <v>5</v>
-      </c>
-      <c r="O38" s="95">
-        <v>3</v>
-      </c>
-      <c r="P38" s="95">
-        <v>9</v>
-      </c>
-      <c r="Q38" s="89">
+      <c r="H38" s="79">
+        <v>1</v>
+      </c>
+      <c r="I38" s="81">
+        <v>2</v>
+      </c>
+      <c r="J38" s="58">
+        <v>2</v>
+      </c>
+      <c r="K38" s="98">
+        <v>4</v>
+      </c>
+      <c r="L38" s="41">
+        <v>10</v>
+      </c>
+      <c r="M38" s="41">
+        <v>7</v>
+      </c>
+      <c r="N38" s="41">
+        <v>5</v>
+      </c>
+      <c r="O38" s="41">
+        <v>3</v>
+      </c>
+      <c r="P38" s="41">
+        <v>9</v>
+      </c>
+      <c r="Q38" s="86">
         <v>5</v>
       </c>
       <c r="R38" s="51">
-        <f>SUM(K38:Q38)/6</f>
+        <f t="shared" si="3"/>
         <v>7.166666666666667</v>
       </c>
-      <c r="S38" s="89">
+      <c r="S38" s="86">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="114">
+      <c r="A39" s="32">
         <v>9</v>
       </c>
       <c r="B39" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="114">
+      <c r="C39" s="32">
         <v>12</v>
       </c>
-      <c r="D39" s="114">
+      <c r="D39" s="32">
         <v>20</v>
       </c>
       <c r="E39" s="25">
@@ -6577,113 +6643,113 @@
       <c r="F39" s="29">
         <v>62</v>
       </c>
-      <c r="G39" s="90">
-        <v>4</v>
-      </c>
-      <c r="H39" s="114">
-        <v>2</v>
-      </c>
-      <c r="I39" s="87">
+      <c r="G39" s="87">
+        <v>4</v>
+      </c>
+      <c r="H39" s="32">
+        <v>2</v>
+      </c>
+      <c r="I39" s="84">
         <v>0</v>
       </c>
       <c r="J39" s="22">
         <v>2</v>
       </c>
-      <c r="K39" s="107">
-        <v>6</v>
-      </c>
-      <c r="L39" s="114">
-        <v>5</v>
-      </c>
-      <c r="M39" s="114">
-        <v>1</v>
-      </c>
-      <c r="N39" s="114">
-        <v>3</v>
-      </c>
-      <c r="O39" s="114">
-        <v>6</v>
-      </c>
-      <c r="P39" s="114">
-        <v>7</v>
-      </c>
-      <c r="Q39" s="86">
+      <c r="K39" s="100">
+        <v>6</v>
+      </c>
+      <c r="L39" s="32">
+        <v>5</v>
+      </c>
+      <c r="M39" s="32">
+        <v>1</v>
+      </c>
+      <c r="N39" s="32">
+        <v>3</v>
+      </c>
+      <c r="O39" s="32">
+        <v>6</v>
+      </c>
+      <c r="P39" s="32">
+        <v>7</v>
+      </c>
+      <c r="Q39" s="83">
         <v>10</v>
       </c>
       <c r="R39" s="34">
-        <f>SUM(K39:Q39)/6</f>
+        <f t="shared" si="3"/>
         <v>6.333333333333333</v>
       </c>
-      <c r="S39" s="86">
+      <c r="S39" s="83">
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="61">
-        <v>10</v>
-      </c>
-      <c r="B40" s="112" t="s">
+      <c r="A40" s="59">
+        <v>10</v>
+      </c>
+      <c r="B40" s="105" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="83">
+      <c r="C40" s="80">
         <v>34</v>
       </c>
-      <c r="D40" s="83">
+      <c r="D40" s="80">
         <v>23</v>
       </c>
-      <c r="E40" s="64">
-        <v>9</v>
-      </c>
-      <c r="F40" s="65">
+      <c r="E40" s="62">
+        <v>9</v>
+      </c>
+      <c r="F40" s="63">
         <v>66</v>
       </c>
-      <c r="G40" s="91">
-        <v>4</v>
-      </c>
-      <c r="H40" s="83">
-        <v>2</v>
-      </c>
-      <c r="I40" s="61">
-        <v>1</v>
-      </c>
-      <c r="J40" s="68">
-        <v>3</v>
-      </c>
-      <c r="K40" s="109">
-        <v>3</v>
-      </c>
-      <c r="L40" s="83">
-        <v>2</v>
-      </c>
-      <c r="M40" s="83">
-        <v>3</v>
-      </c>
-      <c r="N40" s="83">
-        <v>2</v>
-      </c>
-      <c r="O40" s="83">
-        <v>5</v>
-      </c>
-      <c r="P40" s="83">
-        <v>5</v>
-      </c>
-      <c r="Q40" s="61">
-        <v>7</v>
-      </c>
-      <c r="R40" s="74">
-        <f>SUM(K40:Q40)/6</f>
+      <c r="G40" s="88">
+        <v>4</v>
+      </c>
+      <c r="H40" s="80">
+        <v>2</v>
+      </c>
+      <c r="I40" s="59">
+        <v>1</v>
+      </c>
+      <c r="J40" s="66">
+        <v>3</v>
+      </c>
+      <c r="K40" s="102">
+        <v>3</v>
+      </c>
+      <c r="L40" s="80">
+        <v>2</v>
+      </c>
+      <c r="M40" s="80">
+        <v>3</v>
+      </c>
+      <c r="N40" s="80">
+        <v>2</v>
+      </c>
+      <c r="O40" s="80">
+        <v>5</v>
+      </c>
+      <c r="P40" s="80">
+        <v>5</v>
+      </c>
+      <c r="Q40" s="59">
+        <v>7</v>
+      </c>
+      <c r="R40" s="71">
+        <f t="shared" si="3"/>
         <v>4.5</v>
       </c>
-      <c r="S40" s="110">
+      <c r="S40" s="103">
         <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C41" s="111">
+      <c r="C41" s="104">
         <f>SUM(C31:C40)</f>
         <v>202</v>
       </c>
-      <c r="D41" s="111">
+      <c r="D41" s="104">
         <f>SUM(D31:D40)</f>
         <v>159</v>
       </c>

</xml_diff>

<commit_message>
Summary Model and resource updates. Actions: FIX Missing Hi-Tech metadata UPDATE Engine wormhole implementation Problems
</commit_message>
<xml_diff>
--- a/docs/edition_points.xlsx
+++ b/docs/edition_points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Compile\careers\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4CEA3D-60DA-440F-B470-3FF5A1565E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A54710-AEB2-438B-A7E7-E1EA00740406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="765" windowWidth="24900" windowHeight="13545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3570" yWindow="1305" windowWidth="23580" windowHeight="13110" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hi-Tech Jobs" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="97">
   <si>
     <t>Occupation</t>
   </si>
@@ -327,6 +327,12 @@
   </si>
   <si>
     <t>Average Rank</t>
+  </si>
+  <si>
+    <t>Values only in this table except Average Rank</t>
+  </si>
+  <si>
+    <t>Points + Salary</t>
   </si>
 </sst>
 </file>
@@ -521,7 +527,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -807,6 +813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -822,19 +829,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1142,27 +1157,27 @@
   <sheetData>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="107" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="109"/>
+      <c r="C3" s="108" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="110"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="107" t="s">
+      <c r="K3" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="108"/>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108"/>
-      <c r="S3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="110"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -2088,8 +2103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2731D533-3189-49BB-AE83-771387574D8F}">
   <dimension ref="A3:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q49" sqref="Q49"/>
+    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,27 +2125,27 @@
   <sheetData>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="107" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="109"/>
+      <c r="C3" s="108" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="110"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="107" t="s">
+      <c r="K3" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="108"/>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108"/>
-      <c r="S3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="110"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -2184,8 +2199,8 @@
       <c r="Q4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>50</v>
+      <c r="R4" s="33" t="s">
+        <v>94</v>
       </c>
       <c r="S4" s="19" t="s">
         <v>51</v>
@@ -2195,29 +2210,28 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="112">
+      <c r="A5" s="32">
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="113">
+      <c r="C5" s="1">
         <v>44</v>
       </c>
-      <c r="D5" s="113">
+      <c r="D5" s="1">
         <v>32</v>
       </c>
       <c r="E5" s="29">
         <v>15</v>
       </c>
       <c r="F5" s="29">
-        <f>SUM(C5:E5)</f>
         <v>91</v>
       </c>
       <c r="G5" s="26">
         <v>2</v>
       </c>
-      <c r="H5" s="113">
+      <c r="H5" s="1">
         <v>2</v>
       </c>
       <c r="I5" s="7">
@@ -2229,19 +2243,19 @@
       <c r="K5" s="36">
         <v>1</v>
       </c>
-      <c r="L5" s="113">
-        <v>1</v>
-      </c>
-      <c r="M5" s="113">
-        <v>2</v>
-      </c>
-      <c r="N5" s="113">
-        <v>1</v>
-      </c>
-      <c r="O5" s="113">
-        <v>10</v>
-      </c>
-      <c r="P5" s="113">
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>2</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>7</v>
+      </c>
+      <c r="P5" s="1">
         <v>8</v>
       </c>
       <c r="Q5" s="4">
@@ -2249,14 +2263,14 @@
       </c>
       <c r="R5" s="34">
         <f>(O5+SUM(K5:M5))/4</f>
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="S5" s="4">
         <v>1</v>
       </c>
       <c r="T5" s="1">
         <f>SUM(K5:Q5)</f>
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -2272,14 +2286,13 @@
       <c r="D6" s="43">
         <v>21</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="44">
         <v>8</v>
       </c>
       <c r="F6" s="44">
-        <f>SUM(C6:E6)</f>
         <v>42</v>
       </c>
-      <c r="G6" s="53">
+      <c r="G6" s="45">
         <v>2</v>
       </c>
       <c r="H6" s="43">
@@ -2289,7 +2302,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K6" s="48">
         <v>7</v>
@@ -2298,13 +2311,13 @@
         <v>5</v>
       </c>
       <c r="M6" s="49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N6" s="49">
         <v>6</v>
       </c>
       <c r="O6" s="49">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P6" s="49">
         <v>10</v>
@@ -2313,14 +2326,14 @@
         <v>9</v>
       </c>
       <c r="R6" s="51">
-        <f>(O6+SUM(K6:M6))/4</f>
+        <f t="shared" ref="R6:R14" si="0">(O6+SUM(K6:M6))/4</f>
         <v>6.25</v>
       </c>
       <c r="S6" s="50">
         <v>6</v>
       </c>
       <c r="T6" s="1">
-        <f t="shared" ref="T6:T14" si="0">SUM(K6:Q6)</f>
+        <f t="shared" ref="T6:T14" si="1">SUM(K6:Q6)</f>
         <v>50</v>
       </c>
     </row>
@@ -2331,23 +2344,22 @@
       <c r="B7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="113">
+      <c r="C7" s="1">
         <v>12</v>
       </c>
-      <c r="D7" s="113">
+      <c r="D7" s="1">
         <v>12</v>
       </c>
       <c r="E7" s="29">
         <v>0</v>
       </c>
       <c r="F7" s="29">
-        <f>SUM(C7:E7)</f>
         <v>24</v>
       </c>
       <c r="G7" s="26">
         <v>2</v>
       </c>
-      <c r="H7" s="113">
+      <c r="H7" s="1">
         <v>2</v>
       </c>
       <c r="I7" s="4">
@@ -2359,34 +2371,34 @@
       <c r="K7" s="35">
         <v>8</v>
       </c>
-      <c r="L7" s="113">
-        <v>7</v>
-      </c>
-      <c r="M7" s="113">
-        <v>10</v>
-      </c>
-      <c r="N7" s="113">
-        <v>9</v>
-      </c>
-      <c r="O7" s="113">
-        <v>7</v>
-      </c>
-      <c r="P7" s="113">
+      <c r="L7" s="1">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1">
+        <v>10</v>
+      </c>
+      <c r="N7" s="1">
+        <v>9</v>
+      </c>
+      <c r="O7" s="1">
+        <v>10</v>
+      </c>
+      <c r="P7" s="1">
         <v>2</v>
       </c>
       <c r="Q7" s="4">
         <v>1</v>
       </c>
       <c r="R7" s="34">
-        <f>(O7+SUM(K7:M7))/4</f>
-        <v>8</v>
-      </c>
-      <c r="S7" s="115">
+        <f t="shared" si="0"/>
+        <v>8.75</v>
+      </c>
+      <c r="S7" s="4">
         <v>9</v>
       </c>
       <c r="T7" s="1">
-        <f t="shared" si="0"/>
-        <v>44</v>
+        <f t="shared" si="1"/>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -2396,23 +2408,22 @@
       <c r="B8" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="114">
-        <v>4</v>
-      </c>
-      <c r="D8" s="114">
+      <c r="C8" s="43">
+        <v>4</v>
+      </c>
+      <c r="D8" s="43">
         <v>12</v>
       </c>
       <c r="E8" s="44">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F8" s="44">
-        <f>SUM(C8:E8)</f>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G8" s="45">
         <v>8</v>
       </c>
-      <c r="H8" s="114">
+      <c r="H8" s="43">
         <v>3</v>
       </c>
       <c r="I8" s="46">
@@ -2424,34 +2435,34 @@
       <c r="K8" s="48">
         <v>9</v>
       </c>
-      <c r="L8" s="111">
-        <v>6</v>
-      </c>
-      <c r="M8" s="111">
-        <v>5</v>
-      </c>
-      <c r="N8" s="111">
-        <v>10</v>
-      </c>
-      <c r="O8" s="111">
-        <v>1</v>
-      </c>
-      <c r="P8" s="111">
+      <c r="L8" s="49">
+        <v>8</v>
+      </c>
+      <c r="M8" s="49">
+        <v>8</v>
+      </c>
+      <c r="N8" s="49">
+        <v>10</v>
+      </c>
+      <c r="O8" s="49">
+        <v>1</v>
+      </c>
+      <c r="P8" s="49">
         <v>1</v>
       </c>
       <c r="Q8" s="50">
         <v>2</v>
       </c>
       <c r="R8" s="51">
-        <f>(O8+SUM(K8:M8))/4</f>
-        <v>5.25</v>
+        <f t="shared" si="0"/>
+        <v>6.5</v>
       </c>
       <c r="S8" s="50">
         <v>10</v>
       </c>
       <c r="T8" s="1">
-        <f t="shared" si="0"/>
-        <v>34</v>
+        <f t="shared" si="1"/>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -2471,7 +2482,6 @@
         <v>8</v>
       </c>
       <c r="F9" s="14">
-        <f>SUM(C9:E9)</f>
         <v>34</v>
       </c>
       <c r="G9" s="6">
@@ -2490,7 +2500,7 @@
         <v>6</v>
       </c>
       <c r="L9" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M9" s="1">
         <v>3</v>
@@ -2508,15 +2518,15 @@
         <v>7</v>
       </c>
       <c r="R9" s="34">
-        <f>(O9+SUM(K9:M9))/4</f>
-        <v>5.25</v>
-      </c>
-      <c r="S9" s="115">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+      <c r="S9" s="4">
         <v>7</v>
       </c>
       <c r="T9" s="1">
-        <f t="shared" si="0"/>
-        <v>42</v>
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -2526,23 +2536,22 @@
       <c r="B10" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="111">
-        <v>2</v>
-      </c>
-      <c r="D10" s="111">
+      <c r="C10" s="49">
+        <v>2</v>
+      </c>
+      <c r="D10" s="49">
         <v>23</v>
       </c>
       <c r="E10" s="56">
         <v>3</v>
       </c>
       <c r="F10" s="44">
-        <f>SUM(C10:E10)</f>
         <v>28</v>
       </c>
       <c r="G10" s="70">
         <v>2</v>
       </c>
-      <c r="H10" s="111">
+      <c r="H10" s="49">
         <v>2</v>
       </c>
       <c r="I10" s="50">
@@ -2554,34 +2563,34 @@
       <c r="K10" s="48">
         <v>10</v>
       </c>
-      <c r="L10" s="111">
-        <v>4</v>
-      </c>
-      <c r="M10" s="111">
-        <v>9</v>
-      </c>
-      <c r="N10" s="111">
-        <v>7</v>
-      </c>
-      <c r="O10" s="111">
-        <v>8</v>
-      </c>
-      <c r="P10" s="111">
+      <c r="L10" s="49">
+        <v>4</v>
+      </c>
+      <c r="M10" s="49">
+        <v>9</v>
+      </c>
+      <c r="N10" s="49">
+        <v>7</v>
+      </c>
+      <c r="O10" s="49">
+        <v>9</v>
+      </c>
+      <c r="P10" s="49">
         <v>5</v>
       </c>
       <c r="Q10" s="50">
         <v>5</v>
       </c>
       <c r="R10" s="51">
-        <f>(O10+SUM(K10:M10))/4</f>
-        <v>7.75</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="S10" s="50">
         <v>8</v>
       </c>
       <c r="T10" s="1">
-        <f t="shared" si="0"/>
-        <v>48</v>
+        <f t="shared" si="1"/>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -2591,23 +2600,22 @@
       <c r="B11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="113">
+      <c r="C11" s="1">
         <v>38</v>
       </c>
-      <c r="D11" s="113">
+      <c r="D11" s="1">
         <v>6</v>
       </c>
       <c r="E11" s="25">
         <v>5</v>
       </c>
-      <c r="F11" s="14">
-        <f>SUM(C11:E11)</f>
+      <c r="F11" s="29">
         <v>49</v>
       </c>
       <c r="G11" s="26">
         <v>6</v>
       </c>
-      <c r="H11" s="113">
+      <c r="H11" s="1">
         <v>2</v>
       </c>
       <c r="I11" s="4">
@@ -2619,33 +2627,33 @@
       <c r="K11" s="35">
         <v>2</v>
       </c>
-      <c r="L11" s="113">
-        <v>10</v>
-      </c>
-      <c r="M11" s="113">
-        <v>6</v>
-      </c>
-      <c r="N11" s="113">
-        <v>4</v>
-      </c>
-      <c r="O11" s="113">
-        <v>2</v>
-      </c>
-      <c r="P11" s="113">
+      <c r="L11" s="1">
+        <v>9</v>
+      </c>
+      <c r="M11" s="1">
+        <v>6</v>
+      </c>
+      <c r="N11" s="1">
+        <v>4</v>
+      </c>
+      <c r="O11" s="1">
+        <v>3</v>
+      </c>
+      <c r="P11" s="1">
         <v>4</v>
       </c>
       <c r="Q11" s="4">
         <v>4</v>
       </c>
       <c r="R11" s="34">
-        <f>(O11+SUM(K11:M11))/4</f>
-        <v>5</v>
-      </c>
-      <c r="S11" s="115">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="S11" s="50">
         <v>4</v>
       </c>
       <c r="T11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
     </row>
@@ -2666,7 +2674,6 @@
         <v>4</v>
       </c>
       <c r="F12" s="44">
-        <f>SUM(C12:E12)</f>
         <v>42</v>
       </c>
       <c r="G12" s="57">
@@ -2685,7 +2692,7 @@
         <v>4</v>
       </c>
       <c r="L12" s="49">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M12" s="49">
         <v>7</v>
@@ -2694,7 +2701,7 @@
         <v>5</v>
       </c>
       <c r="O12" s="49">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P12" s="49">
         <v>9</v>
@@ -2703,15 +2710,15 @@
         <v>6</v>
       </c>
       <c r="R12" s="51">
-        <f>(O12+SUM(K12:M12))/4</f>
-        <v>5.75</v>
-      </c>
-      <c r="S12" s="50">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="S12" s="4">
         <v>5</v>
       </c>
       <c r="T12" s="1">
-        <f t="shared" si="0"/>
-        <v>43</v>
+        <f t="shared" si="1"/>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -2722,7 +2729,7 @@
         <v>35</v>
       </c>
       <c r="C13" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1">
         <v>24</v>
@@ -2730,12 +2737,11 @@
       <c r="E13" s="15">
         <v>30</v>
       </c>
-      <c r="F13" s="29">
-        <f>SUM(C13:E13)</f>
-        <v>68</v>
+      <c r="F13" s="14">
+        <v>66</v>
       </c>
       <c r="G13" s="13">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H13" s="1">
         <v>2</v>
@@ -2759,7 +2765,7 @@
         <v>2</v>
       </c>
       <c r="O13" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P13" s="1">
         <v>3</v>
@@ -2768,15 +2774,15 @@
         <v>3</v>
       </c>
       <c r="R13" s="34">
-        <f>(O13+SUM(K13:M13))/4</f>
-        <v>3.75</v>
-      </c>
-      <c r="S13" s="115">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>2.75</v>
+      </c>
+      <c r="S13" s="4">
+        <v>3</v>
       </c>
       <c r="T13" s="1">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -2793,11 +2799,10 @@
         <v>28</v>
       </c>
       <c r="E14" s="62">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F14" s="63">
-        <f>SUM(C14:E14)</f>
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="G14" s="64">
         <v>4</v>
@@ -2818,13 +2823,13 @@
         <v>2</v>
       </c>
       <c r="M14" s="61">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N14" s="61">
         <v>3</v>
       </c>
       <c r="O14" s="61">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P14" s="61">
         <v>7</v>
@@ -2833,45 +2838,45 @@
         <v>8</v>
       </c>
       <c r="R14" s="71">
-        <f>(O14+SUM(K14:M14))/4</f>
-        <v>4.5</v>
+        <f t="shared" si="0"/>
+        <v>3.75</v>
       </c>
       <c r="S14" s="69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T14" s="1">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
       <c r="C15" s="1">
         <f>SUM(C5:C14)</f>
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" ref="D15:I15" si="1">SUM(D5:D14)</f>
+        <f t="shared" ref="D15:I15" si="2">SUM(D5:D14)</f>
         <v>176</v>
       </c>
       <c r="E15" s="16">
-        <f t="shared" si="1"/>
-        <v>83</v>
+        <f t="shared" si="2"/>
+        <v>84</v>
       </c>
       <c r="F15" s="16">
         <f>SUM(F5:F14)</f>
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G15" s="17">
-        <f t="shared" si="1"/>
-        <v>39</v>
+        <f t="shared" si="2"/>
+        <v>42</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="J15" s="23"/>
@@ -2947,28 +2952,34 @@
         <v>67</v>
       </c>
     </row>
+    <row r="27" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>95</v>
+      </c>
+    </row>
     <row r="29" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C29" s="107" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="108"/>
-      <c r="E29" s="108"/>
-      <c r="F29" s="108"/>
-      <c r="G29" s="108"/>
-      <c r="H29" s="108"/>
-      <c r="I29" s="109"/>
+      <c r="C29" s="108" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="109"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="109"/>
+      <c r="G29" s="109"/>
+      <c r="H29" s="109"/>
+      <c r="I29" s="110"/>
       <c r="J29" s="18"/>
-      <c r="K29" s="107" t="s">
+      <c r="K29" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="L29" s="108"/>
-      <c r="M29" s="108"/>
-      <c r="N29" s="108"/>
-      <c r="O29" s="108"/>
-      <c r="P29" s="108"/>
-      <c r="Q29" s="108"/>
-      <c r="R29" s="108"/>
-      <c r="S29" s="109"/>
+      <c r="L29" s="109"/>
+      <c r="M29" s="109"/>
+      <c r="N29" s="109"/>
+      <c r="O29" s="109"/>
+      <c r="P29" s="109"/>
+      <c r="Q29" s="109"/>
+      <c r="R29" s="109"/>
+      <c r="S29" s="110"/>
     </row>
     <row r="30" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
@@ -3030,16 +3041,16 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="112">
+      <c r="A31" s="32">
         <v>1</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="113">
+      <c r="C31" s="1">
         <v>44</v>
       </c>
-      <c r="D31" s="113">
+      <c r="D31" s="1">
         <v>32</v>
       </c>
       <c r="E31" s="29">
@@ -3051,7 +3062,7 @@
       <c r="G31" s="26">
         <v>2</v>
       </c>
-      <c r="H31" s="113">
+      <c r="H31" s="1">
         <v>2</v>
       </c>
       <c r="I31" s="7">
@@ -3063,27 +3074,27 @@
       <c r="K31" s="36">
         <v>1</v>
       </c>
-      <c r="L31" s="113">
-        <v>1</v>
-      </c>
-      <c r="M31" s="113">
-        <v>2</v>
-      </c>
-      <c r="N31" s="113">
-        <v>1</v>
-      </c>
-      <c r="O31" s="113">
-        <v>10</v>
-      </c>
-      <c r="P31" s="113">
+      <c r="L31" s="1">
+        <v>1</v>
+      </c>
+      <c r="M31" s="1">
+        <v>2</v>
+      </c>
+      <c r="N31" s="1">
+        <v>1</v>
+      </c>
+      <c r="O31" s="1">
+        <v>7</v>
+      </c>
+      <c r="P31" s="1">
         <v>8</v>
       </c>
       <c r="Q31" s="4">
         <v>10</v>
       </c>
       <c r="R31" s="34">
-        <f>(O31+SUM(K31:M31))/4</f>
-        <v>3.5</v>
+        <f t="shared" ref="R31:R40" si="3">(O31+SUM(K31:M31))/4</f>
+        <v>2.75</v>
       </c>
       <c r="S31" s="4">
         <v>1</v>
@@ -3102,13 +3113,13 @@
       <c r="D32" s="43">
         <v>21</v>
       </c>
-      <c r="E32" s="52">
-        <v>8</v>
-      </c>
-      <c r="F32" s="52">
+      <c r="E32" s="44">
+        <v>8</v>
+      </c>
+      <c r="F32" s="44">
         <v>42</v>
       </c>
-      <c r="G32" s="53">
+      <c r="G32" s="45">
         <v>2</v>
       </c>
       <c r="H32" s="43">
@@ -3118,7 +3129,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K32" s="48">
         <v>7</v>
@@ -3127,13 +3138,13 @@
         <v>5</v>
       </c>
       <c r="M32" s="49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N32" s="49">
         <v>6</v>
       </c>
       <c r="O32" s="49">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P32" s="49">
         <v>10</v>
@@ -3142,7 +3153,7 @@
         <v>9</v>
       </c>
       <c r="R32" s="51">
-        <f>(O32+SUM(K32:M32))/4</f>
+        <f t="shared" si="3"/>
         <v>6.25</v>
       </c>
       <c r="S32" s="50">
@@ -3150,16 +3161,16 @@
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="112">
+      <c r="A33" s="32">
         <v>3</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="113">
+      <c r="C33" s="1">
         <v>12</v>
       </c>
-      <c r="D33" s="113">
+      <c r="D33" s="1">
         <v>12</v>
       </c>
       <c r="E33" s="29">
@@ -3171,7 +3182,7 @@
       <c r="G33" s="26">
         <v>2</v>
       </c>
-      <c r="H33" s="113">
+      <c r="H33" s="1">
         <v>2</v>
       </c>
       <c r="I33" s="4">
@@ -3183,55 +3194,55 @@
       <c r="K33" s="35">
         <v>8</v>
       </c>
-      <c r="L33" s="113">
-        <v>7</v>
-      </c>
-      <c r="M33" s="113">
-        <v>10</v>
-      </c>
-      <c r="N33" s="113">
-        <v>9</v>
-      </c>
-      <c r="O33" s="113">
-        <v>7</v>
-      </c>
-      <c r="P33" s="113">
+      <c r="L33" s="1">
+        <v>7</v>
+      </c>
+      <c r="M33" s="1">
+        <v>10</v>
+      </c>
+      <c r="N33" s="1">
+        <v>9</v>
+      </c>
+      <c r="O33" s="1">
+        <v>10</v>
+      </c>
+      <c r="P33" s="1">
         <v>2</v>
       </c>
       <c r="Q33" s="4">
         <v>1</v>
       </c>
       <c r="R33" s="34">
-        <f>(O33+SUM(K33:M33))/4</f>
-        <v>8</v>
-      </c>
-      <c r="S33" s="115">
+        <f t="shared" si="3"/>
+        <v>8.75</v>
+      </c>
+      <c r="S33" s="4">
         <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="110">
+      <c r="A34" s="41">
         <v>4</v>
       </c>
       <c r="B34" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="114">
-        <v>4</v>
-      </c>
-      <c r="D34" s="114">
+      <c r="C34" s="43">
+        <v>4</v>
+      </c>
+      <c r="D34" s="43">
         <v>12</v>
       </c>
       <c r="E34" s="44">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F34" s="44">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G34" s="45">
         <v>8</v>
       </c>
-      <c r="H34" s="114">
+      <c r="H34" s="43">
         <v>3</v>
       </c>
       <c r="I34" s="46">
@@ -3243,27 +3254,27 @@
       <c r="K34" s="48">
         <v>9</v>
       </c>
-      <c r="L34" s="111">
-        <v>6</v>
-      </c>
-      <c r="M34" s="111">
-        <v>5</v>
-      </c>
-      <c r="N34" s="111">
-        <v>10</v>
-      </c>
-      <c r="O34" s="111">
-        <v>1</v>
-      </c>
-      <c r="P34" s="111">
+      <c r="L34" s="49">
+        <v>8</v>
+      </c>
+      <c r="M34" s="49">
+        <v>8</v>
+      </c>
+      <c r="N34" s="49">
+        <v>10</v>
+      </c>
+      <c r="O34" s="49">
+        <v>1</v>
+      </c>
+      <c r="P34" s="49">
         <v>1</v>
       </c>
       <c r="Q34" s="50">
         <v>2</v>
       </c>
       <c r="R34" s="51">
-        <f>(O34+SUM(K34:M34))/4</f>
-        <v>5.25</v>
+        <f t="shared" si="3"/>
+        <v>6.5</v>
       </c>
       <c r="S34" s="50">
         <v>10</v>
@@ -3304,7 +3315,7 @@
         <v>6</v>
       </c>
       <c r="L35" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M35" s="1">
         <v>3</v>
@@ -3322,24 +3333,24 @@
         <v>7</v>
       </c>
       <c r="R35" s="34">
-        <f>(O35+SUM(K35:M35))/4</f>
-        <v>5.25</v>
-      </c>
-      <c r="S35" s="115">
+        <f t="shared" si="3"/>
+        <v>4.75</v>
+      </c>
+      <c r="S35" s="4">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="110">
+      <c r="A36" s="41">
         <v>6</v>
       </c>
       <c r="B36" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="111">
-        <v>2</v>
-      </c>
-      <c r="D36" s="111">
+      <c r="C36" s="49">
+        <v>2</v>
+      </c>
+      <c r="D36" s="49">
         <v>23</v>
       </c>
       <c r="E36" s="56">
@@ -3351,7 +3362,7 @@
       <c r="G36" s="70">
         <v>2</v>
       </c>
-      <c r="H36" s="111">
+      <c r="H36" s="49">
         <v>2</v>
       </c>
       <c r="I36" s="50">
@@ -3363,43 +3374,43 @@
       <c r="K36" s="48">
         <v>10</v>
       </c>
-      <c r="L36" s="111">
-        <v>4</v>
-      </c>
-      <c r="M36" s="111">
-        <v>9</v>
-      </c>
-      <c r="N36" s="111">
-        <v>7</v>
-      </c>
-      <c r="O36" s="111">
-        <v>8</v>
-      </c>
-      <c r="P36" s="111">
+      <c r="L36" s="49">
+        <v>4</v>
+      </c>
+      <c r="M36" s="49">
+        <v>9</v>
+      </c>
+      <c r="N36" s="49">
+        <v>7</v>
+      </c>
+      <c r="O36" s="49">
+        <v>9</v>
+      </c>
+      <c r="P36" s="49">
         <v>5</v>
       </c>
       <c r="Q36" s="50">
         <v>5</v>
       </c>
       <c r="R36" s="51">
-        <f>(O36+SUM(K36:M36))/4</f>
-        <v>7.75</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="S36" s="50">
         <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="112">
+      <c r="A37" s="32">
         <v>7</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="113">
+      <c r="C37" s="1">
         <v>38</v>
       </c>
-      <c r="D37" s="113">
+      <c r="D37" s="1">
         <v>6</v>
       </c>
       <c r="E37" s="25">
@@ -3411,7 +3422,7 @@
       <c r="G37" s="26">
         <v>6</v>
       </c>
-      <c r="H37" s="113">
+      <c r="H37" s="1">
         <v>2</v>
       </c>
       <c r="I37" s="4">
@@ -3423,29 +3434,29 @@
       <c r="K37" s="35">
         <v>2</v>
       </c>
-      <c r="L37" s="113">
-        <v>10</v>
-      </c>
-      <c r="M37" s="113">
-        <v>6</v>
-      </c>
-      <c r="N37" s="113">
-        <v>4</v>
-      </c>
-      <c r="O37" s="113">
-        <v>2</v>
-      </c>
-      <c r="P37" s="113">
+      <c r="L37" s="1">
+        <v>9</v>
+      </c>
+      <c r="M37" s="1">
+        <v>6</v>
+      </c>
+      <c r="N37" s="1">
+        <v>4</v>
+      </c>
+      <c r="O37" s="1">
+        <v>3</v>
+      </c>
+      <c r="P37" s="1">
         <v>4</v>
       </c>
       <c r="Q37" s="4">
         <v>4</v>
       </c>
-      <c r="R37" s="34">
-        <f>(O37+SUM(K37:M37))/4</f>
-        <v>5</v>
-      </c>
-      <c r="S37" s="115">
+      <c r="R37" s="51">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="S37" s="50">
         <v>4</v>
       </c>
     </row>
@@ -3484,7 +3495,7 @@
         <v>4</v>
       </c>
       <c r="L38" s="49">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M38" s="49">
         <v>7</v>
@@ -3493,7 +3504,7 @@
         <v>5</v>
       </c>
       <c r="O38" s="49">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P38" s="49">
         <v>9</v>
@@ -3501,11 +3512,11 @@
       <c r="Q38" s="50">
         <v>6</v>
       </c>
-      <c r="R38" s="51">
-        <f>(O38+SUM(K38:M38))/4</f>
-        <v>5.75</v>
-      </c>
-      <c r="S38" s="50">
+      <c r="R38" s="34">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="S38" s="4">
         <v>5</v>
       </c>
     </row>
@@ -3517,7 +3528,7 @@
         <v>35</v>
       </c>
       <c r="C39" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D39" s="1">
         <v>24</v>
@@ -3526,10 +3537,10 @@
         <v>30</v>
       </c>
       <c r="F39" s="14">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G39" s="13">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H39" s="1">
         <v>2</v>
@@ -3553,7 +3564,7 @@
         <v>2</v>
       </c>
       <c r="O39" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P39" s="1">
         <v>3</v>
@@ -3562,11 +3573,11 @@
         <v>3</v>
       </c>
       <c r="R39" s="34">
-        <f>(O39+SUM(K39:M39))/4</f>
-        <v>3.75</v>
-      </c>
-      <c r="S39" s="115">
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>2.75</v>
+      </c>
+      <c r="S39" s="4">
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -3583,10 +3594,10 @@
         <v>28</v>
       </c>
       <c r="E40" s="62">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F40" s="63">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="G40" s="64">
         <v>4</v>
@@ -3607,13 +3618,13 @@
         <v>2</v>
       </c>
       <c r="M40" s="61">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N40" s="61">
         <v>3</v>
       </c>
       <c r="O40" s="61">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P40" s="61">
         <v>7</v>
@@ -3622,45 +3633,45 @@
         <v>8</v>
       </c>
       <c r="R40" s="71">
-        <f>(O40+SUM(K40:M40))/4</f>
-        <v>4.5</v>
+        <f t="shared" si="3"/>
+        <v>3.75</v>
       </c>
       <c r="S40" s="69">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F42" s="116"/>
+      <c r="F42" s="107"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F43" s="116"/>
+      <c r="F43" s="107"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F44" s="116"/>
+      <c r="F44" s="107"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F45" s="116"/>
+      <c r="F45" s="107"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F46" s="116"/>
+      <c r="F46" s="107"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F47" s="116"/>
+      <c r="F47" s="107"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F48" s="116"/>
+      <c r="F48" s="107"/>
     </row>
     <row r="49" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="116"/>
+      <c r="F49" s="107"/>
     </row>
     <row r="50" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F50" s="116"/>
+      <c r="F50" s="107"/>
     </row>
     <row r="51" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F51" s="116"/>
+      <c r="F51" s="107"/>
     </row>
     <row r="52" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F52" s="116"/>
+      <c r="F52" s="107"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A31:S40">
@@ -3681,8 +3692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66559D5-1C3E-471D-81A3-258D37D68792}">
   <dimension ref="A3:T39"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3700,27 +3711,27 @@
   <sheetData>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="107" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="109"/>
+      <c r="C3" s="108" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="110"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="107" t="s">
+      <c r="K3" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="108"/>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108"/>
-      <c r="S3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="110"/>
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
@@ -3792,26 +3803,25 @@
       <c r="B5" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="116">
         <v>38</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="115">
         <v>18</v>
       </c>
       <c r="E5" s="29">
         <v>15</v>
       </c>
       <c r="F5" s="29">
-        <f>SUM(C5:E5)</f>
         <v>71</v>
       </c>
-      <c r="G5" s="1">
-        <v>2</v>
-      </c>
-      <c r="H5" s="1">
-        <v>2</v>
-      </c>
-      <c r="I5" s="7">
+      <c r="G5" s="115">
+        <v>2</v>
+      </c>
+      <c r="H5" s="115">
+        <v>2</v>
+      </c>
+      <c r="I5" s="84">
         <v>0</v>
       </c>
       <c r="J5" s="20">
@@ -3820,34 +3830,33 @@
       <c r="K5" s="36">
         <v>1</v>
       </c>
-      <c r="L5" s="1">
-        <v>5</v>
-      </c>
-      <c r="M5" s="1">
-        <v>2</v>
-      </c>
-      <c r="N5" s="1">
-        <v>1</v>
-      </c>
-      <c r="O5" s="1">
-        <v>8</v>
-      </c>
-      <c r="P5" s="1">
-        <v>6</v>
+      <c r="L5" s="116">
+        <v>5</v>
+      </c>
+      <c r="M5" s="116">
+        <v>2</v>
+      </c>
+      <c r="N5" s="116">
+        <v>1</v>
+      </c>
+      <c r="O5" s="116">
+        <v>7</v>
+      </c>
+      <c r="P5" s="116">
+        <v>8</v>
       </c>
       <c r="Q5" s="4">
         <v>10</v>
       </c>
       <c r="R5" s="34">
-        <f>SUM(K5:Q5)/6</f>
-        <v>5.5</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="S5" s="4">
         <v>1</v>
       </c>
       <c r="T5" s="1">
         <f>SUM(K5:Q5)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -3857,26 +3866,25 @@
       <c r="B6" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="43">
-        <v>8</v>
-      </c>
-      <c r="D6" s="79">
+      <c r="C6" s="113">
+        <v>8</v>
+      </c>
+      <c r="D6" s="114">
         <v>21</v>
       </c>
       <c r="E6" s="44">
         <v>8</v>
       </c>
       <c r="F6" s="44">
-        <f>SUM(C6:E6)</f>
         <v>37</v>
       </c>
-      <c r="G6" s="43">
-        <v>1</v>
-      </c>
-      <c r="H6" s="43">
-        <v>1</v>
-      </c>
-      <c r="I6" s="46">
+      <c r="G6" s="114">
+        <v>1</v>
+      </c>
+      <c r="H6" s="114">
+        <v>1</v>
+      </c>
+      <c r="I6" s="81">
         <v>1</v>
       </c>
       <c r="J6" s="47">
@@ -3885,34 +3893,33 @@
       <c r="K6" s="48">
         <v>7</v>
       </c>
-      <c r="L6" s="49">
-        <v>3</v>
-      </c>
-      <c r="M6" s="49">
-        <v>5</v>
-      </c>
-      <c r="N6" s="49">
-        <v>6</v>
-      </c>
-      <c r="O6" s="49">
-        <v>10</v>
-      </c>
-      <c r="P6" s="49">
+      <c r="L6" s="112">
+        <v>3</v>
+      </c>
+      <c r="M6" s="112">
+        <v>5</v>
+      </c>
+      <c r="N6" s="112">
+        <v>6</v>
+      </c>
+      <c r="O6" s="112">
+        <v>9</v>
+      </c>
+      <c r="P6" s="112">
         <v>10</v>
       </c>
       <c r="Q6" s="50">
         <v>8</v>
       </c>
       <c r="R6" s="51">
-        <f t="shared" ref="R6:R14" si="0">SUM(K6:Q6)/6</f>
-        <v>8.1666666666666661</v>
+        <v>8</v>
       </c>
       <c r="S6" s="50">
         <v>6</v>
       </c>
       <c r="T6" s="1">
-        <f t="shared" ref="T6:T14" si="1">SUM(K6:Q6)</f>
-        <v>49</v>
+        <f t="shared" ref="T6:T14" si="0">SUM(K6:Q6)</f>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -3922,26 +3929,25 @@
       <c r="B7" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="116">
         <v>12</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="115">
         <v>12</v>
       </c>
       <c r="E7" s="29">
         <v>0</v>
       </c>
       <c r="F7" s="29">
-        <f>SUM(C7:E7)</f>
         <v>24</v>
       </c>
-      <c r="G7" s="1">
-        <v>2</v>
-      </c>
-      <c r="H7" s="1">
-        <v>2</v>
-      </c>
-      <c r="I7" s="4">
+      <c r="G7" s="115">
+        <v>2</v>
+      </c>
+      <c r="H7" s="115">
+        <v>2</v>
+      </c>
+      <c r="I7" s="83">
         <v>4</v>
       </c>
       <c r="J7" s="22">
@@ -3950,34 +3956,33 @@
       <c r="K7" s="35">
         <v>5</v>
       </c>
-      <c r="L7" s="1">
-        <v>7</v>
-      </c>
-      <c r="M7" s="1">
-        <v>10</v>
-      </c>
-      <c r="N7" s="1">
-        <v>9</v>
-      </c>
-      <c r="O7" s="1">
-        <v>7</v>
-      </c>
-      <c r="P7" s="1">
-        <v>1</v>
+      <c r="L7" s="116">
+        <v>7</v>
+      </c>
+      <c r="M7" s="116">
+        <v>10</v>
+      </c>
+      <c r="N7" s="116">
+        <v>9</v>
+      </c>
+      <c r="O7" s="116">
+        <v>8</v>
+      </c>
+      <c r="P7" s="116">
+        <v>2</v>
       </c>
       <c r="Q7" s="4">
         <v>1</v>
       </c>
       <c r="R7" s="34">
+        <v>7</v>
+      </c>
+      <c r="S7" s="4">
+        <v>10</v>
+      </c>
+      <c r="T7" s="1">
         <f t="shared" si="0"/>
-        <v>6.666666666666667</v>
-      </c>
-      <c r="S7" s="4">
-        <v>9</v>
-      </c>
-      <c r="T7" s="1">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -3987,26 +3992,25 @@
       <c r="B8" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="43">
-        <v>4</v>
-      </c>
-      <c r="D8" s="79">
+      <c r="C8" s="113">
+        <v>4</v>
+      </c>
+      <c r="D8" s="114">
         <v>12</v>
       </c>
       <c r="E8" s="44">
         <v>3</v>
       </c>
       <c r="F8" s="44">
-        <f>SUM(C8:E8)</f>
         <v>19</v>
       </c>
-      <c r="G8" s="72">
-        <v>8</v>
-      </c>
-      <c r="H8" s="43">
-        <v>1</v>
-      </c>
-      <c r="I8" s="46">
+      <c r="G8" s="56">
+        <v>8</v>
+      </c>
+      <c r="H8" s="114">
+        <v>3</v>
+      </c>
+      <c r="I8" s="81">
         <v>2</v>
       </c>
       <c r="J8" s="47">
@@ -4015,34 +4019,33 @@
       <c r="K8" s="48">
         <v>9</v>
       </c>
-      <c r="L8" s="49">
-        <v>8</v>
-      </c>
-      <c r="M8" s="49">
-        <v>8</v>
-      </c>
-      <c r="N8" s="49">
-        <v>10</v>
-      </c>
-      <c r="O8" s="49">
-        <v>1</v>
-      </c>
-      <c r="P8" s="49">
-        <v>9</v>
+      <c r="L8" s="112">
+        <v>8</v>
+      </c>
+      <c r="M8" s="112">
+        <v>8</v>
+      </c>
+      <c r="N8" s="112">
+        <v>10</v>
+      </c>
+      <c r="O8" s="112">
+        <v>1</v>
+      </c>
+      <c r="P8" s="112">
+        <v>1</v>
       </c>
       <c r="Q8" s="50">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R8" s="51">
+        <v>6.5</v>
+      </c>
+      <c r="S8" s="50">
+        <v>9</v>
+      </c>
+      <c r="T8" s="1">
         <f t="shared" si="0"/>
-        <v>8.3333333333333339</v>
-      </c>
-      <c r="S8" s="50">
-        <v>10</v>
-      </c>
-      <c r="T8" s="1">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -4062,16 +4065,15 @@
         <v>8</v>
       </c>
       <c r="F9" s="14">
-        <f t="shared" ref="F9:F14" si="2">SUM(C9:E9)</f>
         <v>28</v>
       </c>
-      <c r="G9" s="73">
-        <v>5</v>
-      </c>
-      <c r="H9" s="5">
-        <v>2</v>
-      </c>
-      <c r="I9" s="7">
+      <c r="G9" s="15">
+        <v>5</v>
+      </c>
+      <c r="H9" s="16">
+        <v>2</v>
+      </c>
+      <c r="I9" s="84">
         <v>1</v>
       </c>
       <c r="J9" s="21">
@@ -4093,21 +4095,20 @@
         <v>3</v>
       </c>
       <c r="P9" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q9" s="4">
         <v>7</v>
       </c>
       <c r="R9" s="34">
+        <v>6.833333333333333</v>
+      </c>
+      <c r="S9" s="4">
+        <v>7</v>
+      </c>
+      <c r="T9" s="1">
         <f t="shared" si="0"/>
-        <v>6.5</v>
-      </c>
-      <c r="S9" s="4">
-        <v>7</v>
-      </c>
-      <c r="T9" s="1">
-        <f t="shared" si="1"/>
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -4117,26 +4118,25 @@
       <c r="B10" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="49">
-        <v>2</v>
-      </c>
-      <c r="D10" s="41">
+      <c r="C10" s="112">
+        <v>2</v>
+      </c>
+      <c r="D10" s="111">
         <v>23</v>
       </c>
       <c r="E10" s="56">
         <v>3</v>
       </c>
       <c r="F10" s="44">
-        <f>SUM(C10:E10)</f>
         <v>28</v>
       </c>
-      <c r="G10" s="74">
-        <v>1</v>
-      </c>
-      <c r="H10" s="49">
-        <v>1</v>
-      </c>
-      <c r="I10" s="50">
+      <c r="G10" s="85">
+        <v>0</v>
+      </c>
+      <c r="H10" s="111">
+        <v>2</v>
+      </c>
+      <c r="I10" s="86">
         <v>2</v>
       </c>
       <c r="J10" s="55">
@@ -4145,34 +4145,33 @@
       <c r="K10" s="48">
         <v>10</v>
       </c>
-      <c r="L10" s="49">
-        <v>2</v>
-      </c>
-      <c r="M10" s="49">
-        <v>9</v>
-      </c>
-      <c r="N10" s="49">
-        <v>8</v>
-      </c>
-      <c r="O10" s="49">
-        <v>9</v>
-      </c>
-      <c r="P10" s="49">
-        <v>8</v>
+      <c r="L10" s="112">
+        <v>2</v>
+      </c>
+      <c r="M10" s="112">
+        <v>9</v>
+      </c>
+      <c r="N10" s="112">
+        <v>8</v>
+      </c>
+      <c r="O10" s="112">
+        <v>10</v>
+      </c>
+      <c r="P10" s="112">
+        <v>4</v>
       </c>
       <c r="Q10" s="50">
         <v>4</v>
       </c>
       <c r="R10" s="51">
+        <v>7.833333333333333</v>
+      </c>
+      <c r="S10" s="50">
+        <v>8</v>
+      </c>
+      <c r="T10" s="1">
         <f t="shared" si="0"/>
-        <v>8.3333333333333339</v>
-      </c>
-      <c r="S10" s="50">
-        <v>8</v>
-      </c>
-      <c r="T10" s="1">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -4192,16 +4191,15 @@
         <v>5</v>
       </c>
       <c r="F11" s="14">
-        <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="G11" s="75">
-        <v>6</v>
-      </c>
-      <c r="H11" s="1">
-        <v>2</v>
-      </c>
-      <c r="I11" s="4">
+      <c r="G11" s="82">
+        <v>6</v>
+      </c>
+      <c r="H11" s="32">
+        <v>2</v>
+      </c>
+      <c r="I11" s="83">
         <v>2</v>
       </c>
       <c r="J11" s="22">
@@ -4223,21 +4221,20 @@
         <v>2</v>
       </c>
       <c r="P11" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q11" s="4">
-        <v>2</v>
-      </c>
-      <c r="R11" s="34">
+        <v>3</v>
+      </c>
+      <c r="R11" s="118">
+        <v>4.833333333333333</v>
+      </c>
+      <c r="S11" s="119">
+        <v>4</v>
+      </c>
+      <c r="T11" s="1">
         <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="S11" s="4">
-        <v>4</v>
-      </c>
-      <c r="T11" s="1">
-        <f t="shared" si="1"/>
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -4247,26 +4244,25 @@
       <c r="B12" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="113">
         <v>28</v>
       </c>
-      <c r="D12" s="79">
+      <c r="D12" s="114">
         <v>6</v>
       </c>
       <c r="E12" s="56">
         <v>4</v>
       </c>
       <c r="F12" s="44">
-        <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="G12" s="76">
-        <v>4</v>
-      </c>
-      <c r="H12" s="43">
-        <v>1</v>
-      </c>
-      <c r="I12" s="46">
+      <c r="G12" s="44">
+        <v>4</v>
+      </c>
+      <c r="H12" s="114">
+        <v>1</v>
+      </c>
+      <c r="I12" s="81">
         <v>2</v>
       </c>
       <c r="J12" s="58">
@@ -4275,34 +4271,33 @@
       <c r="K12" s="48">
         <v>3</v>
       </c>
-      <c r="L12" s="49">
-        <v>10</v>
-      </c>
-      <c r="M12" s="49">
-        <v>7</v>
-      </c>
-      <c r="N12" s="49">
-        <v>5</v>
-      </c>
-      <c r="O12" s="49">
-        <v>4</v>
-      </c>
-      <c r="P12" s="49">
-        <v>7</v>
+      <c r="L12" s="112">
+        <v>10</v>
+      </c>
+      <c r="M12" s="112">
+        <v>7</v>
+      </c>
+      <c r="N12" s="112">
+        <v>5</v>
+      </c>
+      <c r="O12" s="112">
+        <v>5</v>
+      </c>
+      <c r="P12" s="112">
+        <v>9</v>
       </c>
       <c r="Q12" s="50">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R12" s="51">
+        <v>7.333333333333333</v>
+      </c>
+      <c r="S12" s="50">
+        <v>5</v>
+      </c>
+      <c r="T12" s="1">
         <f t="shared" si="0"/>
-        <v>6.5</v>
-      </c>
-      <c r="S12" s="50">
-        <v>5</v>
-      </c>
-      <c r="T12" s="1">
-        <f t="shared" si="1"/>
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -4322,16 +4317,15 @@
         <v>30</v>
       </c>
       <c r="F13" s="29">
-        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="G13" s="77">
-        <v>3</v>
-      </c>
-      <c r="H13" s="1">
-        <v>2</v>
-      </c>
-      <c r="I13" s="7">
+      <c r="G13" s="87">
+        <v>3</v>
+      </c>
+      <c r="H13" s="32">
+        <v>2</v>
+      </c>
+      <c r="I13" s="84">
         <v>0</v>
       </c>
       <c r="J13" s="22">
@@ -4353,21 +4347,20 @@
         <v>6</v>
       </c>
       <c r="P13" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q13" s="4">
         <v>9</v>
       </c>
       <c r="R13" s="34">
+        <v>6</v>
+      </c>
+      <c r="S13" s="4">
+        <v>3</v>
+      </c>
+      <c r="T13" s="1">
         <f t="shared" si="0"/>
-        <v>5.666666666666667</v>
-      </c>
-      <c r="S13" s="4">
-        <v>3</v>
-      </c>
-      <c r="T13" s="1">
-        <f t="shared" si="1"/>
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -4387,16 +4380,15 @@
         <v>9</v>
       </c>
       <c r="F14" s="63">
-        <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="G14" s="78">
-        <v>4</v>
-      </c>
-      <c r="H14" s="61">
-        <v>2</v>
-      </c>
-      <c r="I14" s="65">
+      <c r="G14" s="88">
+        <v>4</v>
+      </c>
+      <c r="H14" s="80">
+        <v>2</v>
+      </c>
+      <c r="I14" s="59">
         <v>1</v>
       </c>
       <c r="J14" s="66">
@@ -4415,24 +4407,23 @@
         <v>2</v>
       </c>
       <c r="O14" s="61">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P14" s="61">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q14" s="65">
         <v>6</v>
       </c>
       <c r="R14" s="71">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="S14" s="69">
+        <v>2</v>
+      </c>
+      <c r="T14" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="S14" s="69">
-        <v>2</v>
-      </c>
-      <c r="T14" s="1">
-        <f t="shared" si="1"/>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -4440,39 +4431,39 @@
         <v>65</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:J15" si="3">SUM(C5:C14)</f>
+        <f t="shared" ref="C15:J15" si="1">SUM(C5:C14)</f>
         <v>154</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>174</v>
       </c>
       <c r="E15" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="F15" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>413</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="3"/>
-        <v>36</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="3"/>
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="J15" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B19" s="37" t="s">
         <v>47</v>
       </c>
@@ -4483,7 +4474,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B20" s="37" t="s">
         <v>46</v>
       </c>
@@ -4494,7 +4485,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B21" s="37" t="s">
         <v>45</v>
       </c>
@@ -4505,7 +4496,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B22" s="37" t="s">
         <v>48</v>
       </c>
@@ -4516,7 +4507,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B23" s="37" t="s">
         <v>9</v>
       </c>
@@ -4527,7 +4518,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B24" s="38" t="s">
         <v>8</v>
       </c>
@@ -4538,7 +4529,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B25" s="37" t="s">
         <v>10</v>
       </c>
@@ -4549,7 +4540,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>49</v>
       </c>
@@ -4607,30 +4598,33 @@
       <c r="S27" s="19" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="32">
+      <c r="T27" s="117" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="115">
         <v>1</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="116">
         <v>38</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="115">
         <v>18</v>
       </c>
       <c r="E28" s="29">
         <v>15</v>
       </c>
       <c r="F28" s="29">
-        <v>67</v>
-      </c>
-      <c r="G28" s="32">
-        <v>2</v>
-      </c>
-      <c r="H28" s="32">
+        <v>71</v>
+      </c>
+      <c r="G28" s="115">
+        <v>2</v>
+      </c>
+      <c r="H28" s="115">
         <v>2</v>
       </c>
       <c r="I28" s="84">
@@ -4642,43 +4636,47 @@
       <c r="K28" s="36">
         <v>1</v>
       </c>
-      <c r="L28" s="1">
-        <v>5</v>
-      </c>
-      <c r="M28" s="1">
-        <v>2</v>
-      </c>
-      <c r="N28" s="1">
-        <v>1</v>
-      </c>
-      <c r="O28" s="1">
-        <v>8</v>
-      </c>
-      <c r="P28" s="1">
-        <v>6</v>
+      <c r="L28" s="116">
+        <v>5</v>
+      </c>
+      <c r="M28" s="116">
+        <v>2</v>
+      </c>
+      <c r="N28" s="116">
+        <v>1</v>
+      </c>
+      <c r="O28" s="116">
+        <v>7</v>
+      </c>
+      <c r="P28" s="116">
+        <v>8</v>
       </c>
       <c r="Q28" s="4">
         <v>10</v>
       </c>
       <c r="R28" s="34">
-        <f t="shared" ref="R28:R37" si="4">SUM(K28:Q28)/6</f>
-        <v>5.5</v>
+        <f>SUM(K28:Q28)/6</f>
+        <v>5.666666666666667</v>
       </c>
       <c r="S28" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="41">
+      <c r="T28" s="104">
+        <f>F28+G28</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="111">
         <v>2</v>
       </c>
       <c r="B29" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="43">
-        <v>8</v>
-      </c>
-      <c r="D29" s="79">
+      <c r="C29" s="113">
+        <v>8</v>
+      </c>
+      <c r="D29" s="114">
         <v>21</v>
       </c>
       <c r="E29" s="44">
@@ -4687,10 +4685,10 @@
       <c r="F29" s="44">
         <v>37</v>
       </c>
-      <c r="G29" s="79">
-        <v>1</v>
-      </c>
-      <c r="H29" s="79">
+      <c r="G29" s="114">
+        <v>1</v>
+      </c>
+      <c r="H29" s="114">
         <v>1</v>
       </c>
       <c r="I29" s="81">
@@ -4702,43 +4700,47 @@
       <c r="K29" s="48">
         <v>7</v>
       </c>
-      <c r="L29" s="49">
-        <v>3</v>
-      </c>
-      <c r="M29" s="49">
-        <v>5</v>
-      </c>
-      <c r="N29" s="49">
-        <v>6</v>
-      </c>
-      <c r="O29" s="49">
-        <v>10</v>
-      </c>
-      <c r="P29" s="49">
+      <c r="L29" s="112">
+        <v>3</v>
+      </c>
+      <c r="M29" s="112">
+        <v>5</v>
+      </c>
+      <c r="N29" s="112">
+        <v>6</v>
+      </c>
+      <c r="O29" s="112">
+        <v>9</v>
+      </c>
+      <c r="P29" s="112">
         <v>10</v>
       </c>
       <c r="Q29" s="50">
         <v>8</v>
       </c>
       <c r="R29" s="51">
-        <f t="shared" si="4"/>
-        <v>8.1666666666666661</v>
+        <f>SUM(K29:Q29)/6</f>
+        <v>8</v>
       </c>
       <c r="S29" s="50">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="32">
+      <c r="T29" s="104">
+        <f t="shared" ref="T29:T37" si="2">F29+G29</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="115">
         <v>3</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="116">
         <v>12</v>
       </c>
-      <c r="D30" s="32">
+      <c r="D30" s="115">
         <v>12</v>
       </c>
       <c r="E30" s="29">
@@ -4747,10 +4749,10 @@
       <c r="F30" s="29">
         <v>24</v>
       </c>
-      <c r="G30" s="32">
-        <v>2</v>
-      </c>
-      <c r="H30" s="32">
+      <c r="G30" s="115">
+        <v>2</v>
+      </c>
+      <c r="H30" s="115">
         <v>2</v>
       </c>
       <c r="I30" s="83">
@@ -4762,43 +4764,47 @@
       <c r="K30" s="35">
         <v>5</v>
       </c>
-      <c r="L30" s="1">
-        <v>7</v>
-      </c>
-      <c r="M30" s="1">
-        <v>10</v>
-      </c>
-      <c r="N30" s="1">
-        <v>9</v>
-      </c>
-      <c r="O30" s="1">
-        <v>7</v>
-      </c>
-      <c r="P30" s="1">
-        <v>1</v>
+      <c r="L30" s="116">
+        <v>7</v>
+      </c>
+      <c r="M30" s="116">
+        <v>10</v>
+      </c>
+      <c r="N30" s="116">
+        <v>9</v>
+      </c>
+      <c r="O30" s="116">
+        <v>8</v>
+      </c>
+      <c r="P30" s="116">
+        <v>2</v>
       </c>
       <c r="Q30" s="4">
         <v>1</v>
       </c>
       <c r="R30" s="34">
-        <f t="shared" si="4"/>
-        <v>6.666666666666667</v>
+        <f>SUM(K30:Q30)/6</f>
+        <v>7</v>
       </c>
       <c r="S30" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="41">
+        <v>10</v>
+      </c>
+      <c r="T30" s="104">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="111">
         <v>4</v>
       </c>
       <c r="B31" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="43">
-        <v>4</v>
-      </c>
-      <c r="D31" s="79">
+      <c r="C31" s="113">
+        <v>4</v>
+      </c>
+      <c r="D31" s="114">
         <v>12</v>
       </c>
       <c r="E31" s="44">
@@ -4810,8 +4816,8 @@
       <c r="G31" s="56">
         <v>8</v>
       </c>
-      <c r="H31" s="79">
-        <v>1</v>
+      <c r="H31" s="114">
+        <v>3</v>
       </c>
       <c r="I31" s="81">
         <v>2</v>
@@ -4822,33 +4828,37 @@
       <c r="K31" s="48">
         <v>9</v>
       </c>
-      <c r="L31" s="49">
-        <v>8</v>
-      </c>
-      <c r="M31" s="49">
-        <v>8</v>
-      </c>
-      <c r="N31" s="49">
-        <v>10</v>
-      </c>
-      <c r="O31" s="49">
-        <v>1</v>
-      </c>
-      <c r="P31" s="49">
-        <v>9</v>
+      <c r="L31" s="112">
+        <v>8</v>
+      </c>
+      <c r="M31" s="112">
+        <v>8</v>
+      </c>
+      <c r="N31" s="112">
+        <v>10</v>
+      </c>
+      <c r="O31" s="112">
+        <v>1</v>
+      </c>
+      <c r="P31" s="112">
+        <v>1</v>
       </c>
       <c r="Q31" s="50">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R31" s="51">
-        <f t="shared" si="4"/>
-        <v>8.3333333333333339</v>
+        <f>SUM(K31:Q31)/6</f>
+        <v>6.5</v>
       </c>
       <c r="S31" s="50">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="T31" s="104">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="32">
         <v>5</v>
       </c>
@@ -4895,30 +4905,34 @@
         <v>3</v>
       </c>
       <c r="P32" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q32" s="4">
         <v>7</v>
       </c>
       <c r="R32" s="34">
-        <f t="shared" si="4"/>
-        <v>6.5</v>
+        <f>SUM(K32:Q32)/6</f>
+        <v>6.833333333333333</v>
       </c>
       <c r="S32" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="41">
+      <c r="T32" s="104">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="111">
         <v>6</v>
       </c>
       <c r="B33" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="49">
-        <v>2</v>
-      </c>
-      <c r="D33" s="41">
+      <c r="C33" s="112">
+        <v>2</v>
+      </c>
+      <c r="D33" s="111">
         <v>23</v>
       </c>
       <c r="E33" s="56">
@@ -4928,10 +4942,10 @@
         <v>28</v>
       </c>
       <c r="G33" s="85">
-        <v>1</v>
-      </c>
-      <c r="H33" s="41">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H33" s="111">
+        <v>2</v>
       </c>
       <c r="I33" s="86">
         <v>2</v>
@@ -4942,33 +4956,37 @@
       <c r="K33" s="48">
         <v>10</v>
       </c>
-      <c r="L33" s="49">
-        <v>2</v>
-      </c>
-      <c r="M33" s="49">
-        <v>9</v>
-      </c>
-      <c r="N33" s="49">
-        <v>8</v>
-      </c>
-      <c r="O33" s="49">
-        <v>9</v>
-      </c>
-      <c r="P33" s="49">
-        <v>8</v>
+      <c r="L33" s="112">
+        <v>2</v>
+      </c>
+      <c r="M33" s="112">
+        <v>9</v>
+      </c>
+      <c r="N33" s="112">
+        <v>8</v>
+      </c>
+      <c r="O33" s="112">
+        <v>10</v>
+      </c>
+      <c r="P33" s="112">
+        <v>4</v>
       </c>
       <c r="Q33" s="50">
         <v>4</v>
       </c>
       <c r="R33" s="51">
-        <f t="shared" si="4"/>
-        <v>8.3333333333333339</v>
+        <f>SUM(K33:Q33)/6</f>
+        <v>7.833333333333333</v>
       </c>
       <c r="S33" s="50">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T33" s="104">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="32">
         <v>7</v>
       </c>
@@ -5015,30 +5033,34 @@
         <v>2</v>
       </c>
       <c r="P34" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q34" s="4">
-        <v>2</v>
-      </c>
-      <c r="R34" s="34">
-        <f t="shared" si="4"/>
-        <v>4.5</v>
-      </c>
-      <c r="S34" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="41">
+        <v>3</v>
+      </c>
+      <c r="R34" s="118">
+        <f>SUM(K34:Q34)/6</f>
+        <v>4.833333333333333</v>
+      </c>
+      <c r="S34" s="119">
+        <v>4</v>
+      </c>
+      <c r="T34" s="104">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="111">
         <v>8</v>
       </c>
       <c r="B35" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="43">
+      <c r="C35" s="113">
         <v>28</v>
       </c>
-      <c r="D35" s="79">
+      <c r="D35" s="114">
         <v>6</v>
       </c>
       <c r="E35" s="56">
@@ -5050,7 +5072,7 @@
       <c r="G35" s="44">
         <v>4</v>
       </c>
-      <c r="H35" s="79">
+      <c r="H35" s="114">
         <v>1</v>
       </c>
       <c r="I35" s="81">
@@ -5062,33 +5084,37 @@
       <c r="K35" s="48">
         <v>3</v>
       </c>
-      <c r="L35" s="49">
-        <v>10</v>
-      </c>
-      <c r="M35" s="49">
-        <v>7</v>
-      </c>
-      <c r="N35" s="49">
-        <v>5</v>
-      </c>
-      <c r="O35" s="49">
-        <v>4</v>
-      </c>
-      <c r="P35" s="49">
-        <v>7</v>
+      <c r="L35" s="112">
+        <v>10</v>
+      </c>
+      <c r="M35" s="112">
+        <v>7</v>
+      </c>
+      <c r="N35" s="112">
+        <v>5</v>
+      </c>
+      <c r="O35" s="112">
+        <v>5</v>
+      </c>
+      <c r="P35" s="112">
+        <v>9</v>
       </c>
       <c r="Q35" s="50">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R35" s="51">
-        <f t="shared" si="4"/>
-        <v>6.5</v>
+        <f>SUM(K35:Q35)/6</f>
+        <v>7.333333333333333</v>
       </c>
       <c r="S35" s="50">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T35" s="104">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="32">
         <v>9</v>
       </c>
@@ -5135,20 +5161,24 @@
         <v>6</v>
       </c>
       <c r="P36" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q36" s="4">
         <v>9</v>
       </c>
       <c r="R36" s="34">
-        <f t="shared" si="4"/>
-        <v>5.666666666666667</v>
+        <f>SUM(K36:Q36)/6</f>
+        <v>6</v>
       </c>
       <c r="S36" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T36" s="104">
+        <f>F36+G36</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="59">
         <v>10</v>
       </c>
@@ -5192,23 +5222,27 @@
         <v>2</v>
       </c>
       <c r="O37" s="61">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P37" s="61">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q37" s="65">
         <v>6</v>
       </c>
       <c r="R37" s="71">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f>SUM(K37:Q37)/6</f>
+        <v>4.166666666666667</v>
       </c>
       <c r="S37" s="69">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T37" s="104">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>67</v>
       </c>
@@ -5246,27 +5280,27 @@
   <sheetData>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="107" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="109"/>
+      <c r="C3" s="108" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="110"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="107" t="s">
+      <c r="K3" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="108"/>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108"/>
-      <c r="S3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="110"/>
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Summary Updates to InDesign models and resource files Actions: FIX engine bug related to travel squares
Problems
</commit_message>
<xml_diff>
--- a/docs/edition_points.xlsx
+++ b/docs/edition_points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Compile\careers\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A54710-AEB2-438B-A7E7-E1EA00740406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A35BE78-5486-4E28-9DEC-86DFDA6BC898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="1305" windowWidth="23580" windowHeight="13110" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30180" yWindow="1425" windowWidth="26640" windowHeight="13110" tabRatio="535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hi-Tech Jobs" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="105">
   <si>
     <t>Occupation</t>
   </si>
@@ -333,6 +333,30 @@
   </si>
   <si>
     <t>Points + Salary</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>occupation squares</t>
+  </si>
+  <si>
+    <t>border squares</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>college squares</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Entrance Fee</t>
+  </si>
+  <si>
+    <t>Cost per point</t>
   </si>
 </sst>
 </file>
@@ -343,7 +367,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,6 +405,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -396,7 +427,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -521,13 +552,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -814,6 +860,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -821,33 +889,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1157,27 +1198,27 @@
   <sheetData>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="108" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="109"/>
-      <c r="I3" s="110"/>
+      <c r="C3" s="118" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="119"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="120"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="108" t="s">
+      <c r="K3" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="109"/>
-      <c r="M3" s="109"/>
-      <c r="N3" s="109"/>
-      <c r="O3" s="109"/>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="109"/>
-      <c r="R3" s="109"/>
-      <c r="S3" s="110"/>
+      <c r="L3" s="119"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="119"/>
+      <c r="P3" s="119"/>
+      <c r="Q3" s="119"/>
+      <c r="R3" s="119"/>
+      <c r="S3" s="120"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -2101,53 +2142,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2731D533-3189-49BB-AE83-771387574D8F}">
-  <dimension ref="A3:T52"/>
+  <dimension ref="A3:W52"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" customWidth="1"/>
+    <col min="14" max="14" width="8" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" customWidth="1"/>
     <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.140625" style="1"/>
+    <col min="22" max="22" width="11.5703125" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="108" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="109"/>
-      <c r="I3" s="110"/>
+      <c r="C3" s="118" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="119"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="120"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="108" t="s">
+      <c r="K3" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="109"/>
-      <c r="M3" s="109"/>
-      <c r="N3" s="109"/>
-      <c r="O3" s="109"/>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="109"/>
-      <c r="R3" s="109"/>
-      <c r="S3" s="110"/>
-    </row>
-    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="L3" s="119"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="119"/>
+      <c r="P3" s="119"/>
+      <c r="Q3" s="119"/>
+      <c r="R3" s="119"/>
+      <c r="S3" s="120"/>
+    </row>
+    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>49</v>
       </c>
@@ -2205,11 +2253,20 @@
       <c r="S4" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T4" s="111" t="s">
+        <v>85</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="V4" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="W4" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="32">
         <v>1</v>
       </c>
@@ -2228,7 +2285,7 @@
       <c r="F5" s="29">
         <v>91</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="77">
         <v>2</v>
       </c>
       <c r="H5" s="1">
@@ -2272,8 +2329,18 @@
         <f>SUM(K5:Q5)</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5" s="4">
+        <v>15</v>
+      </c>
+      <c r="V5" s="106">
+        <v>5000</v>
+      </c>
+      <c r="W5" s="113">
+        <f>V5/F5</f>
+        <v>54.945054945054942</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="41">
         <v>2</v>
       </c>
@@ -2292,7 +2359,7 @@
       <c r="F6" s="44">
         <v>42</v>
       </c>
-      <c r="G6" s="45">
+      <c r="G6" s="72">
         <v>2</v>
       </c>
       <c r="H6" s="43">
@@ -2332,12 +2399,22 @@
       <c r="S6" s="50">
         <v>6</v>
       </c>
-      <c r="T6" s="1">
+      <c r="T6" s="49">
         <f t="shared" ref="T6:T14" si="1">SUM(K6:Q6)</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6" s="50">
+        <v>14</v>
+      </c>
+      <c r="V6" s="112">
+        <v>1000</v>
+      </c>
+      <c r="W6" s="114">
+        <f t="shared" ref="W6:W14" si="2">V6/F6</f>
+        <v>23.80952380952381</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="32">
         <v>3</v>
       </c>
@@ -2356,7 +2433,7 @@
       <c r="F7" s="29">
         <v>24</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="77">
         <v>2</v>
       </c>
       <c r="H7" s="1">
@@ -2400,8 +2477,18 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7" s="4">
+        <v>11</v>
+      </c>
+      <c r="V7" s="106">
+        <v>500</v>
+      </c>
+      <c r="W7" s="113">
+        <f t="shared" si="2"/>
+        <v>20.833333333333332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="41">
         <v>4</v>
       </c>
@@ -2420,7 +2507,7 @@
       <c r="F8" s="44">
         <v>19</v>
       </c>
-      <c r="G8" s="45">
+      <c r="G8" s="72">
         <v>8</v>
       </c>
       <c r="H8" s="43">
@@ -2460,12 +2547,22 @@
       <c r="S8" s="50">
         <v>10</v>
       </c>
-      <c r="T8" s="1">
+      <c r="T8" s="49">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8" s="50">
+        <v>13</v>
+      </c>
+      <c r="V8" s="112">
+        <v>1000</v>
+      </c>
+      <c r="W8" s="114">
+        <f t="shared" si="2"/>
+        <v>52.631578947368418</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="32">
         <v>5</v>
       </c>
@@ -2484,7 +2581,7 @@
       <c r="F9" s="14">
         <v>34</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="73">
         <v>5</v>
       </c>
       <c r="H9" s="5">
@@ -2528,8 +2625,18 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="4">
+        <v>11</v>
+      </c>
+      <c r="V9" s="106">
+        <v>500</v>
+      </c>
+      <c r="W9" s="113">
+        <f t="shared" si="2"/>
+        <v>14.705882352941176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="41">
         <v>6</v>
       </c>
@@ -2548,7 +2655,7 @@
       <c r="F10" s="44">
         <v>28</v>
       </c>
-      <c r="G10" s="70">
+      <c r="G10" s="74">
         <v>2</v>
       </c>
       <c r="H10" s="49">
@@ -2588,12 +2695,22 @@
       <c r="S10" s="50">
         <v>8</v>
       </c>
-      <c r="T10" s="1">
+      <c r="T10" s="49">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="50">
+        <v>12</v>
+      </c>
+      <c r="V10" s="112">
+        <v>1000</v>
+      </c>
+      <c r="W10" s="114">
+        <f t="shared" si="2"/>
+        <v>35.714285714285715</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="32">
         <v>7</v>
       </c>
@@ -2612,7 +2729,7 @@
       <c r="F11" s="29">
         <v>49</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="77">
         <v>6</v>
       </c>
       <c r="H11" s="1">
@@ -2656,8 +2773,18 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="4">
+        <v>12</v>
+      </c>
+      <c r="V11" s="106">
+        <v>5000</v>
+      </c>
+      <c r="W11" s="113">
+        <f>V11/F11</f>
+        <v>102.04081632653062</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="41">
         <v>8</v>
       </c>
@@ -2676,7 +2803,7 @@
       <c r="F12" s="44">
         <v>42</v>
       </c>
-      <c r="G12" s="57">
+      <c r="G12" s="76">
         <v>5</v>
       </c>
       <c r="H12" s="43">
@@ -2716,12 +2843,22 @@
       <c r="S12" s="4">
         <v>5</v>
       </c>
-      <c r="T12" s="1">
+      <c r="T12" s="49">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12" s="50">
+        <v>11</v>
+      </c>
+      <c r="V12" s="112">
+        <v>500</v>
+      </c>
+      <c r="W12" s="114">
+        <f t="shared" si="2"/>
+        <v>11.904761904761905</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="32">
         <v>9</v>
       </c>
@@ -2740,7 +2877,7 @@
       <c r="F13" s="14">
         <v>66</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="75">
         <v>6</v>
       </c>
       <c r="H13" s="1">
@@ -2784,8 +2921,18 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" s="4">
+        <v>14</v>
+      </c>
+      <c r="V13" s="106">
+        <v>4000</v>
+      </c>
+      <c r="W13" s="113">
+        <f t="shared" si="2"/>
+        <v>60.606060606060609</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="59">
         <v>10</v>
       </c>
@@ -2804,7 +2951,7 @@
       <c r="F14" s="63">
         <v>70</v>
       </c>
-      <c r="G14" s="64">
+      <c r="G14" s="78">
         <v>4</v>
       </c>
       <c r="H14" s="61">
@@ -2844,23 +2991,33 @@
       <c r="S14" s="69">
         <v>2</v>
       </c>
-      <c r="T14" s="1">
+      <c r="T14" s="67">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14" s="65">
+        <v>19</v>
+      </c>
+      <c r="V14" s="69">
+        <v>8000</v>
+      </c>
+      <c r="W14" s="115">
+        <f t="shared" si="2"/>
+        <v>114.28571428571429</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
       <c r="C15" s="1">
         <f>SUM(C5:C14)</f>
         <v>205</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" ref="D15:I15" si="2">SUM(D5:D14)</f>
+        <f t="shared" ref="D15:I15" si="3">SUM(D5:D14)</f>
         <v>176</v>
       </c>
       <c r="E15" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>84</v>
       </c>
       <c r="F15" s="16">
@@ -2868,20 +3025,57 @@
         <v>465</v>
       </c>
       <c r="G15" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="J15" s="23"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15" s="116" t="s">
+        <v>98</v>
+      </c>
+      <c r="U15" s="1">
+        <f>SUM(U5:U6)+SUM(U8:U14)</f>
+        <v>121</v>
+      </c>
+      <c r="V15">
+        <f>AVERAGE(V5:V14)</f>
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T16" s="116" t="s">
+        <v>101</v>
+      </c>
+      <c r="U16" s="1">
+        <f>U7</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T17" s="116" t="s">
+        <v>100</v>
+      </c>
+      <c r="U17" s="1">
+        <f>U15+U16</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T18" s="116" t="s">
+        <v>99</v>
+      </c>
+      <c r="U18" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="37" t="s">
         <v>47</v>
       </c>
@@ -2891,8 +3085,15 @@
       <c r="G19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="116" t="s">
+        <v>102</v>
+      </c>
+      <c r="U19" s="110">
+        <f>U17+U18</f>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B20" s="37" t="s">
         <v>46</v>
       </c>
@@ -2903,7 +3104,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B21" s="37" t="s">
         <v>45</v>
       </c>
@@ -2914,7 +3115,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B22" s="37" t="s">
         <v>48</v>
       </c>
@@ -2925,7 +3126,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B23" s="37" t="s">
         <v>9</v>
       </c>
@@ -2936,7 +3137,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B24" s="38" t="s">
         <v>8</v>
       </c>
@@ -2947,41 +3148,41 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="39" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C29" s="108" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="109"/>
-      <c r="E29" s="109"/>
-      <c r="F29" s="109"/>
-      <c r="G29" s="109"/>
-      <c r="H29" s="109"/>
-      <c r="I29" s="110"/>
+    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C29" s="118" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="119"/>
+      <c r="E29" s="119"/>
+      <c r="F29" s="119"/>
+      <c r="G29" s="119"/>
+      <c r="H29" s="119"/>
+      <c r="I29" s="120"/>
       <c r="J29" s="18"/>
-      <c r="K29" s="108" t="s">
+      <c r="K29" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="L29" s="109"/>
-      <c r="M29" s="109"/>
-      <c r="N29" s="109"/>
-      <c r="O29" s="109"/>
-      <c r="P29" s="109"/>
-      <c r="Q29" s="109"/>
-      <c r="R29" s="109"/>
-      <c r="S29" s="110"/>
-    </row>
-    <row r="30" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="L29" s="119"/>
+      <c r="M29" s="119"/>
+      <c r="N29" s="119"/>
+      <c r="O29" s="119"/>
+      <c r="P29" s="119"/>
+      <c r="Q29" s="119"/>
+      <c r="R29" s="119"/>
+      <c r="S29" s="120"/>
+    </row>
+    <row r="30" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
         <v>49</v>
       </c>
@@ -3040,7 +3241,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="32">
         <v>1</v>
       </c>
@@ -3093,14 +3294,14 @@
         <v>10</v>
       </c>
       <c r="R31" s="34">
-        <f t="shared" ref="R31:R40" si="3">(O31+SUM(K31:M31))/4</f>
+        <f t="shared" ref="R31:R40" si="4">(O31+SUM(K31:M31))/4</f>
         <v>2.75</v>
       </c>
       <c r="S31" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="41">
         <v>2</v>
       </c>
@@ -3153,7 +3354,7 @@
         <v>9</v>
       </c>
       <c r="R32" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.25</v>
       </c>
       <c r="S32" s="50">
@@ -3213,7 +3414,7 @@
         <v>1</v>
       </c>
       <c r="R33" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.75</v>
       </c>
       <c r="S33" s="4">
@@ -3273,7 +3474,7 @@
         <v>2</v>
       </c>
       <c r="R34" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.5</v>
       </c>
       <c r="S34" s="50">
@@ -3333,7 +3534,7 @@
         <v>7</v>
       </c>
       <c r="R35" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.75</v>
       </c>
       <c r="S35" s="4">
@@ -3393,7 +3594,7 @@
         <v>5</v>
       </c>
       <c r="R36" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="S36" s="50">
@@ -3453,7 +3654,7 @@
         <v>4</v>
       </c>
       <c r="R37" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="S37" s="50">
@@ -3513,7 +3714,7 @@
         <v>6</v>
       </c>
       <c r="R38" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.5</v>
       </c>
       <c r="S38" s="4">
@@ -3573,7 +3774,7 @@
         <v>3</v>
       </c>
       <c r="R39" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.75</v>
       </c>
       <c r="S39" s="4">
@@ -3633,7 +3834,7 @@
         <v>8</v>
       </c>
       <c r="R40" s="71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.75</v>
       </c>
       <c r="S40" s="69">
@@ -3690,51 +3891,62 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66559D5-1C3E-471D-81A3-258D37D68792}">
-  <dimension ref="A3:T39"/>
+  <dimension ref="A3:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="8" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.140625" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
+    <col min="22" max="22" width="9.85546875" customWidth="1"/>
+    <col min="23" max="23" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="108" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="109"/>
-      <c r="I3" s="110"/>
+      <c r="C3" s="118" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="119"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="120"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="108" t="s">
+      <c r="K3" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="109"/>
-      <c r="M3" s="109"/>
-      <c r="N3" s="109"/>
-      <c r="O3" s="109"/>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="109"/>
-      <c r="R3" s="109"/>
-      <c r="S3" s="110"/>
-      <c r="T3" s="1"/>
-    </row>
-    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="L3" s="119"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="119"/>
+      <c r="P3" s="119"/>
+      <c r="Q3" s="119"/>
+      <c r="R3" s="119"/>
+      <c r="S3" s="120"/>
+      <c r="T3" s="108"/>
+      <c r="U3" s="109"/>
+      <c r="V3" s="109"/>
+      <c r="W3" s="109"/>
+    </row>
+    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>49</v>
       </c>
@@ -3792,21 +4004,30 @@
       <c r="S4" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T4" s="111" t="s">
+        <v>85</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="V4" s="117" t="s">
+        <v>103</v>
+      </c>
+      <c r="W4" s="117" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="32">
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="116">
+      <c r="C5" s="1">
         <v>38</v>
       </c>
-      <c r="D5" s="115">
+      <c r="D5" s="32">
         <v>18</v>
       </c>
       <c r="E5" s="29">
@@ -3815,10 +4036,10 @@
       <c r="F5" s="29">
         <v>71</v>
       </c>
-      <c r="G5" s="115">
-        <v>2</v>
-      </c>
-      <c r="H5" s="115">
+      <c r="G5" s="32">
+        <v>2</v>
+      </c>
+      <c r="H5" s="32">
         <v>2</v>
       </c>
       <c r="I5" s="84">
@@ -3830,19 +4051,19 @@
       <c r="K5" s="36">
         <v>1</v>
       </c>
-      <c r="L5" s="116">
-        <v>5</v>
-      </c>
-      <c r="M5" s="116">
-        <v>2</v>
-      </c>
-      <c r="N5" s="116">
-        <v>1</v>
-      </c>
-      <c r="O5" s="116">
-        <v>7</v>
-      </c>
-      <c r="P5" s="116">
+      <c r="L5" s="1">
+        <v>5</v>
+      </c>
+      <c r="M5" s="1">
+        <v>2</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>7</v>
+      </c>
+      <c r="P5" s="1">
         <v>8</v>
       </c>
       <c r="Q5" s="4">
@@ -3858,18 +4079,28 @@
         <f>SUM(K5:Q5)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5" s="4">
+        <v>13</v>
+      </c>
+      <c r="V5" s="106">
+        <v>5000</v>
+      </c>
+      <c r="W5" s="113">
+        <f>V5/F5</f>
+        <v>70.422535211267601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="41">
         <v>2</v>
       </c>
       <c r="B6" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="113">
-        <v>8</v>
-      </c>
-      <c r="D6" s="114">
+      <c r="C6" s="43">
+        <v>8</v>
+      </c>
+      <c r="D6" s="79">
         <v>21</v>
       </c>
       <c r="E6" s="44">
@@ -3878,10 +4109,10 @@
       <c r="F6" s="44">
         <v>37</v>
       </c>
-      <c r="G6" s="114">
-        <v>1</v>
-      </c>
-      <c r="H6" s="114">
+      <c r="G6" s="79">
+        <v>1</v>
+      </c>
+      <c r="H6" s="79">
         <v>1</v>
       </c>
       <c r="I6" s="81">
@@ -3893,19 +4124,19 @@
       <c r="K6" s="48">
         <v>7</v>
       </c>
-      <c r="L6" s="112">
-        <v>3</v>
-      </c>
-      <c r="M6" s="112">
-        <v>5</v>
-      </c>
-      <c r="N6" s="112">
-        <v>6</v>
-      </c>
-      <c r="O6" s="112">
+      <c r="L6" s="49">
+        <v>3</v>
+      </c>
+      <c r="M6" s="49">
+        <v>5</v>
+      </c>
+      <c r="N6" s="49">
+        <v>6</v>
+      </c>
+      <c r="O6" s="49">
         <v>9</v>
       </c>
-      <c r="P6" s="112">
+      <c r="P6" s="49">
         <v>10</v>
       </c>
       <c r="Q6" s="50">
@@ -3917,22 +4148,32 @@
       <c r="S6" s="50">
         <v>6</v>
       </c>
-      <c r="T6" s="1">
+      <c r="T6" s="49">
         <f t="shared" ref="T6:T14" si="0">SUM(K6:Q6)</f>
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6" s="50">
+        <v>12</v>
+      </c>
+      <c r="V6" s="112">
+        <v>1000</v>
+      </c>
+      <c r="W6" s="114">
+        <f t="shared" ref="W6:W14" si="1">V6/F6</f>
+        <v>27.027027027027028</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="32">
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="116">
+      <c r="C7" s="1">
         <v>12</v>
       </c>
-      <c r="D7" s="115">
+      <c r="D7" s="32">
         <v>12</v>
       </c>
       <c r="E7" s="29">
@@ -3941,10 +4182,10 @@
       <c r="F7" s="29">
         <v>24</v>
       </c>
-      <c r="G7" s="115">
-        <v>2</v>
-      </c>
-      <c r="H7" s="115">
+      <c r="G7" s="32">
+        <v>2</v>
+      </c>
+      <c r="H7" s="32">
         <v>2</v>
       </c>
       <c r="I7" s="83">
@@ -3956,19 +4197,19 @@
       <c r="K7" s="35">
         <v>5</v>
       </c>
-      <c r="L7" s="116">
-        <v>7</v>
-      </c>
-      <c r="M7" s="116">
-        <v>10</v>
-      </c>
-      <c r="N7" s="116">
+      <c r="L7" s="1">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1">
+        <v>10</v>
+      </c>
+      <c r="N7" s="1">
         <v>9</v>
       </c>
-      <c r="O7" s="116">
-        <v>8</v>
-      </c>
-      <c r="P7" s="116">
+      <c r="O7" s="1">
+        <v>8</v>
+      </c>
+      <c r="P7" s="1">
         <v>2</v>
       </c>
       <c r="Q7" s="4">
@@ -3984,18 +4225,28 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7" s="4">
+        <v>11</v>
+      </c>
+      <c r="V7" s="106">
+        <v>500</v>
+      </c>
+      <c r="W7" s="113">
+        <f t="shared" si="1"/>
+        <v>20.833333333333332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="41">
         <v>4</v>
       </c>
       <c r="B8" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="113">
-        <v>4</v>
-      </c>
-      <c r="D8" s="114">
+      <c r="C8" s="43">
+        <v>4</v>
+      </c>
+      <c r="D8" s="79">
         <v>12</v>
       </c>
       <c r="E8" s="44">
@@ -4007,7 +4258,7 @@
       <c r="G8" s="56">
         <v>8</v>
       </c>
-      <c r="H8" s="114">
+      <c r="H8" s="79">
         <v>3</v>
       </c>
       <c r="I8" s="81">
@@ -4019,19 +4270,19 @@
       <c r="K8" s="48">
         <v>9</v>
       </c>
-      <c r="L8" s="112">
-        <v>8</v>
-      </c>
-      <c r="M8" s="112">
-        <v>8</v>
-      </c>
-      <c r="N8" s="112">
-        <v>10</v>
-      </c>
-      <c r="O8" s="112">
-        <v>1</v>
-      </c>
-      <c r="P8" s="112">
+      <c r="L8" s="49">
+        <v>8</v>
+      </c>
+      <c r="M8" s="49">
+        <v>8</v>
+      </c>
+      <c r="N8" s="49">
+        <v>10</v>
+      </c>
+      <c r="O8" s="49">
+        <v>1</v>
+      </c>
+      <c r="P8" s="49">
         <v>1</v>
       </c>
       <c r="Q8" s="50">
@@ -4043,12 +4294,22 @@
       <c r="S8" s="50">
         <v>9</v>
       </c>
-      <c r="T8" s="1">
+      <c r="T8" s="49">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8" s="50">
+        <v>13</v>
+      </c>
+      <c r="V8" s="112">
+        <v>1000</v>
+      </c>
+      <c r="W8" s="114">
+        <f t="shared" si="1"/>
+        <v>52.631578947368418</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="32">
         <v>5</v>
       </c>
@@ -4110,18 +4371,28 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="4">
+        <v>11</v>
+      </c>
+      <c r="V9" s="106">
+        <v>500</v>
+      </c>
+      <c r="W9" s="113">
+        <f>V9/F9</f>
+        <v>17.857142857142858</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="41">
         <v>6</v>
       </c>
       <c r="B10" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="112">
-        <v>2</v>
-      </c>
-      <c r="D10" s="111">
+      <c r="C10" s="49">
+        <v>2</v>
+      </c>
+      <c r="D10" s="41">
         <v>23</v>
       </c>
       <c r="E10" s="56">
@@ -4133,7 +4404,7 @@
       <c r="G10" s="85">
         <v>0</v>
       </c>
-      <c r="H10" s="111">
+      <c r="H10" s="41">
         <v>2</v>
       </c>
       <c r="I10" s="86">
@@ -4145,19 +4416,19 @@
       <c r="K10" s="48">
         <v>10</v>
       </c>
-      <c r="L10" s="112">
-        <v>2</v>
-      </c>
-      <c r="M10" s="112">
+      <c r="L10" s="49">
+        <v>2</v>
+      </c>
+      <c r="M10" s="49">
         <v>9</v>
       </c>
-      <c r="N10" s="112">
-        <v>8</v>
-      </c>
-      <c r="O10" s="112">
-        <v>10</v>
-      </c>
-      <c r="P10" s="112">
+      <c r="N10" s="49">
+        <v>8</v>
+      </c>
+      <c r="O10" s="49">
+        <v>10</v>
+      </c>
+      <c r="P10" s="49">
         <v>4</v>
       </c>
       <c r="Q10" s="50">
@@ -4169,12 +4440,22 @@
       <c r="S10" s="50">
         <v>8</v>
       </c>
-      <c r="T10" s="1">
+      <c r="T10" s="49">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="50">
+        <v>12</v>
+      </c>
+      <c r="V10" s="112">
+        <v>500</v>
+      </c>
+      <c r="W10" s="114">
+        <f t="shared" si="1"/>
+        <v>17.857142857142858</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="32">
         <v>7</v>
       </c>
@@ -4226,28 +4507,38 @@
       <c r="Q11" s="4">
         <v>3</v>
       </c>
-      <c r="R11" s="118">
+      <c r="R11" s="34">
         <v>4.833333333333333</v>
       </c>
-      <c r="S11" s="119">
+      <c r="S11" s="4">
         <v>4</v>
       </c>
       <c r="T11" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="4">
+        <v>12</v>
+      </c>
+      <c r="V11" s="106">
+        <v>3000</v>
+      </c>
+      <c r="W11" s="113">
+        <f>V11/F11</f>
+        <v>68.181818181818187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="41">
         <v>8</v>
       </c>
       <c r="B12" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="113">
+      <c r="C12" s="43">
         <v>28</v>
       </c>
-      <c r="D12" s="114">
+      <c r="D12" s="79">
         <v>6</v>
       </c>
       <c r="E12" s="56">
@@ -4259,7 +4550,7 @@
       <c r="G12" s="44">
         <v>4</v>
       </c>
-      <c r="H12" s="114">
+      <c r="H12" s="79">
         <v>1</v>
       </c>
       <c r="I12" s="81">
@@ -4271,19 +4562,19 @@
       <c r="K12" s="48">
         <v>3</v>
       </c>
-      <c r="L12" s="112">
-        <v>10</v>
-      </c>
-      <c r="M12" s="112">
-        <v>7</v>
-      </c>
-      <c r="N12" s="112">
-        <v>5</v>
-      </c>
-      <c r="O12" s="112">
-        <v>5</v>
-      </c>
-      <c r="P12" s="112">
+      <c r="L12" s="49">
+        <v>10</v>
+      </c>
+      <c r="M12" s="49">
+        <v>7</v>
+      </c>
+      <c r="N12" s="49">
+        <v>5</v>
+      </c>
+      <c r="O12" s="49">
+        <v>5</v>
+      </c>
+      <c r="P12" s="49">
         <v>9</v>
       </c>
       <c r="Q12" s="50">
@@ -4295,12 +4586,22 @@
       <c r="S12" s="50">
         <v>5</v>
       </c>
-      <c r="T12" s="1">
+      <c r="T12" s="49">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12" s="50">
+        <v>11</v>
+      </c>
+      <c r="V12" s="112">
+        <v>1000</v>
+      </c>
+      <c r="W12" s="114">
+        <f t="shared" si="1"/>
+        <v>26.315789473684209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="32">
         <v>9</v>
       </c>
@@ -4362,8 +4663,18 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" s="4">
+        <v>14</v>
+      </c>
+      <c r="V13" s="106">
+        <v>4000</v>
+      </c>
+      <c r="W13" s="113">
+        <f t="shared" si="1"/>
+        <v>66.666666666666671</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="59">
         <v>10</v>
       </c>
@@ -4421,49 +4732,96 @@
       <c r="S14" s="69">
         <v>2</v>
       </c>
-      <c r="T14" s="1">
+      <c r="T14" s="67">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14" s="65">
+        <v>19</v>
+      </c>
+      <c r="V14" s="69">
+        <v>5000</v>
+      </c>
+      <c r="W14" s="115">
+        <f t="shared" si="1"/>
+        <v>78.125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B15" s="39" t="s">
         <v>65</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:J15" si="1">SUM(C5:C14)</f>
+        <f t="shared" ref="C15:J15" si="2">SUM(C5:C14)</f>
         <v>154</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>174</v>
       </c>
       <c r="E15" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="F15" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>413</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="J15" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T15" s="116" t="s">
+        <v>98</v>
+      </c>
+      <c r="U15" s="1">
+        <f>SUM(U5:U6)+SUM(U8:U14)</f>
+        <v>117</v>
+      </c>
+      <c r="V15">
+        <f>AVERAGE(V5:V14)</f>
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T16" s="116" t="s">
+        <v>101</v>
+      </c>
+      <c r="U16" s="1">
+        <f>U7</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T17" s="116" t="s">
+        <v>100</v>
+      </c>
+      <c r="U17" s="1">
+        <f>U15+U16</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T18" s="116" t="s">
+        <v>99</v>
+      </c>
+      <c r="U18" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="37" t="s">
         <v>47</v>
       </c>
@@ -4473,8 +4831,15 @@
       <c r="G19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T19" s="116" t="s">
+        <v>102</v>
+      </c>
+      <c r="U19" s="110">
+        <f>U17+U18</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B20" s="37" t="s">
         <v>46</v>
       </c>
@@ -4485,7 +4850,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B21" s="37" t="s">
         <v>45</v>
       </c>
@@ -4496,7 +4861,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B22" s="37" t="s">
         <v>48</v>
       </c>
@@ -4507,7 +4872,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B23" s="37" t="s">
         <v>9</v>
       </c>
@@ -4518,7 +4883,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B24" s="38" t="s">
         <v>8</v>
       </c>
@@ -4529,7 +4894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B25" s="37" t="s">
         <v>10</v>
       </c>
@@ -4540,7 +4905,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>49</v>
       </c>
@@ -4598,21 +4963,21 @@
       <c r="S27" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="T27" s="117" t="s">
+      <c r="T27" s="28" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="115">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="32">
         <v>1</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="116">
+      <c r="C28" s="1">
         <v>38</v>
       </c>
-      <c r="D28" s="115">
+      <c r="D28" s="32">
         <v>18</v>
       </c>
       <c r="E28" s="29">
@@ -4621,10 +4986,10 @@
       <c r="F28" s="29">
         <v>71</v>
       </c>
-      <c r="G28" s="115">
-        <v>2</v>
-      </c>
-      <c r="H28" s="115">
+      <c r="G28" s="32">
+        <v>2</v>
+      </c>
+      <c r="H28" s="32">
         <v>2</v>
       </c>
       <c r="I28" s="84">
@@ -4636,26 +5001,26 @@
       <c r="K28" s="36">
         <v>1</v>
       </c>
-      <c r="L28" s="116">
-        <v>5</v>
-      </c>
-      <c r="M28" s="116">
-        <v>2</v>
-      </c>
-      <c r="N28" s="116">
-        <v>1</v>
-      </c>
-      <c r="O28" s="116">
-        <v>7</v>
-      </c>
-      <c r="P28" s="116">
+      <c r="L28" s="1">
+        <v>5</v>
+      </c>
+      <c r="M28" s="1">
+        <v>2</v>
+      </c>
+      <c r="N28" s="1">
+        <v>1</v>
+      </c>
+      <c r="O28" s="1">
+        <v>7</v>
+      </c>
+      <c r="P28" s="1">
         <v>8</v>
       </c>
       <c r="Q28" s="4">
         <v>10</v>
       </c>
       <c r="R28" s="34">
-        <f>SUM(K28:Q28)/6</f>
+        <f t="shared" ref="R28:R37" si="3">SUM(K28:Q28)/6</f>
         <v>5.666666666666667</v>
       </c>
       <c r="S28" s="4">
@@ -4666,17 +5031,17 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="111">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="41">
         <v>2</v>
       </c>
       <c r="B29" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="113">
-        <v>8</v>
-      </c>
-      <c r="D29" s="114">
+      <c r="C29" s="43">
+        <v>8</v>
+      </c>
+      <c r="D29" s="79">
         <v>21</v>
       </c>
       <c r="E29" s="44">
@@ -4685,10 +5050,10 @@
       <c r="F29" s="44">
         <v>37</v>
       </c>
-      <c r="G29" s="114">
-        <v>1</v>
-      </c>
-      <c r="H29" s="114">
+      <c r="G29" s="79">
+        <v>1</v>
+      </c>
+      <c r="H29" s="79">
         <v>1</v>
       </c>
       <c r="I29" s="81">
@@ -4700,47 +5065,47 @@
       <c r="K29" s="48">
         <v>7</v>
       </c>
-      <c r="L29" s="112">
-        <v>3</v>
-      </c>
-      <c r="M29" s="112">
-        <v>5</v>
-      </c>
-      <c r="N29" s="112">
-        <v>6</v>
-      </c>
-      <c r="O29" s="112">
+      <c r="L29" s="49">
+        <v>3</v>
+      </c>
+      <c r="M29" s="49">
+        <v>5</v>
+      </c>
+      <c r="N29" s="49">
+        <v>6</v>
+      </c>
+      <c r="O29" s="49">
         <v>9</v>
       </c>
-      <c r="P29" s="112">
+      <c r="P29" s="49">
         <v>10</v>
       </c>
       <c r="Q29" s="50">
         <v>8</v>
       </c>
       <c r="R29" s="51">
-        <f>SUM(K29:Q29)/6</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="S29" s="50">
         <v>6</v>
       </c>
       <c r="T29" s="104">
-        <f t="shared" ref="T29:T37" si="2">F29+G29</f>
+        <f t="shared" ref="T29:T37" si="4">F29+G29</f>
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="115">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="32">
         <v>3</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="116">
+      <c r="C30" s="1">
         <v>12</v>
       </c>
-      <c r="D30" s="115">
+      <c r="D30" s="32">
         <v>12</v>
       </c>
       <c r="E30" s="29">
@@ -4749,10 +5114,10 @@
       <c r="F30" s="29">
         <v>24</v>
       </c>
-      <c r="G30" s="115">
-        <v>2</v>
-      </c>
-      <c r="H30" s="115">
+      <c r="G30" s="32">
+        <v>2</v>
+      </c>
+      <c r="H30" s="32">
         <v>2</v>
       </c>
       <c r="I30" s="83">
@@ -4764,47 +5129,47 @@
       <c r="K30" s="35">
         <v>5</v>
       </c>
-      <c r="L30" s="116">
-        <v>7</v>
-      </c>
-      <c r="M30" s="116">
-        <v>10</v>
-      </c>
-      <c r="N30" s="116">
+      <c r="L30" s="1">
+        <v>7</v>
+      </c>
+      <c r="M30" s="1">
+        <v>10</v>
+      </c>
+      <c r="N30" s="1">
         <v>9</v>
       </c>
-      <c r="O30" s="116">
-        <v>8</v>
-      </c>
-      <c r="P30" s="116">
+      <c r="O30" s="1">
+        <v>8</v>
+      </c>
+      <c r="P30" s="1">
         <v>2</v>
       </c>
       <c r="Q30" s="4">
         <v>1</v>
       </c>
       <c r="R30" s="34">
-        <f>SUM(K30:Q30)/6</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="S30" s="4">
         <v>10</v>
       </c>
       <c r="T30" s="104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="111">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="41">
         <v>4</v>
       </c>
       <c r="B31" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="113">
-        <v>4</v>
-      </c>
-      <c r="D31" s="114">
+      <c r="C31" s="43">
+        <v>4</v>
+      </c>
+      <c r="D31" s="79">
         <v>12</v>
       </c>
       <c r="E31" s="44">
@@ -4816,7 +5181,7 @@
       <c r="G31" s="56">
         <v>8</v>
       </c>
-      <c r="H31" s="114">
+      <c r="H31" s="79">
         <v>3</v>
       </c>
       <c r="I31" s="81">
@@ -4828,37 +5193,37 @@
       <c r="K31" s="48">
         <v>9</v>
       </c>
-      <c r="L31" s="112">
-        <v>8</v>
-      </c>
-      <c r="M31" s="112">
-        <v>8</v>
-      </c>
-      <c r="N31" s="112">
-        <v>10</v>
-      </c>
-      <c r="O31" s="112">
-        <v>1</v>
-      </c>
-      <c r="P31" s="112">
+      <c r="L31" s="49">
+        <v>8</v>
+      </c>
+      <c r="M31" s="49">
+        <v>8</v>
+      </c>
+      <c r="N31" s="49">
+        <v>10</v>
+      </c>
+      <c r="O31" s="49">
+        <v>1</v>
+      </c>
+      <c r="P31" s="49">
         <v>1</v>
       </c>
       <c r="Q31" s="50">
         <v>2</v>
       </c>
       <c r="R31" s="51">
-        <f>SUM(K31:Q31)/6</f>
+        <f t="shared" si="3"/>
         <v>6.5</v>
       </c>
       <c r="S31" s="50">
         <v>9</v>
       </c>
       <c r="T31" s="104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="32">
         <v>5</v>
       </c>
@@ -4911,28 +5276,28 @@
         <v>7</v>
       </c>
       <c r="R32" s="34">
-        <f>SUM(K32:Q32)/6</f>
+        <f t="shared" si="3"/>
         <v>6.833333333333333</v>
       </c>
       <c r="S32" s="4">
         <v>7</v>
       </c>
       <c r="T32" s="104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="111">
+      <c r="A33" s="41">
         <v>6</v>
       </c>
       <c r="B33" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="112">
-        <v>2</v>
-      </c>
-      <c r="D33" s="111">
+      <c r="C33" s="49">
+        <v>2</v>
+      </c>
+      <c r="D33" s="41">
         <v>23</v>
       </c>
       <c r="E33" s="56">
@@ -4944,7 +5309,7 @@
       <c r="G33" s="85">
         <v>0</v>
       </c>
-      <c r="H33" s="111">
+      <c r="H33" s="41">
         <v>2</v>
       </c>
       <c r="I33" s="86">
@@ -4956,33 +5321,33 @@
       <c r="K33" s="48">
         <v>10</v>
       </c>
-      <c r="L33" s="112">
-        <v>2</v>
-      </c>
-      <c r="M33" s="112">
+      <c r="L33" s="49">
+        <v>2</v>
+      </c>
+      <c r="M33" s="49">
         <v>9</v>
       </c>
-      <c r="N33" s="112">
-        <v>8</v>
-      </c>
-      <c r="O33" s="112">
-        <v>10</v>
-      </c>
-      <c r="P33" s="112">
+      <c r="N33" s="49">
+        <v>8</v>
+      </c>
+      <c r="O33" s="49">
+        <v>10</v>
+      </c>
+      <c r="P33" s="49">
         <v>4</v>
       </c>
       <c r="Q33" s="50">
         <v>4</v>
       </c>
       <c r="R33" s="51">
-        <f>SUM(K33:Q33)/6</f>
+        <f t="shared" si="3"/>
         <v>7.833333333333333</v>
       </c>
       <c r="S33" s="50">
         <v>8</v>
       </c>
       <c r="T33" s="104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
     </row>
@@ -5038,29 +5403,29 @@
       <c r="Q34" s="4">
         <v>3</v>
       </c>
-      <c r="R34" s="118">
-        <f>SUM(K34:Q34)/6</f>
+      <c r="R34" s="34">
+        <f t="shared" si="3"/>
         <v>4.833333333333333</v>
       </c>
-      <c r="S34" s="119">
+      <c r="S34" s="4">
         <v>4</v>
       </c>
       <c r="T34" s="104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="111">
+      <c r="A35" s="41">
         <v>8</v>
       </c>
       <c r="B35" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="113">
+      <c r="C35" s="43">
         <v>28</v>
       </c>
-      <c r="D35" s="114">
+      <c r="D35" s="79">
         <v>6</v>
       </c>
       <c r="E35" s="56">
@@ -5072,7 +5437,7 @@
       <c r="G35" s="44">
         <v>4</v>
       </c>
-      <c r="H35" s="114">
+      <c r="H35" s="79">
         <v>1</v>
       </c>
       <c r="I35" s="81">
@@ -5084,33 +5449,33 @@
       <c r="K35" s="48">
         <v>3</v>
       </c>
-      <c r="L35" s="112">
-        <v>10</v>
-      </c>
-      <c r="M35" s="112">
-        <v>7</v>
-      </c>
-      <c r="N35" s="112">
-        <v>5</v>
-      </c>
-      <c r="O35" s="112">
-        <v>5</v>
-      </c>
-      <c r="P35" s="112">
+      <c r="L35" s="49">
+        <v>10</v>
+      </c>
+      <c r="M35" s="49">
+        <v>7</v>
+      </c>
+      <c r="N35" s="49">
+        <v>5</v>
+      </c>
+      <c r="O35" s="49">
+        <v>5</v>
+      </c>
+      <c r="P35" s="49">
         <v>9</v>
       </c>
       <c r="Q35" s="50">
         <v>5</v>
       </c>
       <c r="R35" s="51">
-        <f>SUM(K35:Q35)/6</f>
+        <f t="shared" si="3"/>
         <v>7.333333333333333</v>
       </c>
       <c r="S35" s="50">
         <v>5</v>
       </c>
       <c r="T35" s="104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
     </row>
@@ -5167,7 +5532,7 @@
         <v>9</v>
       </c>
       <c r="R36" s="34">
-        <f>SUM(K36:Q36)/6</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="S36" s="4">
@@ -5231,14 +5596,14 @@
         <v>6</v>
       </c>
       <c r="R37" s="71">
-        <f>SUM(K37:Q37)/6</f>
+        <f t="shared" si="3"/>
         <v>4.166666666666667</v>
       </c>
       <c r="S37" s="69">
         <v>2</v>
       </c>
       <c r="T37" s="104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
     </row>
@@ -5262,10 +5627,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5E5147-5992-4431-822F-ABC86F78CFE9}">
-  <dimension ref="A3:T43"/>
+  <dimension ref="A3:W43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5276,34 +5641,38 @@
     <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.42578125" customWidth="1"/>
     <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="108" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="109"/>
-      <c r="I3" s="110"/>
+      <c r="C3" s="118" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="119"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="120"/>
       <c r="J3" s="18"/>
-      <c r="K3" s="108" t="s">
+      <c r="K3" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="109"/>
-      <c r="M3" s="109"/>
-      <c r="N3" s="109"/>
-      <c r="O3" s="109"/>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="109"/>
-      <c r="R3" s="109"/>
-      <c r="S3" s="110"/>
-      <c r="T3" s="1"/>
-    </row>
-    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="L3" s="119"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="119"/>
+      <c r="P3" s="119"/>
+      <c r="Q3" s="119"/>
+      <c r="R3" s="119"/>
+      <c r="S3" s="120"/>
+      <c r="T3" s="108"/>
+      <c r="U3" s="109"/>
+      <c r="V3" s="109"/>
+      <c r="W3" s="109"/>
+    </row>
+    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>49</v>
       </c>
@@ -5361,11 +5730,20 @@
       <c r="S4" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="28" t="s">
+      <c r="T4" s="111" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="V4" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="W4" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="32">
         <v>1</v>
       </c>
@@ -5428,8 +5806,18 @@
         <f>SUM(K5:Q5)</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5" s="4">
+        <v>13</v>
+      </c>
+      <c r="V5" s="106">
+        <v>5000</v>
+      </c>
+      <c r="W5" s="113">
+        <f>V5/F5</f>
+        <v>64.102564102564102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="41">
         <v>2</v>
       </c>
@@ -5488,12 +5876,22 @@
       <c r="S6" s="86">
         <v>6</v>
       </c>
-      <c r="T6" s="1">
+      <c r="T6" s="49">
         <f t="shared" ref="T6:T14" si="0">SUM(K6:Q6)</f>
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6" s="50">
+        <v>12</v>
+      </c>
+      <c r="V6" s="112">
+        <v>1000</v>
+      </c>
+      <c r="W6" s="114">
+        <f t="shared" ref="W6:W14" si="1">V6/F6</f>
+        <v>25.641025641025642</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="32">
         <v>3</v>
       </c>
@@ -5556,8 +5954,18 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7" s="4">
+        <v>11</v>
+      </c>
+      <c r="V7" s="106">
+        <v>500</v>
+      </c>
+      <c r="W7" s="113">
+        <f t="shared" si="1"/>
+        <v>20.833333333333332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="41">
         <v>4</v>
       </c>
@@ -5616,12 +6024,22 @@
       <c r="S8" s="86">
         <v>10</v>
       </c>
-      <c r="T8" s="1">
+      <c r="T8" s="49">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8" s="50">
+        <v>13</v>
+      </c>
+      <c r="V8" s="112">
+        <v>1000</v>
+      </c>
+      <c r="W8" s="114">
+        <f t="shared" si="1"/>
+        <v>52.631578947368418</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="32">
         <v>5</v>
       </c>
@@ -5638,7 +6056,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="14">
-        <f t="shared" ref="F9:F14" si="1">SUM(C9:E9)</f>
+        <f t="shared" ref="F9:F14" si="2">SUM(C9:E9)</f>
         <v>36</v>
       </c>
       <c r="G9" s="73">
@@ -5684,8 +6102,18 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="4">
+        <v>11</v>
+      </c>
+      <c r="V9" s="106">
+        <v>500</v>
+      </c>
+      <c r="W9" s="113">
+        <f t="shared" si="1"/>
+        <v>13.888888888888889</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="41">
         <v>6</v>
       </c>
@@ -5744,12 +6172,22 @@
       <c r="S10" s="86">
         <v>8</v>
       </c>
-      <c r="T10" s="1">
+      <c r="T10" s="49">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="50">
+        <v>12</v>
+      </c>
+      <c r="V10" s="112">
+        <v>500</v>
+      </c>
+      <c r="W10" s="114">
+        <f t="shared" si="1"/>
+        <v>17.857142857142858</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="32">
         <v>7</v>
       </c>
@@ -5766,7 +6204,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="G11" s="75">
@@ -5812,8 +6250,18 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="4">
+        <v>12</v>
+      </c>
+      <c r="V11" s="106">
+        <v>5000</v>
+      </c>
+      <c r="W11" s="113">
+        <f>V11/F11</f>
+        <v>102.04081632653062</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="41">
         <v>8</v>
       </c>
@@ -5830,7 +6278,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="G12" s="76">
@@ -5872,12 +6320,22 @@
       <c r="S12" s="86">
         <v>5</v>
       </c>
-      <c r="T12" s="1">
+      <c r="T12" s="49">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12" s="50">
+        <v>11</v>
+      </c>
+      <c r="V12" s="112">
+        <v>1000</v>
+      </c>
+      <c r="W12" s="114">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="32">
         <v>9</v>
       </c>
@@ -5894,7 +6352,7 @@
         <v>30</v>
       </c>
       <c r="F13" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
       <c r="G13" s="77">
@@ -5940,8 +6398,18 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" s="4">
+        <v>14</v>
+      </c>
+      <c r="V13" s="106">
+        <v>4000</v>
+      </c>
+      <c r="W13" s="113">
+        <f t="shared" si="1"/>
+        <v>64.516129032258064</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="59">
         <v>10</v>
       </c>
@@ -5958,7 +6426,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="G14" s="78">
@@ -6000,49 +6468,92 @@
       <c r="S14" s="103">
         <v>2</v>
       </c>
-      <c r="T14" s="1">
+      <c r="T14" s="67">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14" s="65">
+        <v>19</v>
+      </c>
+      <c r="V14" s="69">
+        <v>5000</v>
+      </c>
+      <c r="W14" s="115">
+        <f t="shared" si="1"/>
+        <v>75.757575757575751</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B15" s="39" t="s">
         <v>65</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:J15" si="2">SUM(C5:C14)</f>
+        <f t="shared" ref="C15:J15" si="3">SUM(C5:C14)</f>
         <v>202</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>159</v>
       </c>
       <c r="E15" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="F15" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>441</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="J15" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15" s="116" t="s">
+        <v>98</v>
+      </c>
+      <c r="U15" s="1">
+        <f>SUM(U5:U6)+SUM(U8:U14)</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T16" s="116" t="s">
+        <v>101</v>
+      </c>
+      <c r="U16" s="1">
+        <f>U7</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T17" s="116" t="s">
+        <v>100</v>
+      </c>
+      <c r="U17" s="1">
+        <f>U15+U16</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T18" s="116" t="s">
+        <v>99</v>
+      </c>
+      <c r="U18" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="37" t="s">
         <v>47</v>
       </c>
@@ -6052,8 +6563,15 @@
       <c r="G19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="116" t="s">
+        <v>102</v>
+      </c>
+      <c r="U19" s="110">
+        <f>U17+U18</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B20" s="37" t="s">
         <v>46</v>
       </c>
@@ -6064,7 +6582,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B21" s="37" t="s">
         <v>45</v>
       </c>
@@ -6075,7 +6593,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B22" s="37" t="s">
         <v>48</v>
       </c>
@@ -6086,7 +6604,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B23" s="37" t="s">
         <v>9</v>
       </c>
@@ -6097,7 +6615,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B24" s="38" t="s">
         <v>8</v>
       </c>
@@ -6108,7 +6626,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B25" s="37" t="s">
         <v>10</v>
       </c>
@@ -6119,7 +6637,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="89" t="s">
         <v>49</v>
       </c>
@@ -6178,7 +6696,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="32">
         <v>1</v>
       </c>
@@ -6231,14 +6749,14 @@
         <v>9</v>
       </c>
       <c r="R31" s="34">
-        <f t="shared" ref="R31:R40" si="3">SUM(K31:Q31)/6</f>
+        <f t="shared" ref="R31:R40" si="4">SUM(K31:Q31)/6</f>
         <v>4.833333333333333</v>
       </c>
       <c r="S31" s="83">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="41">
         <v>2</v>
       </c>
@@ -6291,7 +6809,7 @@
         <v>8</v>
       </c>
       <c r="R32" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.5</v>
       </c>
       <c r="S32" s="86">
@@ -6351,7 +6869,7 @@
         <v>1</v>
       </c>
       <c r="R33" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="S33" s="83">
@@ -6411,7 +6929,7 @@
         <v>4</v>
       </c>
       <c r="R34" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="S34" s="86">
@@ -6471,7 +6989,7 @@
         <v>6</v>
       </c>
       <c r="R35" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="S35" s="106">
@@ -6531,7 +7049,7 @@
         <v>2</v>
       </c>
       <c r="R36" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="S36" s="86">
@@ -6591,7 +7109,7 @@
         <v>3</v>
       </c>
       <c r="R37" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.833333333333333</v>
       </c>
       <c r="S37" s="83">
@@ -6651,7 +7169,7 @@
         <v>5</v>
       </c>
       <c r="R38" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.166666666666667</v>
       </c>
       <c r="S38" s="86">
@@ -6711,7 +7229,7 @@
         <v>10</v>
       </c>
       <c r="R39" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.333333333333333</v>
       </c>
       <c r="S39" s="83">
@@ -6771,7 +7289,7 @@
         <v>7</v>
       </c>
       <c r="R40" s="71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.5</v>
       </c>
       <c r="S40" s="103">

</xml_diff>

<commit_message>
Summary Models and resource updates Actions: ADD shortcut tag to the shortcut images in Hi-Tech and Jazz-Age editions UPDATE resource files to match models and other corrections Problems
</commit_message>
<xml_diff>
--- a/docs/edition_points.xlsx
+++ b/docs/edition_points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Compile\careers\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A35BE78-5486-4E28-9DEC-86DFDA6BC898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FA47FB-A1CC-415D-A6D9-97233A8037A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30180" yWindow="1425" windowWidth="26640" windowHeight="13110" tabRatio="535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1005" yWindow="1500" windowWidth="26640" windowHeight="13110" tabRatio="535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hi-Tech Jobs" sheetId="1" r:id="rId1"/>
@@ -2144,8 +2144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2731D533-3189-49BB-AE83-771387574D8F}">
   <dimension ref="A3:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Summary Bug fix, resource updates Actions: FIX Problem with editions.json point_icons processing UPDATE Destinations-London resources
Problems
</commit_message>
<xml_diff>
--- a/docs/edition_points.xlsx
+++ b/docs/edition_points.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Compile\careers\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FA47FB-A1CC-415D-A6D9-97233A8037A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AECCC8-DD32-4EBF-8DFD-933C14DF13FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="1500" windowWidth="26640" windowHeight="13110" tabRatio="535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30435" yWindow="1335" windowWidth="26640" windowHeight="13110" tabRatio="535" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hi-Tech Jobs" sheetId="1" r:id="rId1"/>
@@ -281,15 +281,9 @@
     <t>Harrods</t>
   </si>
   <si>
-    <t>Westminster</t>
-  </si>
-  <si>
     <t>Stonehenge</t>
   </si>
   <si>
-    <t>Houses of Parliament</t>
-  </si>
-  <si>
     <t>Buckingham Palace</t>
   </si>
   <si>
@@ -357,6 +351,12 @@
   </si>
   <si>
     <t>Cost per point</t>
+  </si>
+  <si>
+    <t>Westminster Abbey</t>
+  </si>
+  <si>
+    <t>Palace of Westminster</t>
   </si>
 </sst>
 </file>
@@ -2144,7 +2144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2731D533-3189-49BB-AE83-771387574D8F}">
   <dimension ref="A3:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -2248,22 +2248,22 @@
         <v>7</v>
       </c>
       <c r="R4" s="33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="S4" s="19" t="s">
         <v>51</v>
       </c>
       <c r="T4" s="111" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="V4" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="W4" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="J15" s="23"/>
       <c r="T15" s="116" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="U15" s="1">
         <f>SUM(U5:U6)+SUM(U8:U14)</f>
@@ -3051,7 +3051,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="T16" s="116" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="U16" s="1">
         <f>U7</f>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T17" s="116" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U17" s="1">
         <f>U15+U16</f>
@@ -3069,7 +3069,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T18" s="116" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="U18" s="1">
         <v>42</v>
@@ -3080,13 +3080,13 @@
         <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G19" t="s">
         <v>41</v>
       </c>
       <c r="T19" s="116" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="U19" s="110">
         <f>U17+U18</f>
@@ -3098,7 +3098,7 @@
         <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G20" t="s">
         <v>42</v>
@@ -3120,7 +3120,7 @@
         <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G22" t="s">
         <v>44</v>
@@ -3156,7 +3156,7 @@
     <row r="27" spans="1:21" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3235,7 +3235,7 @@
         <v>7</v>
       </c>
       <c r="R30" s="33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="S30" s="19" t="s">
         <v>51</v>
@@ -3894,7 +3894,7 @@
   <dimension ref="A3:W39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4005,16 +4005,16 @@
         <v>51</v>
       </c>
       <c r="T4" s="111" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="V4" s="117" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="W4" s="117" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -4784,7 +4784,7 @@
         <v>21</v>
       </c>
       <c r="T15" s="116" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="U15" s="1">
         <f>SUM(U5:U6)+SUM(U8:U14)</f>
@@ -4797,7 +4797,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="T16" s="116" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="U16" s="1">
         <f>U7</f>
@@ -4806,7 +4806,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T17" s="116" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U17" s="1">
         <f>U15+U16</f>
@@ -4815,7 +4815,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T18" s="116" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="U18" s="1">
         <v>42</v>
@@ -4832,7 +4832,7 @@
         <v>41</v>
       </c>
       <c r="T19" s="116" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="U19" s="110">
         <f>U17+U18</f>
@@ -4964,7 +4964,7 @@
         <v>51</v>
       </c>
       <c r="T27" s="28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
@@ -5629,8 +5629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5E5147-5992-4431-822F-ABC86F78CFE9}">
   <dimension ref="A3:W43"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5731,16 +5731,16 @@
         <v>51</v>
       </c>
       <c r="T4" s="111" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="V4" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="W4" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -6044,7 +6044,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="C9" s="5">
         <v>16</v>
@@ -6118,7 +6118,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="49">
         <v>2</v>
@@ -6192,7 +6192,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="C11" s="1">
         <v>38</v>
@@ -6266,7 +6266,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C12" s="43">
         <v>30</v>
@@ -6340,7 +6340,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1">
         <v>12</v>
@@ -6414,7 +6414,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="60" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C14" s="61">
         <v>34</v>
@@ -6520,7 +6520,7 @@
         <v>21</v>
       </c>
       <c r="T15" s="116" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="U15" s="1">
         <f>SUM(U5:U6)+SUM(U8:U14)</f>
@@ -6529,7 +6529,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="T16" s="116" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="U16" s="1">
         <f>U7</f>
@@ -6538,7 +6538,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T17" s="116" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U17" s="1">
         <f>U15+U16</f>
@@ -6547,7 +6547,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T18" s="116" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="U18" s="1">
         <v>42</v>
@@ -6558,13 +6558,13 @@
         <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G19" t="s">
         <v>41</v>
       </c>
       <c r="T19" s="116" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="U19" s="110">
         <f>U17+U18</f>
@@ -6576,7 +6576,7 @@
         <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G20" t="s">
         <v>42</v>
@@ -6587,7 +6587,7 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G21" t="s">
         <v>43</v>
@@ -6598,7 +6598,7 @@
         <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G22" t="s">
         <v>44</v>
@@ -6609,7 +6609,7 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G23" t="s">
         <v>26</v>
@@ -6620,7 +6620,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G24" t="s">
         <v>25</v>
@@ -6631,7 +6631,7 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G25" t="s">
         <v>66</v>
@@ -6704,10 +6704,10 @@
         <v>75</v>
       </c>
       <c r="C31" s="32">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D31" s="32">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E31" s="29">
         <v>10</v>
@@ -6884,7 +6884,7 @@
         <v>78</v>
       </c>
       <c r="C34" s="79">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D34" s="79">
         <v>12</v>
@@ -6941,10 +6941,10 @@
         <v>5</v>
       </c>
       <c r="B35" s="101" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="C35" s="16">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D35" s="16">
         <v>12</v>
@@ -7001,13 +7001,13 @@
         <v>6</v>
       </c>
       <c r="B36" s="97" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" s="41">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="D36" s="41">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E36" s="56">
         <v>3</v>
@@ -7061,13 +7061,13 @@
         <v>7</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="C37" s="32">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="D37" s="32">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E37" s="15">
         <v>5</v>
@@ -7121,13 +7121,13 @@
         <v>8</v>
       </c>
       <c r="B38" s="99" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C38" s="79">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D38" s="79">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E38" s="56">
         <v>4</v>
@@ -7181,13 +7181,13 @@
         <v>9</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C39" s="32">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D39" s="32">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E39" s="25">
         <v>30</v>
@@ -7241,13 +7241,13 @@
         <v>10</v>
       </c>
       <c r="B40" s="105" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C40" s="80">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D40" s="80">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E40" s="62">
         <v>9</v>
@@ -7297,13 +7297,13 @@
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C41" s="104">
+      <c r="C41" s="32">
         <f>SUM(C31:C40)</f>
-        <v>202</v>
-      </c>
-      <c r="D41" s="104">
+        <v>218</v>
+      </c>
+      <c r="D41" s="32">
         <f>SUM(D31:D40)</f>
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>